<commit_message>
Added a new ExcelDataReader.
</commit_message>
<xml_diff>
--- a/BarcodeScanner/planning kinderen en leiding.xlsx
+++ b/BarcodeScanner/planning kinderen en leiding.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="-150" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="1590" yWindow="-150" windowWidth="19320" windowHeight="12120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kleine speltakken" sheetId="1" r:id="rId1"/>
     <sheet name="Grote speltakken" sheetId="2" r:id="rId2"/>
     <sheet name="Leiding Kleine speltakken" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -363,8 +363,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/mm/yy\ h:mm;@"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -634,31 +637,34 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -668,6 +674,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -705,7 +714,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -718,9 +727,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -758,7 +767,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -792,7 +801,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -827,10 +835,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1003,15 +1010,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
@@ -1020,23 +1028,23 @@
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+    <row r="1" spans="1:11" s="4" customFormat="1" ht="12.75"/>
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="15.75">
+      <c r="A2" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1047,7 +1055,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A4" s="36"/>
       <c r="B4" s="37"/>
       <c r="C4" s="27" t="s">
@@ -1072,22 +1080,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C5" s="41" t="s">
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="29">
+        <v>40831.395833333336</v>
+      </c>
+      <c r="B5" s="29">
+        <v>40831.416666666664</v>
+      </c>
+      <c r="C5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="43"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="6">
         <v>0.39583333333333331</v>
       </c>
@@ -1095,12 +1103,12 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="B6" s="7">
-        <v>0.43055555555555558</v>
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A6" s="29">
+        <v>40831.416666666664</v>
+      </c>
+      <c r="B6" s="30">
+        <v>40831.430555555555</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>15</v>
@@ -1111,16 +1119,16 @@
       <c r="E6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="39" t="s">
+      <c r="H6" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="33" t="s">
         <v>45</v>
       </c>
       <c r="J6" s="6">
@@ -1130,12 +1138,12 @@
         <v>0.43055555555555558</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>0.43055555555555558</v>
-      </c>
-      <c r="B7" s="7">
-        <v>0.44444444444444442</v>
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A7" s="29">
+        <v>40831.430555555555</v>
+      </c>
+      <c r="B7" s="30">
+        <v>40831.444444444445</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>16</v>
@@ -1146,10 +1154,10 @@
       <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="35"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="6">
         <v>0.43055555555555558</v>
       </c>
@@ -1157,12 +1165,12 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="B8" s="7">
-        <v>0.45833333333333331</v>
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A8" s="29">
+        <v>40831.444444444445</v>
+      </c>
+      <c r="B8" s="30">
+        <v>40831.458333333336</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>17</v>
@@ -1173,10 +1181,10 @@
       <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="35"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="6">
         <v>0.44444444444444442</v>
       </c>
@@ -1184,12 +1192,12 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="B9" s="7">
-        <v>0.47222222222222199</v>
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A9" s="29">
+        <v>40831.458333333336</v>
+      </c>
+      <c r="B9" s="30">
+        <v>40831.472222222219</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>18</v>
@@ -1200,16 +1208,16 @@
       <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="35"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="6">
         <v>0.45833333333333331</v>
       </c>
@@ -1217,12 +1225,12 @@
         <v>0.47222222222222199</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>0.47222222222222199</v>
-      </c>
-      <c r="B10" s="7">
-        <v>0.48611111111111099</v>
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A10" s="29">
+        <v>40831.472222222219</v>
+      </c>
+      <c r="B10" s="30">
+        <v>40831.486111111109</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>19</v>
@@ -1233,10 +1241,10 @@
       <c r="E10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="35"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="6">
         <v>0.47222222222222199</v>
       </c>
@@ -1244,12 +1252,12 @@
         <v>0.48611111111111099</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>0.48611111111111099</v>
-      </c>
-      <c r="B11" s="7">
-        <v>0.5</v>
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A11" s="29">
+        <v>40831.486111111109</v>
+      </c>
+      <c r="B11" s="30">
+        <v>40831.5</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>20</v>
@@ -1260,10 +1268,10 @@
       <c r="E11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="35"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="6">
         <v>0.48611111111111099</v>
       </c>
@@ -1271,22 +1279,22 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="B12" s="7">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="C12" s="35" t="s">
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A12" s="29">
+        <v>40831.5</v>
+      </c>
+      <c r="B12" s="30">
+        <v>40831.527777777781</v>
+      </c>
+      <c r="C12" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="6">
         <v>0.5</v>
       </c>
@@ -1294,12 +1302,12 @@
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>0.52777777777777801</v>
-      </c>
-      <c r="B13" s="7">
-        <v>0.54166666666666696</v>
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A13" s="29">
+        <v>40831.527777777781</v>
+      </c>
+      <c r="B13" s="30">
+        <v>40831.541666666664</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>21</v>
@@ -1310,16 +1318,16 @@
       <c r="E13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="38" t="s">
+      <c r="H13" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="35" t="s">
+      <c r="I13" s="42" t="s">
         <v>46</v>
       </c>
       <c r="J13" s="6">
@@ -1329,12 +1337,12 @@
         <v>0.54166666666666696</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="B14" s="7">
-        <v>0.55555555555555602</v>
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A14" s="29">
+        <v>40831.541666666664</v>
+      </c>
+      <c r="B14" s="30">
+        <v>40831.555555555555</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>22</v>
@@ -1345,10 +1353,10 @@
       <c r="E14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="35"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="6">
         <v>0.54166666666666696</v>
       </c>
@@ -1356,12 +1364,12 @@
         <v>0.55555555555555602</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>0.55555555555555602</v>
-      </c>
-      <c r="B15" s="7">
-        <v>0.56944444444444497</v>
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A15" s="29">
+        <v>40831.555555555555</v>
+      </c>
+      <c r="B15" s="30">
+        <v>40831.569444444445</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>23</v>
@@ -1372,10 +1380,10 @@
       <c r="E15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="35"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="6">
         <v>0.55555555555555602</v>
       </c>
@@ -1383,12 +1391,12 @@
         <v>0.56944444444444497</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>0.56944444444444497</v>
-      </c>
-      <c r="B16" s="7">
-        <v>0.58333333333333404</v>
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A16" s="29">
+        <v>40831.569444444445</v>
+      </c>
+      <c r="B16" s="30">
+        <v>40831.583333333336</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>24</v>
@@ -1399,16 +1407,16 @@
       <c r="E16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="38" t="s">
+      <c r="G16" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="35"/>
+      <c r="I16" s="42"/>
       <c r="J16" s="6">
         <v>0.56944444444444497</v>
       </c>
@@ -1416,12 +1424,12 @@
         <v>0.58333333333333404</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
-        <v>0.58333333333333404</v>
-      </c>
-      <c r="B17" s="7">
-        <v>0.59722222222222299</v>
+    <row r="17" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A17" s="29">
+        <v>40831.583333333336</v>
+      </c>
+      <c r="B17" s="30">
+        <v>40831.597222222219</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>25</v>
@@ -1432,10 +1440,10 @@
       <c r="E17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="30"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="35"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="42"/>
       <c r="J17" s="6">
         <v>0.58333333333333404</v>
       </c>
@@ -1443,12 +1451,12 @@
         <v>0.59722222222222299</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
-        <v>0.59722222222222299</v>
-      </c>
-      <c r="B18" s="7">
-        <v>0.61111111111111205</v>
+    <row r="18" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A18" s="29">
+        <v>40831.597222222219</v>
+      </c>
+      <c r="B18" s="30">
+        <v>40831.611111111109</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>26</v>
@@ -1459,10 +1467,10 @@
       <c r="E18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="35"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="42"/>
       <c r="J18" s="6">
         <v>0.59722222222222299</v>
       </c>
@@ -1470,12 +1478,12 @@
         <v>0.61111111111111205</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
-        <v>0.61111111111111205</v>
-      </c>
-      <c r="B19" s="7">
-        <v>0.625</v>
+    <row r="19" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A19" s="29">
+        <v>40831.611111111109</v>
+      </c>
+      <c r="B19" s="30">
+        <v>40831.625</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>27</v>
@@ -1486,16 +1494,16 @@
       <c r="E19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="38" t="s">
+      <c r="G19" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="38" t="s">
+      <c r="H19" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="35" t="s">
+      <c r="I19" s="42" t="s">
         <v>47</v>
       </c>
       <c r="J19" s="6">
@@ -1505,12 +1513,12 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="B20" s="7">
-        <v>0.63888888888888895</v>
+    <row r="20" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A20" s="29">
+        <v>40831.625</v>
+      </c>
+      <c r="B20" s="30">
+        <v>40831.638888888891</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>28</v>
@@ -1521,10 +1529,10 @@
       <c r="E20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="30"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="35"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="42"/>
       <c r="J20" s="6">
         <v>0.625</v>
       </c>
@@ -1532,12 +1540,12 @@
         <v>0.63888888888888895</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="B21" s="7">
-        <v>0.65277777777777801</v>
+    <row r="21" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A21" s="29">
+        <v>40831.638888888891</v>
+      </c>
+      <c r="B21" s="30">
+        <v>40831.652777777781</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>29</v>
@@ -1548,10 +1556,10 @@
       <c r="E21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="35"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="42"/>
       <c r="J21" s="6">
         <v>0.63888888888888895</v>
       </c>
@@ -1559,12 +1567,12 @@
         <v>0.65277777777777801</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
-        <v>0.65277777777777801</v>
-      </c>
-      <c r="B22" s="7">
-        <v>0.66666666666666696</v>
+    <row r="22" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A22" s="29">
+        <v>40831.652777777781</v>
+      </c>
+      <c r="B22" s="30">
+        <v>40831.666666666664</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>30</v>
@@ -1575,16 +1583,16 @@
       <c r="E22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="29" t="s">
+      <c r="F22" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="38" t="s">
+      <c r="G22" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="H22" s="38" t="s">
+      <c r="H22" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="35"/>
+      <c r="I22" s="42"/>
       <c r="J22" s="6">
         <v>0.65277777777777801</v>
       </c>
@@ -1592,12 +1600,12 @@
         <v>0.66666666666666696</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="6">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="B23" s="7">
-        <v>0.68055555555555602</v>
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A23" s="29">
+        <v>40831.666666666664</v>
+      </c>
+      <c r="B23" s="30">
+        <v>40831.680555555555</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>31</v>
@@ -1608,10 +1616,10 @@
       <c r="E23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="35"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="42"/>
       <c r="J23" s="6">
         <v>0.66666666666666696</v>
       </c>
@@ -1619,12 +1627,12 @@
         <v>0.68055555555555602</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="6">
-        <v>0.68055555555555602</v>
-      </c>
-      <c r="B24" s="7">
-        <v>0.69444444444444453</v>
+    <row r="24" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A24" s="29">
+        <v>40831.680555555555</v>
+      </c>
+      <c r="B24" s="30">
+        <v>40831.694444444445</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>32</v>
@@ -1635,10 +1643,10 @@
       <c r="E24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="35"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="42"/>
       <c r="J24" s="6">
         <v>0.68055555555555602</v>
       </c>
@@ -1646,22 +1654,22 @@
         <v>0.69444444444444453</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
-        <v>0.69444444444444497</v>
-      </c>
-      <c r="B25" s="7">
-        <v>0.73611111111111116</v>
-      </c>
-      <c r="C25" s="35" t="s">
+    <row r="25" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A25" s="29">
+        <v>40831.694444444445</v>
+      </c>
+      <c r="B25" s="30">
+        <v>40831.736111111109</v>
+      </c>
+      <c r="C25" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
       <c r="J25" s="6">
         <v>0.69444444444444497</v>
       </c>
@@ -1669,22 +1677,22 @@
         <v>0.73611111111111116</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
-        <v>0.73611111111111205</v>
-      </c>
-      <c r="B26" s="7">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="C26" s="35" t="s">
+    <row r="26" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A26" s="29">
+        <v>40831.736111111109</v>
+      </c>
+      <c r="B26" s="30">
+        <v>40831.770833333336</v>
+      </c>
+      <c r="C26" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
       <c r="J26" s="6">
         <v>0.73611111111111205</v>
       </c>
@@ -1692,22 +1700,22 @@
         <v>0.77083333333333337</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="6">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="B27" s="7">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="C27" s="35" t="s">
+    <row r="27" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A27" s="29">
+        <v>40831.770833333336</v>
+      </c>
+      <c r="B27" s="30">
+        <v>40831.791666666664</v>
+      </c>
+      <c r="C27" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
       <c r="J27" s="6">
         <v>0.77083333333333337</v>
       </c>
@@ -1715,22 +1723,22 @@
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="6">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="B28" s="7">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="C28" s="35" t="s">
+    <row r="28" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A28" s="29">
+        <v>40831.791666666664</v>
+      </c>
+      <c r="B28" s="30">
+        <v>40831.916666666664</v>
+      </c>
+      <c r="C28" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
       <c r="J28" s="6">
         <v>0.79166666666666663</v>
       </c>
@@ -1738,22 +1746,22 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="6">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="B29" s="7">
-        <v>0.9375</v>
-      </c>
-      <c r="C29" s="35" t="s">
+    <row r="29" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A29" s="29">
+        <v>40831.916666666664</v>
+      </c>
+      <c r="B29" s="30">
+        <v>40831.9375</v>
+      </c>
+      <c r="C29" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
       <c r="J29" s="6">
         <v>0.91666666666666663</v>
       </c>
@@ -1761,22 +1769,22 @@
         <v>0.9375</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="6">
-        <v>0.9375</v>
-      </c>
-      <c r="B30" s="7">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="C30" s="35" t="s">
+    <row r="30" spans="1:11" s="4" customFormat="1" ht="12.75">
+      <c r="A30" s="29">
+        <v>40831.9375</v>
+      </c>
+      <c r="B30" s="30">
+        <v>40831.291666666664</v>
+      </c>
+      <c r="C30" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
       <c r="J30" s="6">
         <v>0.9375</v>
       </c>
@@ -1784,7 +1792,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="22"/>
@@ -1797,7 +1805,7 @@
       <c r="J31" s="21"/>
       <c r="K31" s="21"/>
     </row>
-    <row r="32" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A32" s="21"/>
       <c r="B32" s="21"/>
       <c r="C32" s="22"/>
@@ -1808,22 +1816,22 @@
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
+    <row r="33" spans="1:11" s="4" customFormat="1" ht="15.75">
+      <c r="A33" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-    </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+    </row>
+    <row r="34" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A34" s="34"/>
       <c r="B34" s="34"/>
       <c r="C34" s="9" t="s">
@@ -1845,21 +1853,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A35" s="8">
         <v>0.29166666666666669</v>
       </c>
       <c r="B35" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
       <c r="I35" s="8">
         <v>0.29166666666666669</v>
       </c>
@@ -1867,21 +1875,21 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A36" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="B36" s="8">
         <v>0.3611111111111111</v>
       </c>
-      <c r="C36" s="33" t="s">
+      <c r="C36" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
       <c r="I36" s="8">
         <v>0.33333333333333331</v>
       </c>
@@ -1889,21 +1897,21 @@
         <v>0.3611111111111111</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A37" s="8">
         <v>0.3611111111111111</v>
       </c>
       <c r="B37" s="8">
         <v>0.40277777777777773</v>
       </c>
-      <c r="C37" s="33" t="s">
+      <c r="C37" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
       <c r="I37" s="8">
         <v>0.3611111111111111</v>
       </c>
@@ -1911,7 +1919,7 @@
         <v>0.40277777777777773</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A38" s="8">
         <v>0.40277777777777801</v>
       </c>
@@ -1924,16 +1932,16 @@
       <c r="D38" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="29" t="s">
+      <c r="E38" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="29" t="s">
+      <c r="F38" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G38" s="29" t="s">
+      <c r="G38" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="H38" s="29" t="s">
+      <c r="H38" s="32" t="s">
         <v>74</v>
       </c>
       <c r="I38" s="8">
@@ -1943,7 +1951,7 @@
         <v>0.41666666666666702</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A39" s="8">
         <v>0.41666666666666702</v>
       </c>
@@ -1956,10 +1964,10 @@
       <c r="D39" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="30"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="38"/>
       <c r="I39" s="8">
         <v>0.41666666666666702</v>
       </c>
@@ -1967,7 +1975,7 @@
         <v>0.43055555555555602</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A40" s="8">
         <v>0.43055555555555602</v>
       </c>
@@ -1980,16 +1988,16 @@
       <c r="D40" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E40" s="29" t="s">
+      <c r="E40" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="F40" s="29" t="s">
+      <c r="F40" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="G40" s="29" t="s">
+      <c r="G40" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="H40" s="30"/>
+      <c r="H40" s="38"/>
       <c r="I40" s="8">
         <v>0.43055555555555602</v>
       </c>
@@ -1997,7 +2005,7 @@
         <v>0.44444444444444497</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A41" s="8">
         <v>0.44444444444444497</v>
       </c>
@@ -2010,10 +2018,10 @@
       <c r="D41" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
       <c r="I41" s="8">
         <v>0.44444444444444497</v>
       </c>
@@ -2021,7 +2029,7 @@
         <v>0.45833333333333298</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A42" s="8">
         <v>0.45833333333333298</v>
       </c>
@@ -2034,16 +2042,16 @@
       <c r="D42" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="29" t="s">
+      <c r="E42" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="F42" s="29" t="s">
+      <c r="F42" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="G42" s="29" t="s">
+      <c r="G42" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="H42" s="29" t="s">
+      <c r="H42" s="32" t="s">
         <v>75</v>
       </c>
       <c r="I42" s="8">
@@ -2053,7 +2061,7 @@
         <v>0.47222222222222199</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A43" s="8">
         <v>0.47222222222222199</v>
       </c>
@@ -2066,10 +2074,10 @@
       <c r="D43" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="30"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="38"/>
       <c r="I43" s="8">
         <v>0.47222222222222199</v>
       </c>
@@ -2077,7 +2085,7 @@
         <v>0.48611111111111099</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A44" s="8">
         <v>0.48611111111111099</v>
       </c>
@@ -2090,16 +2098,16 @@
       <c r="D44" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E44" s="29" t="s">
+      <c r="E44" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="F44" s="29" t="s">
+      <c r="F44" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="G44" s="29" t="s">
+      <c r="G44" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="H44" s="30"/>
+      <c r="H44" s="38"/>
       <c r="I44" s="8">
         <v>0.48611111111111099</v>
       </c>
@@ -2107,7 +2115,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A45" s="8">
         <v>0.5</v>
       </c>
@@ -2120,10 +2128,10 @@
       <c r="D45" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
       <c r="I45" s="8">
         <v>0.5</v>
       </c>
@@ -2131,21 +2139,21 @@
         <v>0.51388888888888895</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A46" s="8">
         <v>0.51388888888888895</v>
       </c>
       <c r="B46" s="8">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C46" s="35" t="s">
+      <c r="C46" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="35"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
       <c r="I46" s="8">
         <v>0.51388888888888895</v>
       </c>
@@ -2153,7 +2161,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A47" s="8">
         <v>0.54166666666666696</v>
       </c>
@@ -2166,16 +2174,16 @@
       <c r="D47" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E47" s="29" t="s">
+      <c r="E47" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="F47" s="29" t="s">
+      <c r="F47" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="G47" s="29" t="s">
+      <c r="G47" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="H47" s="29" t="s">
+      <c r="H47" s="32" t="s">
         <v>76</v>
       </c>
       <c r="I47" s="8">
@@ -2185,7 +2193,7 @@
         <v>0.55555555555555602</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A48" s="8">
         <v>0.55555555555555602</v>
       </c>
@@ -2198,10 +2206,10 @@
       <c r="D48" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="30"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="38"/>
       <c r="I48" s="8">
         <v>0.55555555555555602</v>
       </c>
@@ -2209,7 +2217,7 @@
         <v>0.56944444444444398</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" s="4" customFormat="1" ht="12.75">
       <c r="A49" s="8">
         <v>0.56944444444444398</v>
       </c>
@@ -2222,16 +2230,16 @@
       <c r="D49" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E49" s="29" t="s">
+      <c r="E49" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="F49" s="29" t="s">
+      <c r="F49" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="G49" s="29" t="s">
+      <c r="G49" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="H49" s="30"/>
+      <c r="H49" s="38"/>
       <c r="I49" s="8">
         <v>0.56944444444444398</v>
       </c>
@@ -2239,7 +2247,7 @@
         <v>0.58333333333333304</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75">
       <c r="A50" s="8">
         <v>0.58333333333333304</v>
       </c>
@@ -2252,10 +2260,10 @@
       <c r="D50" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="31"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
       <c r="I50" s="8">
         <v>0.58333333333333304</v>
       </c>
@@ -2263,21 +2271,21 @@
         <v>0.59722222222222199</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" s="4" customFormat="1" ht="12.75">
       <c r="A51" s="8">
         <v>0.59722222222222199</v>
       </c>
       <c r="B51" s="8">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C51" s="33" t="s">
+      <c r="C51" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="D51" s="33"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
       <c r="I51" s="8">
         <v>0.59722222222222199</v>
       </c>
@@ -2285,21 +2293,21 @@
         <v>0.63888888888888895</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75">
       <c r="A52" s="8">
         <v>0.63888888888888895</v>
       </c>
       <c r="B52" s="8">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C52" s="33" t="s">
+      <c r="C52" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="33"/>
-      <c r="H52" s="33"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
       <c r="I52" s="8">
         <v>0.63888888888888895</v>
       </c>
@@ -2307,20 +2315,16 @@
         <v>0.64583333333333337</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:10" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:10" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:10" s="4" customFormat="1" ht="12.75"/>
+    <row r="54" spans="1:10" s="4" customFormat="1" ht="12.75"/>
+    <row r="55" spans="1:10" s="4" customFormat="1" ht="12.75"/>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="H22:H24"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
     <mergeCell ref="C5:I5"/>
     <mergeCell ref="C12:I12"/>
     <mergeCell ref="C25:I25"/>
     <mergeCell ref="C26:I26"/>
     <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
     <mergeCell ref="I6:I11"/>
     <mergeCell ref="I13:I18"/>
     <mergeCell ref="I19:I24"/>
@@ -2328,6 +2332,7 @@
     <mergeCell ref="H9:H11"/>
     <mergeCell ref="H13:H15"/>
     <mergeCell ref="H16:H18"/>
+    <mergeCell ref="F42:F43"/>
     <mergeCell ref="H19:H21"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="G6:G8"/>
@@ -2339,6 +2344,11 @@
     <mergeCell ref="G16:G18"/>
     <mergeCell ref="F19:F21"/>
     <mergeCell ref="G19:G21"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="G49:G50"/>
     <mergeCell ref="F22:F24"/>
     <mergeCell ref="G22:G24"/>
     <mergeCell ref="C51:H51"/>
@@ -2354,24 +2364,22 @@
     <mergeCell ref="C46:H46"/>
     <mergeCell ref="F40:F41"/>
     <mergeCell ref="G40:G41"/>
-    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="G42:G43"/>
     <mergeCell ref="H38:H41"/>
     <mergeCell ref="H42:H45"/>
     <mergeCell ref="H47:H50"/>
     <mergeCell ref="A33:K33"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
     <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C36:H36"/>
-    <mergeCell ref="C37:H37"/>
-    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2379,14 +2387,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="4"/>
     <col min="3" max="3" width="14.42578125" style="4" customWidth="1"/>
@@ -2399,22 +2407,22 @@
     <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:11" ht="15.75">
+      <c r="A1" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="36" t="s">
         <v>50</v>
       </c>
@@ -2438,21 +2446,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="6">
         <v>0.39583333333333331</v>
       </c>
       <c r="B3" s="6">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
       <c r="I3" s="7">
         <v>0.39583333333333331</v>
       </c>
@@ -2460,21 +2468,21 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15" customHeight="1">
       <c r="A4" s="6">
         <v>0.41666666666666669</v>
       </c>
       <c r="B4" s="7">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
       <c r="I4" s="7">
         <v>0.41666666666666669</v>
       </c>
@@ -2482,21 +2490,21 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="A5" s="6">
         <v>0.45833333333333331</v>
       </c>
       <c r="B5" s="7">
         <v>0.5</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
       <c r="I5" s="7">
         <v>0.45833333333333331</v>
       </c>
@@ -2504,7 +2512,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="8">
         <v>0.5</v>
       </c>
@@ -2536,7 +2544,7 @@
         <v>0.51388888888888895</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="8">
         <v>0.51388888888888895</v>
       </c>
@@ -2568,7 +2576,7 @@
         <v>0.52777777777777801</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="8">
         <v>0.52777777777777801</v>
       </c>
@@ -2600,7 +2608,7 @@
         <v>0.54166666666666696</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="8">
         <v>0.54166666666666696</v>
       </c>
@@ -2632,21 +2640,21 @@
         <v>0.55555555555555602</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="6">
         <v>0.55555555555555558</v>
       </c>
       <c r="B10" s="7">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
       <c r="I10" s="7">
         <v>0.55555555555555558</v>
       </c>
@@ -2654,7 +2662,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" s="8">
         <v>0.58333333333333337</v>
       </c>
@@ -2686,7 +2694,7 @@
         <v>0.59722222222222221</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" s="8">
         <v>0.59722222222222299</v>
       </c>
@@ -2718,7 +2726,7 @@
         <v>0.61111111111111205</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" s="8">
         <v>0.61111111111111205</v>
       </c>
@@ -2750,7 +2758,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" s="8">
         <v>0.625</v>
       </c>
@@ -2782,7 +2790,7 @@
         <v>0.63888888888888895</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" s="8">
         <v>0.63888888888888895</v>
       </c>
@@ -2814,7 +2822,7 @@
         <v>0.65277777777777801</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" s="8">
         <v>0.65277777777777801</v>
       </c>
@@ -2846,7 +2854,7 @@
         <v>0.66666666666666696</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="8">
         <v>0.66666666666666696</v>
       </c>
@@ -2878,7 +2886,7 @@
         <v>0.68055555555555602</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" s="8">
         <v>0.68055555555555602</v>
       </c>
@@ -2910,21 +2918,21 @@
         <v>0.69444444444444453</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="15" customHeight="1">
       <c r="A19" s="6">
         <v>0.69444444444444497</v>
       </c>
       <c r="B19" s="7">
         <v>0.73611111111111116</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
       <c r="I19" s="7">
         <v>0.69444444444444497</v>
       </c>
@@ -2932,21 +2940,21 @@
         <v>0.73611111111111116</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="15" customHeight="1">
       <c r="A20" s="6">
         <v>0.73611111111111205</v>
       </c>
       <c r="B20" s="7">
         <v>0.77083333333333337</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="43"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="45"/>
       <c r="I20" s="7">
         <v>0.73611111111111205</v>
       </c>
@@ -2954,21 +2962,21 @@
         <v>0.77083333333333337</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="15" customHeight="1">
       <c r="A21" s="15">
         <v>0.77083333333333337</v>
       </c>
       <c r="B21" s="16">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
       <c r="I21" s="16">
         <v>0.77083333333333337</v>
       </c>
@@ -2976,7 +2984,7 @@
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="7"/>
       <c r="B22" s="17"/>
       <c r="C22" s="18" t="s">
@@ -3000,7 +3008,7 @@
       <c r="I22" s="7"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="20">
         <v>0.79166666666666663</v>
       </c>
@@ -3032,7 +3040,7 @@
         <v>0.80208333333333337</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="8">
         <v>0.80208333333333337</v>
       </c>
@@ -3064,7 +3072,7 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="8">
         <v>0.8125</v>
       </c>
@@ -3096,7 +3104,7 @@
         <v>0.82291666666666696</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" s="8">
         <v>0.82291666666666696</v>
       </c>
@@ -3128,7 +3136,7 @@
         <v>0.83333333333333404</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" s="8">
         <v>0.83333333333333404</v>
       </c>
@@ -3160,7 +3168,7 @@
         <v>0.84375</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" s="8">
         <v>0.84375</v>
       </c>
@@ -3192,7 +3200,7 @@
         <v>0.85416666666666696</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" s="8">
         <v>0.85416666666666696</v>
       </c>
@@ -3224,7 +3232,7 @@
         <v>0.86458333333333404</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" s="8">
         <v>0.86458333333333404</v>
       </c>
@@ -3256,7 +3264,7 @@
         <v>0.875000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" s="8">
         <v>0.875000000000001</v>
       </c>
@@ -3288,7 +3296,7 @@
         <v>0.88541666666666696</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" s="8">
         <v>0.88541666666666696</v>
       </c>
@@ -3320,7 +3328,7 @@
         <v>0.89583333333333404</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11">
       <c r="A33" s="8">
         <v>0.89583333333333404</v>
       </c>
@@ -3352,7 +3360,7 @@
         <v>0.906250000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11">
       <c r="A34" s="8">
         <v>0.906250000000001</v>
       </c>
@@ -3384,21 +3392,21 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11">
       <c r="A35" s="6">
         <v>0.91666666666666663</v>
       </c>
       <c r="B35" s="7">
         <v>0</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="42"/>
       <c r="I35" s="7">
         <v>0.91666666666666663</v>
       </c>
@@ -3406,21 +3414,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11">
       <c r="A36" s="6">
         <v>0</v>
       </c>
       <c r="B36" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="42"/>
       <c r="I36" s="7">
         <v>0</v>
       </c>
@@ -3428,7 +3436,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="22"/>
@@ -3440,7 +3448,7 @@
       <c r="I37" s="21"/>
       <c r="J37" s="21"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11">
       <c r="A38" s="21"/>
       <c r="B38" s="21"/>
       <c r="C38" s="22"/>
@@ -3450,7 +3458,7 @@
       <c r="G38" s="22"/>
       <c r="H38" s="22"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="22"/>
@@ -3460,22 +3468,22 @@
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
     </row>
-    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
+    <row r="40" spans="1:11" ht="15.75">
+      <c r="A40" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -3488,7 +3496,7 @@
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="A42" s="34" t="s">
         <v>51</v>
       </c>
@@ -3515,22 +3523,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="A43" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="B43" s="8">
         <v>0.3611111111111111</v>
       </c>
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="46"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="48"/>
       <c r="J43" s="8">
         <v>0.33333333333333331</v>
       </c>
@@ -3538,22 +3546,22 @@
         <v>0.3611111111111111</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11">
       <c r="A44" s="8">
         <v>0.3611111111111111</v>
       </c>
       <c r="B44" s="8">
         <v>0.3888888888888889</v>
       </c>
-      <c r="C44" s="44" t="s">
+      <c r="C44" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="46"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="48"/>
       <c r="J44" s="8">
         <v>0.3611111111111111</v>
       </c>
@@ -3561,7 +3569,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="A45" s="8">
         <v>0.3888888888888889</v>
       </c>
@@ -3596,7 +3604,7 @@
         <v>0.40277777777777773</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="A46" s="8">
         <v>0.40277777777777801</v>
       </c>
@@ -3631,7 +3639,7 @@
         <v>0.41666666666666702</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11">
       <c r="A47" s="8">
         <v>0.41666666666666702</v>
       </c>
@@ -3666,7 +3674,7 @@
         <v>0.43055555555555602</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11">
       <c r="A48" s="8">
         <v>0.43055555555555602</v>
       </c>
@@ -3701,7 +3709,7 @@
         <v>0.44444444444444497</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11">
       <c r="A49" s="8">
         <v>0.44444444444444497</v>
       </c>
@@ -3736,7 +3744,7 @@
         <v>0.45833333333333298</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11">
       <c r="A50" s="8">
         <v>0.45833333333333298</v>
       </c>
@@ -3771,7 +3779,7 @@
         <v>0.47222222222222199</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11">
       <c r="A51" s="8">
         <v>0.47222222222222199</v>
       </c>
@@ -3806,7 +3814,7 @@
         <v>0.48611111111111099</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11">
       <c r="A52" s="8">
         <v>0.48611111111111099</v>
       </c>
@@ -3841,22 +3849,22 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11">
       <c r="A53" s="8">
         <v>0.5</v>
       </c>
       <c r="B53" s="8">
         <v>0.52777777777777779</v>
       </c>
-      <c r="C53" s="41" t="s">
+      <c r="C53" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="43"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="44"/>
+      <c r="H53" s="44"/>
+      <c r="I53" s="45"/>
       <c r="J53" s="8">
         <v>0.5</v>
       </c>
@@ -3864,7 +3872,7 @@
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11">
       <c r="A54" s="8">
         <v>0.52777777777777779</v>
       </c>
@@ -3899,7 +3907,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11">
       <c r="A55" s="8">
         <v>0.54166666666666696</v>
       </c>
@@ -3934,7 +3942,7 @@
         <v>0.55555555555555602</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11">
       <c r="A56" s="8">
         <v>0.55555555555555602</v>
       </c>
@@ -3969,7 +3977,7 @@
         <v>0.56944444444444398</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11">
       <c r="A57" s="8">
         <v>0.56944444444444398</v>
       </c>
@@ -4004,7 +4012,7 @@
         <v>0.58333333333333304</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11">
       <c r="A58" s="8">
         <v>0.58333333333333304</v>
       </c>
@@ -4039,7 +4047,7 @@
         <v>0.59722222222222199</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11">
       <c r="A59" s="8">
         <v>0.59722222222222199</v>
       </c>
@@ -4074,7 +4082,7 @@
         <v>0.61111111111111105</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11">
       <c r="A60" s="8">
         <v>0.61111111111111105</v>
       </c>
@@ -4109,7 +4117,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11">
       <c r="A61" s="8">
         <v>0.625</v>
       </c>
@@ -4144,22 +4152,22 @@
         <v>0.63888888888888895</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11">
       <c r="A62" s="8">
         <v>0.63888888888888895</v>
       </c>
       <c r="B62" s="8">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C62" s="44" t="s">
+      <c r="C62" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="D62" s="45"/>
-      <c r="E62" s="45"/>
-      <c r="F62" s="45"/>
-      <c r="G62" s="45"/>
-      <c r="H62" s="45"/>
-      <c r="I62" s="46"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="47"/>
+      <c r="F62" s="47"/>
+      <c r="G62" s="47"/>
+      <c r="H62" s="47"/>
+      <c r="I62" s="48"/>
       <c r="J62" s="8">
         <v>0.63888888888888895</v>
       </c>
@@ -4169,6 +4177,8 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C43:I43"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A40:K40"/>
@@ -4184,8 +4194,6 @@
     <mergeCell ref="C36:H36"/>
     <mergeCell ref="C44:I44"/>
     <mergeCell ref="C53:I53"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C43:I43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4193,14 +4201,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18:AB19"/>
+      <selection activeCell="G9" sqref="G9:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="8.28515625" customWidth="1"/>
     <col min="4" max="13" width="6.7109375" customWidth="1"/>
@@ -4209,25 +4217,25 @@
     <col min="16" max="24" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="C1" s="51" t="s">
+    <row r="1" spans="1:30">
+      <c r="C1" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+    </row>
+    <row r="2" spans="1:30">
       <c r="A2" s="2" t="s">
         <v>108</v>
       </c>
@@ -4317,7 +4325,7 @@
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3" s="2" t="s">
         <v>109</v>
       </c>
@@ -4405,24 +4413,24 @@
       </c>
       <c r="AD3" s="2"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="50" t="s">
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K4" s="50"/>
+      <c r="K4" s="52"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -4435,16 +4443,16 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
-      <c r="X4" s="47" t="s">
+      <c r="X4" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y4" s="48"/>
-      <c r="Z4" s="49"/>
-      <c r="AA4" s="47"/>
-      <c r="AB4" s="49"/>
+      <c r="Y4" s="50"/>
+      <c r="Z4" s="51"/>
+      <c r="AA4" s="49"/>
+      <c r="AB4" s="51"/>
       <c r="AC4" s="2"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -4453,39 +4461,39 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="50" t="s">
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="50"/>
-      <c r="L5" s="47" t="s">
+      <c r="K5" s="52"/>
+      <c r="L5" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="48"/>
-      <c r="T5" s="48"/>
-      <c r="U5" s="48"/>
-      <c r="V5" s="48"/>
-      <c r="W5" s="49"/>
-      <c r="X5" s="47" t="s">
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="50"/>
+      <c r="T5" s="50"/>
+      <c r="U5" s="50"/>
+      <c r="V5" s="50"/>
+      <c r="W5" s="51"/>
+      <c r="X5" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y5" s="48"/>
-      <c r="Z5" s="49"/>
+      <c r="Y5" s="50"/>
+      <c r="Z5" s="51"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -4497,10 +4505,10 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="50" t="s">
+      <c r="J6" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="50"/>
+      <c r="K6" s="52"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -4513,16 +4521,16 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
-      <c r="X6" s="47" t="s">
+      <c r="X6" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y6" s="48"/>
-      <c r="Z6" s="49"/>
+      <c r="Y6" s="50"/>
+      <c r="Z6" s="51"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -4534,10 +4542,10 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="50" t="s">
+      <c r="J7" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K7" s="50"/>
+      <c r="K7" s="52"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -4550,16 +4558,16 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
-      <c r="X7" s="47" t="s">
+      <c r="X7" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y7" s="48"/>
-      <c r="Z7" s="49"/>
+      <c r="Y7" s="50"/>
+      <c r="Z7" s="51"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -4571,36 +4579,36 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="50" t="s">
+      <c r="J8" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="50"/>
-      <c r="L8" s="47" t="s">
+      <c r="K8" s="52"/>
+      <c r="L8" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="48"/>
-      <c r="U8" s="48"/>
-      <c r="V8" s="48"/>
-      <c r="W8" s="49"/>
-      <c r="X8" s="47" t="s">
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="50"/>
+      <c r="S8" s="50"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="50"/>
+      <c r="V8" s="50"/>
+      <c r="W8" s="51"/>
+      <c r="X8" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y8" s="48"/>
-      <c r="Z8" s="49"/>
-      <c r="AA8" s="47" t="s">
+      <c r="Y8" s="50"/>
+      <c r="Z8" s="51"/>
+      <c r="AA8" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="AB8" s="49"/>
+      <c r="AB8" s="51"/>
       <c r="AC8" s="2"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
@@ -4609,15 +4617,15 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="47" t="s">
+      <c r="G9" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="48"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="50" t="s">
+      <c r="H9" s="50"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="50"/>
+      <c r="K9" s="52"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -4630,18 +4638,18 @@
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
-      <c r="X9" s="47" t="s">
+      <c r="X9" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y9" s="48"/>
-      <c r="Z9" s="49"/>
-      <c r="AA9" s="47" t="s">
+      <c r="Y9" s="50"/>
+      <c r="Z9" s="51"/>
+      <c r="AA9" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="AB9" s="49"/>
+      <c r="AB9" s="51"/>
       <c r="AC9" s="2"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -4653,10 +4661,10 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="50" t="s">
+      <c r="J10" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K10" s="50"/>
+      <c r="K10" s="52"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -4669,16 +4677,16 @@
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
-      <c r="X10" s="47" t="s">
+      <c r="X10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y10" s="48"/>
-      <c r="Z10" s="49"/>
+      <c r="Y10" s="50"/>
+      <c r="Z10" s="51"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
@@ -4690,38 +4698,38 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="50" t="s">
+      <c r="J11" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50" t="s">
+      <c r="K11" s="52"/>
+      <c r="L11" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50" t="s">
+      <c r="M11" s="52"/>
+      <c r="N11" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="O11" s="50"/>
-      <c r="P11" s="50" t="s">
+      <c r="O11" s="52"/>
+      <c r="P11" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="Q11" s="50"/>
+      <c r="Q11" s="52"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
-      <c r="X11" s="47" t="s">
+      <c r="X11" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y11" s="48"/>
-      <c r="Z11" s="49"/>
+      <c r="Y11" s="50"/>
+      <c r="Z11" s="51"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -4733,34 +4741,34 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="50" t="s">
+      <c r="J12" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50"/>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="50"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
-      <c r="X12" s="47" t="s">
+      <c r="X12" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y12" s="48"/>
-      <c r="Z12" s="49"/>
-      <c r="AA12" s="47" t="s">
+      <c r="Y12" s="50"/>
+      <c r="Z12" s="51"/>
+      <c r="AA12" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="AB12" s="49"/>
+      <c r="AB12" s="51"/>
       <c r="AC12" s="2"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -4769,15 +4777,15 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="47" t="s">
+      <c r="G13" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="H13" s="48"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="50" t="s">
+      <c r="H13" s="50"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K13" s="50"/>
+      <c r="K13" s="52"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -4790,18 +4798,18 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-      <c r="X13" s="47" t="s">
+      <c r="X13" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y13" s="48"/>
-      <c r="Z13" s="49"/>
-      <c r="AA13" s="47" t="s">
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="51"/>
+      <c r="AA13" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="AB13" s="49"/>
+      <c r="AB13" s="51"/>
       <c r="AC13" s="2"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
@@ -4813,55 +4821,55 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="50" t="s">
+      <c r="J14" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50" t="s">
+      <c r="K14" s="52"/>
+      <c r="L14" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50" t="s">
+      <c r="M14" s="52"/>
+      <c r="N14" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="O14" s="50"/>
-      <c r="P14" s="50" t="s">
+      <c r="O14" s="52"/>
+      <c r="P14" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="Q14" s="50"/>
+      <c r="Q14" s="52"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
-      <c r="X14" s="47" t="s">
+      <c r="X14" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y14" s="48"/>
-      <c r="Z14" s="49"/>
+      <c r="Y14" s="50"/>
+      <c r="Z14" s="51"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="50" t="s">
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K15" s="50"/>
+      <c r="K15" s="52"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -4874,16 +4882,16 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
-      <c r="X15" s="47" t="s">
+      <c r="X15" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y15" s="48"/>
-      <c r="Z15" s="49"/>
+      <c r="Y15" s="50"/>
+      <c r="Z15" s="51"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
@@ -4895,10 +4903,10 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="50" t="s">
+      <c r="J16" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K16" s="50"/>
+      <c r="K16" s="52"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -4911,16 +4919,16 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
-      <c r="X16" s="47" t="s">
+      <c r="X16" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y16" s="48"/>
-      <c r="Z16" s="49"/>
+      <c r="Y16" s="50"/>
+      <c r="Z16" s="51"/>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
@@ -4932,10 +4940,10 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="50" t="s">
+      <c r="J17" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K17" s="50"/>
+      <c r="K17" s="52"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -4948,16 +4956,16 @@
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
-      <c r="X17" s="47" t="s">
+      <c r="X17" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y17" s="48"/>
-      <c r="Z17" s="49"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="51"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
@@ -4969,15 +4977,15 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="50" t="s">
+      <c r="J18" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K18" s="50"/>
-      <c r="L18" s="47" t="s">
+      <c r="K18" s="52"/>
+      <c r="L18" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="M18" s="48"/>
-      <c r="N18" s="49"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="51"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -4987,18 +4995,18 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
-      <c r="X18" s="47" t="s">
+      <c r="X18" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y18" s="48"/>
-      <c r="Z18" s="49"/>
-      <c r="AA18" s="47" t="s">
+      <c r="Y18" s="50"/>
+      <c r="Z18" s="51"/>
+      <c r="AA18" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="AB18" s="49"/>
+      <c r="AB18" s="51"/>
       <c r="AC18" s="2"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
@@ -5010,10 +5018,10 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="50" t="s">
+      <c r="J19" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="50"/>
+      <c r="K19" s="52"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -5026,18 +5034,18 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
-      <c r="X19" s="47" t="s">
+      <c r="X19" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y19" s="48"/>
-      <c r="Z19" s="49"/>
-      <c r="AA19" s="47" t="s">
+      <c r="Y19" s="50"/>
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="AB19" s="49"/>
+      <c r="AB19" s="51"/>
       <c r="AC19" s="2"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -5049,10 +5057,10 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="50" t="s">
+      <c r="J20" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K20" s="50"/>
+      <c r="K20" s="52"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -5065,16 +5073,16 @@
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
-      <c r="X20" s="47" t="s">
+      <c r="X20" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y20" s="48"/>
-      <c r="Z20" s="49"/>
+      <c r="Y20" s="50"/>
+      <c r="Z20" s="51"/>
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
@@ -5086,10 +5094,10 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="50" t="s">
+      <c r="J21" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K21" s="50"/>
+      <c r="K21" s="52"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -5102,16 +5110,16 @@
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
-      <c r="X21" s="47" t="s">
+      <c r="X21" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y21" s="48"/>
-      <c r="Z21" s="49"/>
+      <c r="Y21" s="50"/>
+      <c r="Z21" s="51"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
@@ -5123,10 +5131,10 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="50" t="s">
+      <c r="J22" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K22" s="50"/>
+      <c r="K22" s="52"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -5139,16 +5147,16 @@
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
-      <c r="X22" s="47" t="s">
+      <c r="X22" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y22" s="48"/>
-      <c r="Z22" s="49"/>
+      <c r="Y22" s="50"/>
+      <c r="Z22" s="51"/>
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
@@ -5160,10 +5168,10 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="50" t="s">
+      <c r="J23" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K23" s="50"/>
+      <c r="K23" s="52"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -5176,16 +5184,16 @@
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
-      <c r="X23" s="47" t="s">
+      <c r="X23" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y23" s="48"/>
-      <c r="Z23" s="49"/>
+      <c r="Y23" s="50"/>
+      <c r="Z23" s="51"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
@@ -5197,10 +5205,10 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="50" t="s">
+      <c r="J24" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K24" s="50"/>
+      <c r="K24" s="52"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -5213,16 +5221,16 @@
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
-      <c r="X24" s="47" t="s">
+      <c r="X24" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y24" s="48"/>
-      <c r="Z24" s="49"/>
+      <c r="Y24" s="50"/>
+      <c r="Z24" s="51"/>
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
@@ -5234,10 +5242,10 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="50" t="s">
+      <c r="J25" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K25" s="50"/>
+      <c r="K25" s="52"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -5250,16 +5258,16 @@
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
-      <c r="X25" s="47" t="s">
+      <c r="X25" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y25" s="48"/>
-      <c r="Z25" s="49"/>
+      <c r="Y25" s="50"/>
+      <c r="Z25" s="51"/>
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
@@ -5271,10 +5279,10 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="50" t="s">
+      <c r="J26" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K26" s="50"/>
+      <c r="K26" s="52"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -5287,16 +5295,16 @@
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
-      <c r="X26" s="47" t="s">
+      <c r="X26" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y26" s="48"/>
-      <c r="Z26" s="49"/>
+      <c r="Y26" s="50"/>
+      <c r="Z26" s="51"/>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
@@ -5308,10 +5316,10 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="50" t="s">
+      <c r="J27" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K27" s="50"/>
+      <c r="K27" s="52"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -5324,16 +5332,16 @@
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
-      <c r="X27" s="47" t="s">
+      <c r="X27" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y27" s="48"/>
-      <c r="Z27" s="49"/>
+      <c r="Y27" s="50"/>
+      <c r="Z27" s="51"/>
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
@@ -5345,10 +5353,10 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="50" t="s">
+      <c r="J28" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K28" s="50"/>
+      <c r="K28" s="52"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -5361,16 +5369,16 @@
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
-      <c r="X28" s="47" t="s">
+      <c r="X28" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y28" s="48"/>
-      <c r="Z28" s="49"/>
+      <c r="Y28" s="50"/>
+      <c r="Z28" s="51"/>
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
@@ -5382,10 +5390,10 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="50" t="s">
+      <c r="J29" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K29" s="50"/>
+      <c r="K29" s="52"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -5398,16 +5406,16 @@
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
-      <c r="X29" s="47" t="s">
+      <c r="X29" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y29" s="48"/>
-      <c r="Z29" s="49"/>
+      <c r="Y29" s="50"/>
+      <c r="Z29" s="51"/>
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
@@ -5419,10 +5427,10 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="50" t="s">
+      <c r="J30" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K30" s="50"/>
+      <c r="K30" s="52"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -5435,16 +5443,16 @@
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
-      <c r="X30" s="47" t="s">
+      <c r="X30" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y30" s="48"/>
-      <c r="Z30" s="49"/>
+      <c r="Y30" s="50"/>
+      <c r="Z30" s="51"/>
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
@@ -5456,10 +5464,10 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="50" t="s">
+      <c r="J31" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K31" s="50"/>
+      <c r="K31" s="52"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -5472,16 +5480,16 @@
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
-      <c r="X31" s="47" t="s">
+      <c r="X31" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y31" s="48"/>
-      <c r="Z31" s="49"/>
+      <c r="Y31" s="50"/>
+      <c r="Z31" s="51"/>
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
@@ -5493,10 +5501,10 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="50" t="s">
+      <c r="J32" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K32" s="50"/>
+      <c r="K32" s="52"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5509,16 +5517,16 @@
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
-      <c r="X32" s="47" t="s">
+      <c r="X32" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y32" s="48"/>
-      <c r="Z32" s="49"/>
+      <c r="Y32" s="50"/>
+      <c r="Z32" s="51"/>
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
@@ -5530,10 +5538,10 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="50" t="s">
+      <c r="J33" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K33" s="50"/>
+      <c r="K33" s="52"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5546,16 +5554,16 @@
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
-      <c r="X33" s="47" t="s">
+      <c r="X33" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y33" s="48"/>
-      <c r="Z33" s="49"/>
+      <c r="Y33" s="50"/>
+      <c r="Z33" s="51"/>
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
@@ -5567,10 +5575,10 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="50" t="s">
+      <c r="J34" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K34" s="50"/>
+      <c r="K34" s="52"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5583,16 +5591,16 @@
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
-      <c r="X34" s="47" t="s">
+      <c r="X34" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y34" s="48"/>
-      <c r="Z34" s="49"/>
+      <c r="Y34" s="50"/>
+      <c r="Z34" s="51"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
@@ -5604,10 +5612,10 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="50" t="s">
+      <c r="J35" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K35" s="50"/>
+      <c r="K35" s="52"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5620,16 +5628,16 @@
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
-      <c r="X35" s="47" t="s">
+      <c r="X35" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y35" s="48"/>
-      <c r="Z35" s="49"/>
+      <c r="Y35" s="50"/>
+      <c r="Z35" s="51"/>
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
       <c r="AC35" s="2"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
@@ -5641,10 +5649,10 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="50" t="s">
+      <c r="J36" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K36" s="50"/>
+      <c r="K36" s="52"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5657,16 +5665,16 @@
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
       <c r="W36" s="2"/>
-      <c r="X36" s="47" t="s">
+      <c r="X36" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y36" s="48"/>
-      <c r="Z36" s="49"/>
+      <c r="Y36" s="50"/>
+      <c r="Z36" s="51"/>
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
       <c r="AC36" s="2"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
@@ -5678,10 +5686,10 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="50" t="s">
+      <c r="J37" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="K37" s="50"/>
+      <c r="K37" s="52"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5694,11 +5702,11 @@
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
       <c r="W37" s="2"/>
-      <c r="X37" s="47" t="s">
+      <c r="X37" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="Y37" s="48"/>
-      <c r="Z37" s="49"/>
+      <c r="Y37" s="50"/>
+      <c r="Z37" s="51"/>
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
       <c r="AC37" s="2"/>

</xml_diff>

<commit_message>
Finished the new ExcelDataReader. The format of the excel-file was altered to make things work in this way: - exact date and time in first 2 columns, and the cell format set accordingly. - no more vertically stretched cells. horizontally stretched cells work, but cant do both
</commit_message>
<xml_diff>
--- a/BarcodeScanner/planning kinderen en leiding.xlsx
+++ b/BarcodeScanner/planning kinderen en leiding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="-150" windowWidth="19320" windowHeight="12120" activeTab="1"/>
+    <workbookView xWindow="1590" yWindow="-150" windowWidth="19320" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="Kleine speltakken" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="114">
   <si>
     <t>Avondeten</t>
   </si>
@@ -150,9 +150,6 @@
     <t>13 + 14 + 15+ 16 + 17 + 18</t>
   </si>
   <si>
-    <t>19 + 20 + 21 + 22 + 23 + 24</t>
-  </si>
-  <si>
     <t>13 + 14 + 15 + 16 + 17 + 18 + 19 + 20 + 21 + 22 + 23 + 24</t>
   </si>
   <si>
@@ -358,6 +355,9 @@
   </si>
   <si>
     <t>Spullen klaarleggen</t>
+  </si>
+  <si>
+    <t>25+26+27+28+29+30</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -454,15 +454,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -559,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -582,37 +573,37 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -630,10 +621,10 @@
     <xf numFmtId="20" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -643,37 +634,22 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -682,7 +658,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -691,7 +667,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -700,7 +676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -710,6 +686,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1013,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1022,27 +1001,27 @@
     <col min="1" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="12.75"/>
     <row r="2" spans="1:11" s="4" customFormat="1" ht="15.75">
-      <c r="A2" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
+      <c r="A2" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A3" s="3"/>
@@ -1056,8 +1035,8 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="27" t="s">
         <v>8</v>
       </c>
@@ -1087,15 +1066,15 @@
       <c r="B5" s="29">
         <v>40831.416666666664</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="45"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="6">
         <v>0.39583333333333331</v>
       </c>
@@ -1103,7 +1082,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="12.75">
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A6" s="29">
         <v>40831.416666666664</v>
       </c>
@@ -1119,17 +1098,17 @@
       <c r="E6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="33" t="s">
-        <v>45</v>
+      <c r="I6" s="31" t="s">
+        <v>44</v>
       </c>
       <c r="J6" s="6">
         <v>0.41666666666666669</v>
@@ -1154,10 +1133,18 @@
       <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="42"/>
+      <c r="F7" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>44</v>
+      </c>
       <c r="J7" s="6">
         <v>0.43055555555555558</v>
       </c>
@@ -1181,10 +1168,18 @@
       <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="42"/>
+      <c r="F8" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>44</v>
+      </c>
       <c r="J8" s="6">
         <v>0.44444444444444442</v>
       </c>
@@ -1192,7 +1187,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="12.75">
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A9" s="29">
         <v>40831.458333333336</v>
       </c>
@@ -1208,16 +1203,18 @@
       <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="42"/>
+      <c r="I9" s="31" t="s">
+        <v>44</v>
+      </c>
       <c r="J9" s="6">
         <v>0.45833333333333331</v>
       </c>
@@ -1241,10 +1238,18 @@
       <c r="E10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="42"/>
+      <c r="F10" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>44</v>
+      </c>
       <c r="J10" s="6">
         <v>0.47222222222222199</v>
       </c>
@@ -1268,10 +1273,18 @@
       <c r="E11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="42"/>
+      <c r="F11" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>44</v>
+      </c>
       <c r="J11" s="6">
         <v>0.48611111111111099</v>
       </c>
@@ -1286,15 +1299,15 @@
       <c r="B12" s="30">
         <v>40831.527777777781</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="6">
         <v>0.5</v>
       </c>
@@ -1302,7 +1315,7 @@
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="12.75">
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A13" s="29">
         <v>40831.527777777781</v>
       </c>
@@ -1318,17 +1331,17 @@
       <c r="E13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="39" t="s">
+      <c r="G13" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="39" t="s">
+      <c r="H13" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="42" t="s">
-        <v>46</v>
+      <c r="I13" s="31" t="s">
+        <v>45</v>
       </c>
       <c r="J13" s="6">
         <v>0.52777777777777801</v>
@@ -1353,10 +1366,18 @@
       <c r="E14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="42"/>
+      <c r="F14" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="31" t="s">
+        <v>45</v>
+      </c>
       <c r="J14" s="6">
         <v>0.54166666666666696</v>
       </c>
@@ -1380,10 +1401,18 @@
       <c r="E15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="42"/>
+      <c r="F15" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>45</v>
+      </c>
       <c r="J15" s="6">
         <v>0.55555555555555602</v>
       </c>
@@ -1391,7 +1420,7 @@
         <v>0.56944444444444497</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75">
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A16" s="29">
         <v>40831.569444444445</v>
       </c>
@@ -1407,16 +1436,18 @@
       <c r="E16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="G16" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="I16" s="42"/>
+      <c r="H16" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>45</v>
+      </c>
       <c r="J16" s="6">
         <v>0.56944444444444497</v>
       </c>
@@ -1440,10 +1471,18 @@
       <c r="E17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="42"/>
+      <c r="F17" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>45</v>
+      </c>
       <c r="J17" s="6">
         <v>0.58333333333333404</v>
       </c>
@@ -1467,10 +1506,18 @@
       <c r="E18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="42"/>
+      <c r="F18" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="31" t="s">
+        <v>45</v>
+      </c>
       <c r="J18" s="6">
         <v>0.59722222222222299</v>
       </c>
@@ -1478,7 +1525,7 @@
         <v>0.61111111111111205</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="4" customFormat="1" ht="12.75">
+    <row r="19" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A19" s="29">
         <v>40831.611111111109</v>
       </c>
@@ -1494,17 +1541,17 @@
       <c r="E19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="39" t="s">
+      <c r="G19" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" s="42" t="s">
-        <v>47</v>
+      <c r="H19" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="31" t="s">
+        <v>46</v>
       </c>
       <c r="J19" s="6">
         <v>0.61111111111111205</v>
@@ -1529,10 +1576,18 @@
       <c r="E20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="38"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="42"/>
+      <c r="F20" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="J20" s="6">
         <v>0.625</v>
       </c>
@@ -1556,10 +1611,18 @@
       <c r="E21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="42"/>
+      <c r="F21" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="J21" s="6">
         <v>0.63888888888888895</v>
       </c>
@@ -1567,7 +1630,7 @@
         <v>0.65277777777777801</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" ht="12.75">
+    <row r="22" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A22" s="29">
         <v>40831.652777777781</v>
       </c>
@@ -1583,16 +1646,18 @@
       <c r="E22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="H22" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="I22" s="42"/>
+      <c r="G22" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="J22" s="6">
         <v>0.65277777777777801</v>
       </c>
@@ -1616,10 +1681,18 @@
       <c r="E23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="42"/>
+      <c r="F23" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="J23" s="6">
         <v>0.66666666666666696</v>
       </c>
@@ -1643,10 +1716,18 @@
       <c r="E24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="33"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="42"/>
+      <c r="F24" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="H24" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="I24" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="J24" s="6">
         <v>0.68055555555555602</v>
       </c>
@@ -1661,15 +1742,15 @@
       <c r="B25" s="30">
         <v>40831.736111111109</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
       <c r="J25" s="6">
         <v>0.69444444444444497</v>
       </c>
@@ -1684,15 +1765,15 @@
       <c r="B26" s="30">
         <v>40831.770833333336</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
       <c r="J26" s="6">
         <v>0.73611111111111205</v>
       </c>
@@ -1707,15 +1788,15 @@
       <c r="B27" s="30">
         <v>40831.791666666664</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
       <c r="J27" s="6">
         <v>0.77083333333333337</v>
       </c>
@@ -1730,15 +1811,15 @@
       <c r="B28" s="30">
         <v>40831.916666666664</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
       <c r="J28" s="6">
         <v>0.79166666666666663</v>
       </c>
@@ -1753,15 +1834,15 @@
       <c r="B29" s="30">
         <v>40831.9375</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
       <c r="J29" s="6">
         <v>0.91666666666666663</v>
       </c>
@@ -1776,15 +1857,15 @@
       <c r="B30" s="30">
         <v>40831.291666666664</v>
       </c>
-      <c r="C30" s="42" t="s">
+      <c r="C30" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
       <c r="J30" s="6">
         <v>0.9375</v>
       </c>
@@ -1817,23 +1898,23 @@
       <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:11" s="4" customFormat="1" ht="15.75">
-      <c r="A33" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
+      <c r="A33" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
     </row>
     <row r="34" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A34" s="34"/>
-      <c r="B34" s="34"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="9" t="s">
         <v>9</v>
       </c>
@@ -1854,20 +1935,20 @@
       </c>
     </row>
     <row r="35" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A35" s="8">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="B35" s="8">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C35" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
+      <c r="A35" s="49">
+        <v>40832.291666666664</v>
+      </c>
+      <c r="B35" s="49">
+        <v>40832.333333333336</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
       <c r="I35" s="8">
         <v>0.29166666666666669</v>
       </c>
@@ -1876,20 +1957,20 @@
       </c>
     </row>
     <row r="36" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A36" s="8">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="B36" s="8">
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="C36" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
+      <c r="A36" s="49">
+        <v>40832.333333333336</v>
+      </c>
+      <c r="B36" s="49">
+        <v>40832.361111111109</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
       <c r="I36" s="8">
         <v>0.33333333333333331</v>
       </c>
@@ -1898,20 +1979,20 @@
       </c>
     </row>
     <row r="37" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A37" s="8">
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="B37" s="8">
-        <v>0.40277777777777773</v>
-      </c>
-      <c r="C37" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="35"/>
-      <c r="H37" s="35"/>
+      <c r="A37" s="49">
+        <v>40832.361111111109</v>
+      </c>
+      <c r="B37" s="49">
+        <v>40832.402777777781</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
       <c r="I37" s="8">
         <v>0.3611111111111111</v>
       </c>
@@ -1920,29 +2001,29 @@
       </c>
     </row>
     <row r="38" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A38" s="8">
-        <v>0.40277777777777801</v>
-      </c>
-      <c r="B38" s="8">
-        <v>0.41666666666666702</v>
+      <c r="A38" s="49">
+        <v>40832.402777777781</v>
+      </c>
+      <c r="B38" s="49">
+        <v>40832.416666666664</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E38" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F38" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="G38" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="H38" s="32" t="s">
-        <v>74</v>
+      <c r="G38" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="H38" s="31" t="s">
+        <v>73</v>
       </c>
       <c r="I38" s="8">
         <v>0.40277777777777801</v>
@@ -1952,22 +2033,30 @@
       </c>
     </row>
     <row r="39" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A39" s="8">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="B39" s="8">
-        <v>0.43055555555555602</v>
+      <c r="A39" s="49">
+        <v>40832.416666666664</v>
+      </c>
+      <c r="B39" s="49">
+        <v>40832.430555555555</v>
       </c>
       <c r="C39" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="38"/>
+      <c r="E39" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="H39" s="31" t="s">
+        <v>73</v>
+      </c>
       <c r="I39" s="8">
         <v>0.41666666666666702</v>
       </c>
@@ -1976,28 +2065,30 @@
       </c>
     </row>
     <row r="40" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A40" s="8">
-        <v>0.43055555555555602</v>
-      </c>
-      <c r="B40" s="8">
-        <v>0.44444444444444497</v>
+      <c r="A40" s="49">
+        <v>40832.430555555555</v>
+      </c>
+      <c r="B40" s="49">
+        <v>40832.444444444445</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E40" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="F40" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="G40" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="H40" s="38"/>
+      <c r="G40" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="H40" s="31" t="s">
+        <v>73</v>
+      </c>
       <c r="I40" s="8">
         <v>0.43055555555555602</v>
       </c>
@@ -2006,22 +2097,30 @@
       </c>
     </row>
     <row r="41" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A41" s="8">
-        <v>0.44444444444444497</v>
-      </c>
-      <c r="B41" s="8">
-        <v>0.45833333333333298</v>
+      <c r="A41" s="49">
+        <v>40832.444444444445</v>
+      </c>
+      <c r="B41" s="49">
+        <v>40832.458333333336</v>
       </c>
       <c r="C41" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
+      <c r="E41" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="G41" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>73</v>
+      </c>
       <c r="I41" s="8">
         <v>0.44444444444444497</v>
       </c>
@@ -2030,29 +2129,29 @@
       </c>
     </row>
     <row r="42" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A42" s="8">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="B42" s="8">
-        <v>0.47222222222222199</v>
+      <c r="A42" s="49">
+        <v>40832.458333333336</v>
+      </c>
+      <c r="B42" s="49">
+        <v>40832.472222222219</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E42" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="F42" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="G42" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H42" s="32" t="s">
-        <v>75</v>
+      <c r="G42" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="H42" s="31" t="s">
+        <v>74</v>
       </c>
       <c r="I42" s="8">
         <v>0.45833333333333298</v>
@@ -2062,22 +2161,30 @@
       </c>
     </row>
     <row r="43" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A43" s="8">
-        <v>0.47222222222222199</v>
-      </c>
-      <c r="B43" s="8">
-        <v>0.48611111111111099</v>
+      <c r="A43" s="49">
+        <v>40832.472222222219</v>
+      </c>
+      <c r="B43" s="49">
+        <v>40832.486111111109</v>
       </c>
       <c r="C43" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="38"/>
+      <c r="E43" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="F43" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="G43" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="H43" s="31" t="s">
+        <v>74</v>
+      </c>
       <c r="I43" s="8">
         <v>0.47222222222222199</v>
       </c>
@@ -2086,28 +2193,30 @@
       </c>
     </row>
     <row r="44" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A44" s="8">
-        <v>0.48611111111111099</v>
-      </c>
-      <c r="B44" s="8">
-        <v>0.5</v>
+      <c r="A44" s="49">
+        <v>40832.486111111109</v>
+      </c>
+      <c r="B44" s="49">
+        <v>40832.5</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="F44" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="F44" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="G44" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="H44" s="38"/>
+      <c r="G44" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="H44" s="31" t="s">
+        <v>74</v>
+      </c>
       <c r="I44" s="8">
         <v>0.48611111111111099</v>
       </c>
@@ -2116,22 +2225,30 @@
       </c>
     </row>
     <row r="45" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A45" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="B45" s="8">
-        <v>0.51388888888888895</v>
+      <c r="A45" s="49">
+        <v>40832.5</v>
+      </c>
+      <c r="B45" s="49">
+        <v>40832.513888888891</v>
       </c>
       <c r="C45" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
+      <c r="E45" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="G45" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>74</v>
+      </c>
       <c r="I45" s="8">
         <v>0.5</v>
       </c>
@@ -2140,20 +2257,20 @@
       </c>
     </row>
     <row r="46" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A46" s="8">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="B46" s="8">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C46" s="42" t="s">
+      <c r="A46" s="49">
+        <v>40832.513888888891</v>
+      </c>
+      <c r="B46" s="49">
+        <v>40832.541666666664</v>
+      </c>
+      <c r="C46" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
       <c r="I46" s="8">
         <v>0.51388888888888895</v>
       </c>
@@ -2162,29 +2279,29 @@
       </c>
     </row>
     <row r="47" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A47" s="8">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="B47" s="8">
-        <v>0.55555555555555602</v>
+      <c r="A47" s="49">
+        <v>40832.541666666664</v>
+      </c>
+      <c r="B47" s="49">
+        <v>40832.555555555555</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F47" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="F47" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G47" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="H47" s="32" t="s">
-        <v>76</v>
+      <c r="G47" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H47" s="31" t="s">
+        <v>75</v>
       </c>
       <c r="I47" s="8">
         <v>0.54166666666666696</v>
@@ -2194,22 +2311,30 @@
       </c>
     </row>
     <row r="48" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A48" s="8">
-        <v>0.55555555555555602</v>
-      </c>
-      <c r="B48" s="8">
-        <v>0.56944444444444398</v>
+      <c r="A48" s="49">
+        <v>40832.555555555555</v>
+      </c>
+      <c r="B48" s="49">
+        <v>40832.569444444445</v>
       </c>
       <c r="C48" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="38"/>
+      <c r="E48" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F48" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="G48" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H48" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="I48" s="8">
         <v>0.55555555555555602</v>
       </c>
@@ -2218,28 +2343,30 @@
       </c>
     </row>
     <row r="49" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A49" s="8">
-        <v>0.56944444444444398</v>
-      </c>
-      <c r="B49" s="8">
-        <v>0.58333333333333304</v>
+      <c r="A49" s="49">
+        <v>40832.569444444445</v>
+      </c>
+      <c r="B49" s="49">
+        <v>40832.583333333336</v>
       </c>
       <c r="C49" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="F49" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E49" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F49" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="G49" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="H49" s="38"/>
+      <c r="G49" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H49" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="I49" s="8">
         <v>0.56944444444444398</v>
       </c>
@@ -2248,22 +2375,30 @@
       </c>
     </row>
     <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A50" s="8">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="B50" s="8">
-        <v>0.59722222222222199</v>
+      <c r="A50" s="49">
+        <v>40832.583333333336</v>
+      </c>
+      <c r="B50" s="49">
+        <v>40832.597222222219</v>
       </c>
       <c r="C50" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="E50" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="F50" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
+      <c r="G50" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H50" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="I50" s="8">
         <v>0.58333333333333304</v>
       </c>
@@ -2272,20 +2407,20 @@
       </c>
     </row>
     <row r="51" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A51" s="8">
-        <v>0.59722222222222199</v>
-      </c>
-      <c r="B51" s="8">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="C51" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="35"/>
+      <c r="A51" s="49">
+        <v>40832.597222222219</v>
+      </c>
+      <c r="B51" s="49">
+        <v>40832.638888888891</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="34"/>
+      <c r="G51" s="34"/>
+      <c r="H51" s="34"/>
       <c r="I51" s="8">
         <v>0.59722222222222199</v>
       </c>
@@ -2294,20 +2429,20 @@
       </c>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A52" s="8">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="B52" s="8">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="C52" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="35"/>
+      <c r="A52" s="49">
+        <v>40832.638888888891</v>
+      </c>
+      <c r="B52" s="49">
+        <v>40832.645833333336</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="34"/>
       <c r="I52" s="8">
         <v>0.63888888888888895</v>
       </c>
@@ -2319,67 +2454,25 @@
     <row r="54" spans="1:10" s="4" customFormat="1" ht="12.75"/>
     <row r="55" spans="1:10" s="4" customFormat="1" ht="12.75"/>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="18">
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C28:I28"/>
     <mergeCell ref="C5:I5"/>
     <mergeCell ref="C12:I12"/>
     <mergeCell ref="C25:I25"/>
     <mergeCell ref="C26:I26"/>
     <mergeCell ref="C27:I27"/>
-    <mergeCell ref="I6:I11"/>
-    <mergeCell ref="I13:I18"/>
-    <mergeCell ref="I19:I24"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="H22:H24"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="G22:G24"/>
     <mergeCell ref="C51:H51"/>
     <mergeCell ref="C52:H52"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
     <mergeCell ref="C46:H46"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
     <mergeCell ref="A2:K2"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="C35:H35"/>
     <mergeCell ref="C36:H36"/>
     <mergeCell ref="C37:H37"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="H38:H41"/>
-    <mergeCell ref="H42:H45"/>
-    <mergeCell ref="H47:H50"/>
     <mergeCell ref="A33:K33"/>
-    <mergeCell ref="F49:F50"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2390,8 +2483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2408,25 +2501,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
+      <c r="A1" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="37"/>
+      <c r="A2" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="36"/>
       <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
@@ -2453,14 +2546,14 @@
       <c r="B3" s="6">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="7">
         <v>0.39583333333333331</v>
       </c>
@@ -2475,14 +2568,14 @@
       <c r="B4" s="7">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C4" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="C4" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
       <c r="I4" s="7">
         <v>0.41666666666666669</v>
       </c>
@@ -2497,14 +2590,14 @@
       <c r="B5" s="7">
         <v>0.5</v>
       </c>
-      <c r="C5" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
+      <c r="C5" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
       <c r="I5" s="7">
         <v>0.45833333333333331</v>
       </c>
@@ -2520,22 +2613,22 @@
         <v>0.51388888888888895</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>82</v>
-      </c>
       <c r="G6" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I6" s="25">
         <v>0.5</v>
@@ -2552,22 +2645,22 @@
         <v>0.52777777777777801</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>80</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>81</v>
       </c>
       <c r="I7" s="25">
         <v>0.51388888888888895</v>
@@ -2584,22 +2677,22 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>83</v>
-      </c>
       <c r="E8" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I8" s="25">
         <v>0.52777777777777801</v>
@@ -2616,22 +2709,22 @@
         <v>0.55555555555555602</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>83</v>
       </c>
       <c r="I9" s="25">
         <v>0.54166666666666696</v>
@@ -2647,14 +2740,14 @@
       <c r="B10" s="7">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
       <c r="I10" s="7">
         <v>0.55555555555555558</v>
       </c>
@@ -2670,22 +2763,22 @@
         <v>0.59722222222222221</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="E11" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>86</v>
-      </c>
       <c r="G11" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I11" s="25">
         <v>0.58333333333333337</v>
@@ -2702,22 +2795,22 @@
         <v>0.61111111111111205</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>84</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="I12" s="25">
         <v>0.59722222222222299</v>
@@ -2734,22 +2827,22 @@
         <v>0.625</v>
       </c>
       <c r="C13" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>87</v>
-      </c>
       <c r="E13" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I13" s="25">
         <v>0.61111111111111205</v>
@@ -2766,22 +2859,22 @@
         <v>0.63888888888888895</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>86</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>87</v>
       </c>
       <c r="I14" s="25">
         <v>0.625</v>
@@ -2798,22 +2891,22 @@
         <v>0.65277777777777801</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="E15" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>90</v>
-      </c>
       <c r="G15" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I15" s="25">
         <v>0.63888888888888895</v>
@@ -2830,22 +2923,22 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="12" t="s">
         <v>88</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>89</v>
       </c>
       <c r="I16" s="25">
         <v>0.65277777777777801</v>
@@ -2862,22 +2955,22 @@
         <v>0.68055555555555602</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>91</v>
-      </c>
       <c r="E17" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I17" s="25">
         <v>0.66666666666666696</v>
@@ -2894,22 +2987,22 @@
         <v>0.69444444444444453</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>91</v>
       </c>
       <c r="I18" s="25">
         <v>0.68055555555555602</v>
@@ -2925,14 +3018,14 @@
       <c r="B19" s="7">
         <v>0.73611111111111116</v>
       </c>
-      <c r="C19" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
+      <c r="C19" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
       <c r="I19" s="7">
         <v>0.69444444444444497</v>
       </c>
@@ -2947,14 +3040,14 @@
       <c r="B20" s="7">
         <v>0.77083333333333337</v>
       </c>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="45"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="40"/>
       <c r="I20" s="7">
         <v>0.73611111111111205</v>
       </c>
@@ -2969,14 +3062,14 @@
       <c r="B21" s="16">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
       <c r="I21" s="16">
         <v>0.77083333333333337</v>
       </c>
@@ -3016,22 +3109,22 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="C23" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="E23" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>82</v>
-      </c>
       <c r="H23" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I23" s="26">
         <v>0.79166666666666663</v>
@@ -3048,22 +3141,22 @@
         <v>0.8125</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I24" s="25">
         <v>0.80208333333333337</v>
@@ -3080,22 +3173,22 @@
         <v>0.82291666666666696</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>83</v>
-      </c>
       <c r="E25" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I25" s="25">
         <v>0.8125</v>
@@ -3112,22 +3205,22 @@
         <v>0.83333333333333404</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I26" s="25">
         <v>0.82291666666666696</v>
@@ -3144,22 +3237,22 @@
         <v>0.84375</v>
       </c>
       <c r="C27" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="E27" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>86</v>
-      </c>
       <c r="H27" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I27" s="25">
         <v>0.83333333333333404</v>
@@ -3176,22 +3269,22 @@
         <v>0.85416666666666696</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I28" s="25">
         <v>0.84375</v>
@@ -3208,22 +3301,22 @@
         <v>0.86458333333333404</v>
       </c>
       <c r="C29" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>87</v>
-      </c>
       <c r="E29" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I29" s="25">
         <v>0.85416666666666696</v>
@@ -3240,22 +3333,22 @@
         <v>0.875000000000001</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I30" s="25">
         <v>0.86458333333333404</v>
@@ -3272,22 +3365,22 @@
         <v>0.88541666666666696</v>
       </c>
       <c r="C31" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="E31" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>90</v>
-      </c>
       <c r="H31" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I31" s="25">
         <v>0.875000000000001</v>
@@ -3304,22 +3397,22 @@
         <v>0.89583333333333404</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I32" s="25">
         <v>0.88541666666666696</v>
@@ -3336,22 +3429,22 @@
         <v>0.906250000000001</v>
       </c>
       <c r="C33" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>91</v>
-      </c>
       <c r="E33" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I33" s="25">
         <v>0.89583333333333404</v>
@@ -3368,22 +3461,22 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I34" s="25">
         <v>0.906250000000001</v>
@@ -3399,14 +3492,14 @@
       <c r="B35" s="7">
         <v>0</v>
       </c>
-      <c r="C35" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
+      <c r="C35" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
       <c r="I35" s="7">
         <v>0.91666666666666663</v>
       </c>
@@ -3421,14 +3514,14 @@
       <c r="B36" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C36" s="42" t="s">
+      <c r="C36" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
       <c r="I36" s="7">
         <v>0</v>
       </c>
@@ -3469,19 +3562,19 @@
       <c r="H39" s="22"/>
     </row>
     <row r="40" spans="1:11" ht="15.75">
-      <c r="A40" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="31"/>
+      <c r="A40" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32"/>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="3"/>
@@ -3497,10 +3590,10 @@
       <c r="K41" s="3"/>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="34"/>
+      <c r="A42" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="33"/>
       <c r="C42" s="9" t="s">
         <v>8</v>
       </c>
@@ -3530,15 +3623,15 @@
       <c r="B43" s="8">
         <v>0.3611111111111111</v>
       </c>
-      <c r="C43" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="48"/>
+      <c r="C43" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="43"/>
       <c r="J43" s="8">
         <v>0.33333333333333331</v>
       </c>
@@ -3553,15 +3646,15 @@
       <c r="B44" s="8">
         <v>0.3888888888888889</v>
       </c>
-      <c r="C44" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
-      <c r="I44" s="48"/>
+      <c r="C44" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="43"/>
       <c r="J44" s="8">
         <v>0.3611111111111111</v>
       </c>
@@ -3577,25 +3670,25 @@
         <v>0.40277777777777773</v>
       </c>
       <c r="C45" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="D45" s="24" t="s">
+      <c r="E45" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="10" t="s">
-        <v>95</v>
-      </c>
       <c r="F45" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I45" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J45" s="8">
         <v>0.3888888888888889</v>
@@ -3612,25 +3705,25 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J46" s="8">
         <v>0.40277777777777801</v>
@@ -3647,25 +3740,25 @@
         <v>0.43055555555555602</v>
       </c>
       <c r="C47" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="D47" s="24" t="s">
-        <v>96</v>
-      </c>
       <c r="E47" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J47" s="8">
         <v>0.41666666666666702</v>
@@ -3682,19 +3775,19 @@
         <v>0.44444444444444497</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H48" s="11" t="s">
         <v>24</v>
@@ -3717,25 +3810,25 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="C49" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D49" s="24" t="s">
+      <c r="E49" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E49" s="10" t="s">
-        <v>90</v>
-      </c>
       <c r="F49" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J49" s="8">
         <v>0.44444444444444497</v>
@@ -3752,25 +3845,25 @@
         <v>0.47222222222222199</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H50" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I50" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J50" s="8">
         <v>0.45833333333333298</v>
@@ -3787,25 +3880,25 @@
         <v>0.48611111111111099</v>
       </c>
       <c r="C51" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="D51" s="24" t="s">
-        <v>91</v>
-      </c>
       <c r="E51" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J51" s="8">
         <v>0.47222222222222199</v>
@@ -3822,19 +3915,19 @@
         <v>0.5</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H52" s="11" t="s">
         <v>19</v>
@@ -3856,15 +3949,15 @@
       <c r="B53" s="8">
         <v>0.52777777777777779</v>
       </c>
-      <c r="C53" s="43" t="s">
+      <c r="C53" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="44"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="44"/>
-      <c r="H53" s="44"/>
-      <c r="I53" s="45"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="39"/>
+      <c r="I53" s="40"/>
       <c r="J53" s="8">
         <v>0.5</v>
       </c>
@@ -3880,25 +3973,25 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C54" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="D54" s="24" t="s">
+      <c r="E54" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="F54" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G54" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F54" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>100</v>
-      </c>
       <c r="H54" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J54" s="8">
         <v>0.52777777777777779</v>
@@ -3915,10 +4008,10 @@
         <v>0.55555555555555602</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E55" s="11" t="s">
         <v>19</v>
@@ -3927,13 +4020,13 @@
         <v>24</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J55" s="8">
         <v>0.54166666666666696</v>
@@ -3950,25 +4043,25 @@
         <v>0.56944444444444398</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D56" s="24" t="s">
         <v>19</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J56" s="8">
         <v>0.55555555555555602</v>
@@ -3988,22 +4081,22 @@
         <v>19</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G57" s="11" t="s">
         <v>24</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J57" s="8">
         <v>0.56944444444444398</v>
@@ -4020,25 +4113,25 @@
         <v>0.59722222222222199</v>
       </c>
       <c r="C58" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="D58" s="24" t="s">
+      <c r="E58" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E58" s="10" t="s">
-        <v>102</v>
-      </c>
       <c r="F58" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I58" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J58" s="8">
         <v>0.58333333333333304</v>
@@ -4055,10 +4148,10 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E59" s="11" t="s">
         <v>24</v>
@@ -4067,13 +4160,13 @@
         <v>19</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H59" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J59" s="8">
         <v>0.59722222222222199</v>
@@ -4090,25 +4183,25 @@
         <v>0.625</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D60" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J60" s="8">
         <v>0.61111111111111105</v>
@@ -4128,22 +4221,22 @@
         <v>24</v>
       </c>
       <c r="D61" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G61" s="11" t="s">
         <v>19</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I61" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J61" s="8">
         <v>0.625</v>
@@ -4159,15 +4252,15 @@
       <c r="B62" s="8">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C62" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="D62" s="47"/>
-      <c r="E62" s="47"/>
-      <c r="F62" s="47"/>
-      <c r="G62" s="47"/>
-      <c r="H62" s="47"/>
-      <c r="I62" s="48"/>
+      <c r="C62" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62" s="42"/>
+      <c r="E62" s="42"/>
+      <c r="F62" s="42"/>
+      <c r="G62" s="42"/>
+      <c r="H62" s="42"/>
+      <c r="I62" s="43"/>
       <c r="J62" s="8">
         <v>0.63888888888888895</v>
       </c>
@@ -4218,26 +4311,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
-      <c r="C1" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
+      <c r="C1" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="1">
@@ -4327,7 +4420,7 @@
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1">
@@ -4419,18 +4512,18 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" s="52"/>
+      <c r="D4" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="47"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -4443,13 +4536,13 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
-      <c r="X4" s="49" t="s">
+      <c r="X4" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y4" s="50"/>
-      <c r="Z4" s="51"/>
-      <c r="AA4" s="49"/>
-      <c r="AB4" s="51"/>
+      <c r="Y4" s="45"/>
+      <c r="Z4" s="46"/>
+      <c r="AA4" s="44"/>
+      <c r="AB4" s="46"/>
       <c r="AC4" s="2"/>
     </row>
     <row r="5" spans="1:30">
@@ -4461,34 +4554,34 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K5" s="52"/>
-      <c r="L5" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="51"/>
-      <c r="X5" s="49" t="s">
+      <c r="G5" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="45"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="47"/>
+      <c r="L5" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="45"/>
+      <c r="U5" s="45"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y5" s="50"/>
-      <c r="Z5" s="51"/>
+      <c r="Y5" s="45"/>
+      <c r="Z5" s="46"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
@@ -4505,10 +4598,10 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="52"/>
+      <c r="J6" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="47"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -4521,11 +4614,11 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
-      <c r="X6" s="49" t="s">
+      <c r="X6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y6" s="50"/>
-      <c r="Z6" s="51"/>
+      <c r="Y6" s="45"/>
+      <c r="Z6" s="46"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
@@ -4542,10 +4635,10 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="52"/>
+      <c r="J7" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="47"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -4558,11 +4651,11 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
-      <c r="X7" s="49" t="s">
+      <c r="X7" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y7" s="50"/>
-      <c r="Z7" s="51"/>
+      <c r="Y7" s="45"/>
+      <c r="Z7" s="46"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -4579,33 +4672,33 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="52"/>
-      <c r="L8" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="50"/>
-      <c r="U8" s="50"/>
-      <c r="V8" s="50"/>
-      <c r="W8" s="51"/>
-      <c r="X8" s="49" t="s">
+      <c r="J8" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="47"/>
+      <c r="L8" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="45"/>
+      <c r="U8" s="45"/>
+      <c r="V8" s="45"/>
+      <c r="W8" s="46"/>
+      <c r="X8" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y8" s="50"/>
-      <c r="Z8" s="51"/>
-      <c r="AA8" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB8" s="51"/>
+      <c r="Y8" s="45"/>
+      <c r="Z8" s="46"/>
+      <c r="AA8" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB8" s="46"/>
       <c r="AC8" s="2"/>
     </row>
     <row r="9" spans="1:30">
@@ -4617,15 +4710,15 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="H9" s="50"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K9" s="52"/>
+      <c r="G9" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="45"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="47"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -4638,15 +4731,15 @@
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
-      <c r="X9" s="49" t="s">
+      <c r="X9" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y9" s="50"/>
-      <c r="Z9" s="51"/>
-      <c r="AA9" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB9" s="51"/>
+      <c r="Y9" s="45"/>
+      <c r="Z9" s="46"/>
+      <c r="AA9" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB9" s="46"/>
       <c r="AC9" s="2"/>
     </row>
     <row r="10" spans="1:30">
@@ -4661,10 +4754,10 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" s="52"/>
+      <c r="J10" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10" s="47"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -4677,11 +4770,11 @@
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
-      <c r="X10" s="49" t="s">
+      <c r="X10" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y10" s="50"/>
-      <c r="Z10" s="51"/>
+      <c r="Y10" s="45"/>
+      <c r="Z10" s="46"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
@@ -4698,33 +4791,33 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52" t="s">
+      <c r="J11" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52" t="s">
-        <v>107</v>
-      </c>
-      <c r="O11" s="52"/>
-      <c r="P11" s="52" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q11" s="52"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q11" s="47"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
-      <c r="X11" s="49" t="s">
+      <c r="X11" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y11" s="50"/>
-      <c r="Z11" s="51"/>
+      <c r="Y11" s="45"/>
+      <c r="Z11" s="46"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
@@ -4741,31 +4834,31 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52"/>
+      <c r="J12" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
-      <c r="X12" s="49" t="s">
+      <c r="X12" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y12" s="50"/>
-      <c r="Z12" s="51"/>
-      <c r="AA12" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB12" s="51"/>
+      <c r="Y12" s="45"/>
+      <c r="Z12" s="46"/>
+      <c r="AA12" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB12" s="46"/>
       <c r="AC12" s="2"/>
     </row>
     <row r="13" spans="1:30">
@@ -4777,15 +4870,15 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="H13" s="50"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K13" s="52"/>
+      <c r="G13" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="45"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K13" s="47"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -4798,15 +4891,15 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-      <c r="X13" s="49" t="s">
+      <c r="X13" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y13" s="50"/>
-      <c r="Z13" s="51"/>
-      <c r="AA13" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB13" s="51"/>
+      <c r="Y13" s="45"/>
+      <c r="Z13" s="46"/>
+      <c r="AA13" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB13" s="46"/>
       <c r="AC13" s="2"/>
     </row>
     <row r="14" spans="1:30">
@@ -4821,33 +4914,33 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52" t="s">
+      <c r="J14" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52" t="s">
-        <v>107</v>
-      </c>
-      <c r="O14" s="52"/>
-      <c r="P14" s="52" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q14" s="52"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q14" s="47"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
-      <c r="X14" s="49" t="s">
+      <c r="X14" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y14" s="50"/>
-      <c r="Z14" s="51"/>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="46"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
@@ -4858,18 +4951,18 @@
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K15" s="52"/>
+      <c r="D15" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="47"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -4882,11 +4975,11 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
-      <c r="X15" s="49" t="s">
+      <c r="X15" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y15" s="50"/>
-      <c r="Z15" s="51"/>
+      <c r="Y15" s="45"/>
+      <c r="Z15" s="46"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
@@ -4903,10 +4996,10 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K16" s="52"/>
+      <c r="J16" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16" s="47"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -4919,11 +5012,11 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
-      <c r="X16" s="49" t="s">
+      <c r="X16" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y16" s="50"/>
-      <c r="Z16" s="51"/>
+      <c r="Y16" s="45"/>
+      <c r="Z16" s="46"/>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
@@ -4940,10 +5033,10 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K17" s="52"/>
+      <c r="J17" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17" s="47"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -4956,11 +5049,11 @@
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
-      <c r="X17" s="49" t="s">
+      <c r="X17" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y17" s="50"/>
-      <c r="Z17" s="51"/>
+      <c r="Y17" s="45"/>
+      <c r="Z17" s="46"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
@@ -4977,15 +5070,15 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K18" s="52"/>
-      <c r="L18" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="M18" s="50"/>
-      <c r="N18" s="51"/>
+      <c r="J18" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="47"/>
+      <c r="L18" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="M18" s="45"/>
+      <c r="N18" s="46"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -4995,15 +5088,15 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
-      <c r="X18" s="49" t="s">
+      <c r="X18" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y18" s="50"/>
-      <c r="Z18" s="51"/>
-      <c r="AA18" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB18" s="51"/>
+      <c r="Y18" s="45"/>
+      <c r="Z18" s="46"/>
+      <c r="AA18" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB18" s="46"/>
       <c r="AC18" s="2"/>
     </row>
     <row r="19" spans="1:29">
@@ -5018,10 +5111,10 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K19" s="52"/>
+      <c r="J19" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K19" s="47"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -5034,15 +5127,15 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
-      <c r="X19" s="49" t="s">
+      <c r="X19" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y19" s="50"/>
-      <c r="Z19" s="51"/>
-      <c r="AA19" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB19" s="51"/>
+      <c r="Y19" s="45"/>
+      <c r="Z19" s="46"/>
+      <c r="AA19" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB19" s="46"/>
       <c r="AC19" s="2"/>
     </row>
     <row r="20" spans="1:29">
@@ -5057,10 +5150,10 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K20" s="52"/>
+      <c r="J20" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K20" s="47"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -5073,11 +5166,11 @@
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
-      <c r="X20" s="49" t="s">
+      <c r="X20" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y20" s="50"/>
-      <c r="Z20" s="51"/>
+      <c r="Y20" s="45"/>
+      <c r="Z20" s="46"/>
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
@@ -5094,10 +5187,10 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K21" s="52"/>
+      <c r="J21" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K21" s="47"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -5110,11 +5203,11 @@
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
-      <c r="X21" s="49" t="s">
+      <c r="X21" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y21" s="50"/>
-      <c r="Z21" s="51"/>
+      <c r="Y21" s="45"/>
+      <c r="Z21" s="46"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
@@ -5131,10 +5224,10 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K22" s="52"/>
+      <c r="J22" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K22" s="47"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -5147,11 +5240,11 @@
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
-      <c r="X22" s="49" t="s">
+      <c r="X22" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y22" s="50"/>
-      <c r="Z22" s="51"/>
+      <c r="Y22" s="45"/>
+      <c r="Z22" s="46"/>
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
@@ -5168,10 +5261,10 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K23" s="52"/>
+      <c r="J23" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K23" s="47"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -5184,11 +5277,11 @@
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
-      <c r="X23" s="49" t="s">
+      <c r="X23" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y23" s="50"/>
-      <c r="Z23" s="51"/>
+      <c r="Y23" s="45"/>
+      <c r="Z23" s="46"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
@@ -5205,10 +5298,10 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K24" s="52"/>
+      <c r="J24" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K24" s="47"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -5221,11 +5314,11 @@
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
-      <c r="X24" s="49" t="s">
+      <c r="X24" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y24" s="50"/>
-      <c r="Z24" s="51"/>
+      <c r="Y24" s="45"/>
+      <c r="Z24" s="46"/>
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
@@ -5242,10 +5335,10 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K25" s="52"/>
+      <c r="J25" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K25" s="47"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -5258,11 +5351,11 @@
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
-      <c r="X25" s="49" t="s">
+      <c r="X25" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y25" s="50"/>
-      <c r="Z25" s="51"/>
+      <c r="Y25" s="45"/>
+      <c r="Z25" s="46"/>
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
@@ -5279,10 +5372,10 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K26" s="52"/>
+      <c r="J26" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K26" s="47"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -5295,11 +5388,11 @@
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
-      <c r="X26" s="49" t="s">
+      <c r="X26" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y26" s="50"/>
-      <c r="Z26" s="51"/>
+      <c r="Y26" s="45"/>
+      <c r="Z26" s="46"/>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
@@ -5316,10 +5409,10 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K27" s="52"/>
+      <c r="J27" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K27" s="47"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -5332,11 +5425,11 @@
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
-      <c r="X27" s="49" t="s">
+      <c r="X27" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y27" s="50"/>
-      <c r="Z27" s="51"/>
+      <c r="Y27" s="45"/>
+      <c r="Z27" s="46"/>
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
@@ -5353,10 +5446,10 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K28" s="52"/>
+      <c r="J28" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K28" s="47"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -5369,11 +5462,11 @@
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
-      <c r="X28" s="49" t="s">
+      <c r="X28" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y28" s="50"/>
-      <c r="Z28" s="51"/>
+      <c r="Y28" s="45"/>
+      <c r="Z28" s="46"/>
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
@@ -5390,10 +5483,10 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K29" s="52"/>
+      <c r="J29" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K29" s="47"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -5406,11 +5499,11 @@
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
-      <c r="X29" s="49" t="s">
+      <c r="X29" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y29" s="50"/>
-      <c r="Z29" s="51"/>
+      <c r="Y29" s="45"/>
+      <c r="Z29" s="46"/>
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
@@ -5427,10 +5520,10 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K30" s="52"/>
+      <c r="J30" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K30" s="47"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -5443,11 +5536,11 @@
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
-      <c r="X30" s="49" t="s">
+      <c r="X30" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y30" s="50"/>
-      <c r="Z30" s="51"/>
+      <c r="Y30" s="45"/>
+      <c r="Z30" s="46"/>
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
@@ -5464,10 +5557,10 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K31" s="52"/>
+      <c r="J31" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K31" s="47"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -5480,11 +5573,11 @@
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
-      <c r="X31" s="49" t="s">
+      <c r="X31" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y31" s="50"/>
-      <c r="Z31" s="51"/>
+      <c r="Y31" s="45"/>
+      <c r="Z31" s="46"/>
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
@@ -5501,10 +5594,10 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K32" s="52"/>
+      <c r="J32" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K32" s="47"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5517,11 +5610,11 @@
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
-      <c r="X32" s="49" t="s">
+      <c r="X32" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y32" s="50"/>
-      <c r="Z32" s="51"/>
+      <c r="Y32" s="45"/>
+      <c r="Z32" s="46"/>
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
@@ -5538,10 +5631,10 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K33" s="52"/>
+      <c r="J33" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K33" s="47"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5554,11 +5647,11 @@
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
-      <c r="X33" s="49" t="s">
+      <c r="X33" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y33" s="50"/>
-      <c r="Z33" s="51"/>
+      <c r="Y33" s="45"/>
+      <c r="Z33" s="46"/>
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
@@ -5575,10 +5668,10 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K34" s="52"/>
+      <c r="J34" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K34" s="47"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5591,11 +5684,11 @@
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
-      <c r="X34" s="49" t="s">
+      <c r="X34" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y34" s="50"/>
-      <c r="Z34" s="51"/>
+      <c r="Y34" s="45"/>
+      <c r="Z34" s="46"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
@@ -5612,10 +5705,10 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K35" s="52"/>
+      <c r="J35" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K35" s="47"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5628,11 +5721,11 @@
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
-      <c r="X35" s="49" t="s">
+      <c r="X35" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y35" s="50"/>
-      <c r="Z35" s="51"/>
+      <c r="Y35" s="45"/>
+      <c r="Z35" s="46"/>
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
       <c r="AC35" s="2"/>
@@ -5649,10 +5742,10 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K36" s="52"/>
+      <c r="J36" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K36" s="47"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5665,11 +5758,11 @@
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
       <c r="W36" s="2"/>
-      <c r="X36" s="49" t="s">
+      <c r="X36" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y36" s="50"/>
-      <c r="Z36" s="51"/>
+      <c r="Y36" s="45"/>
+      <c r="Z36" s="46"/>
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
       <c r="AC36" s="2"/>
@@ -5686,10 +5779,10 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="K37" s="52"/>
+      <c r="J37" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K37" s="47"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5702,11 +5795,11 @@
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
       <c r="W37" s="2"/>
-      <c r="X37" s="49" t="s">
+      <c r="X37" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="Y37" s="50"/>
-      <c r="Z37" s="51"/>
+      <c r="Y37" s="45"/>
+      <c r="Z37" s="46"/>
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
       <c r="AC37" s="2"/>

</xml_diff>

<commit_message>
Added pictures for all activities, which also show in the program Also fixed an error in the schedule, due to the post-processing
</commit_message>
<xml_diff>
--- a/BarcodeScanner/planning kinderen en leiding.xlsx
+++ b/BarcodeScanner/planning kinderen en leiding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="-150" windowWidth="19320" windowHeight="12120"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="9480" windowHeight="7920"/>
   </bookViews>
   <sheets>
     <sheet name="Kleine speltakken" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="115">
   <si>
     <t>Avondeten</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>25+26+27+28+29+30</t>
+  </si>
+  <si>
+    <t>19 + 20 + 21 + 22 + 23 + 24</t>
   </si>
 </sst>
 </file>
@@ -399,12 +402,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="12">
@@ -550,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -637,22 +646,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -686,9 +704,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -992,8 +1007,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C5" sqref="C5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1009,19 +1025,19 @@
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="12.75"/>
     <row r="2" spans="1:11" s="4" customFormat="1" ht="15.75">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
     </row>
     <row r="3" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A3" s="3"/>
@@ -1035,8 +1051,8 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="27" t="s">
         <v>8</v>
       </c>
@@ -1066,15 +1082,15 @@
       <c r="B5" s="29">
         <v>40831.416666666664</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="40"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="43"/>
       <c r="J5" s="6">
         <v>0.39583333333333331</v>
       </c>
@@ -1098,13 +1114,13 @@
       <c r="E6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="33" t="s">
         <v>33</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="33" t="s">
         <v>40</v>
       </c>
       <c r="I6" s="31" t="s">
@@ -1133,13 +1149,13 @@
       <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="33" t="s">
         <v>33</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="33" t="s">
         <v>40</v>
       </c>
       <c r="I7" s="31" t="s">
@@ -1168,13 +1184,13 @@
       <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="33" t="s">
         <v>33</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="33" t="s">
         <v>40</v>
       </c>
       <c r="I8" s="31" t="s">
@@ -1206,7 +1222,7 @@
       <c r="F9" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="33" t="s">
         <v>40</v>
       </c>
       <c r="H9" s="31" t="s">
@@ -1241,7 +1257,7 @@
       <c r="F10" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="33" t="s">
         <v>40</v>
       </c>
       <c r="H10" s="31" t="s">
@@ -1276,7 +1292,7 @@
       <c r="F11" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="33" t="s">
         <v>40</v>
       </c>
       <c r="H11" s="31" t="s">
@@ -1299,15 +1315,15 @@
       <c r="B12" s="30">
         <v>40831.527777777781</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="6">
         <v>0.5</v>
       </c>
@@ -1331,13 +1347,13 @@
       <c r="E13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="33" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="H13" s="33" t="s">
         <v>42</v>
       </c>
       <c r="I13" s="31" t="s">
@@ -1366,13 +1382,13 @@
       <c r="E14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="33" t="s">
         <v>35</v>
       </c>
       <c r="G14" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="33" t="s">
         <v>42</v>
       </c>
       <c r="I14" s="31" t="s">
@@ -1401,13 +1417,13 @@
       <c r="E15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="33" t="s">
         <v>35</v>
       </c>
       <c r="G15" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="33" t="s">
         <v>42</v>
       </c>
       <c r="I15" s="31" t="s">
@@ -1439,11 +1455,11 @@
       <c r="F16" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="33" t="s">
         <v>42</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I16" s="31" t="s">
         <v>45</v>
@@ -1474,11 +1490,11 @@
       <c r="F17" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="33" t="s">
         <v>42</v>
       </c>
       <c r="H17" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I17" s="31" t="s">
         <v>45</v>
@@ -1509,11 +1525,11 @@
       <c r="F18" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="33" t="s">
         <v>42</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I18" s="31" t="s">
         <v>45</v>
@@ -1541,14 +1557,14 @@
       <c r="E19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="33" t="s">
         <v>37</v>
       </c>
       <c r="G19" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="31" t="s">
-        <v>43</v>
+      <c r="H19" s="33" t="s">
+        <v>114</v>
       </c>
       <c r="I19" s="31" t="s">
         <v>46</v>
@@ -1576,14 +1592,14 @@
       <c r="E20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="33" t="s">
         <v>37</v>
       </c>
       <c r="G20" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="31" t="s">
-        <v>43</v>
+      <c r="H20" s="33" t="s">
+        <v>114</v>
       </c>
       <c r="I20" s="31" t="s">
         <v>46</v>
@@ -1611,14 +1627,14 @@
       <c r="E21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="33" t="s">
         <v>37</v>
       </c>
       <c r="G21" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="31" t="s">
-        <v>43</v>
+      <c r="H21" s="33" t="s">
+        <v>114</v>
       </c>
       <c r="I21" s="31" t="s">
         <v>46</v>
@@ -1646,14 +1662,14 @@
       <c r="E22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="31" t="s">
-        <v>38</v>
+      <c r="G22" s="33" t="s">
+        <v>114</v>
       </c>
       <c r="H22" s="31" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="I22" s="31" t="s">
         <v>46</v>
@@ -1681,14 +1697,14 @@
       <c r="E23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="31" t="s">
-        <v>38</v>
+      <c r="G23" s="33" t="s">
+        <v>114</v>
       </c>
       <c r="H23" s="31" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="I23" s="31" t="s">
         <v>46</v>
@@ -1716,14 +1732,14 @@
       <c r="E24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="31" t="s">
+      <c r="F24" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="G24" s="31" t="s">
-        <v>113</v>
+      <c r="G24" s="33" t="s">
+        <v>114</v>
       </c>
       <c r="H24" s="31" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="I24" s="31" t="s">
         <v>46</v>
@@ -1742,15 +1758,15 @@
       <c r="B25" s="30">
         <v>40831.736111111109</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
       <c r="J25" s="6">
         <v>0.69444444444444497</v>
       </c>
@@ -1765,15 +1781,15 @@
       <c r="B26" s="30">
         <v>40831.770833333336</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
       <c r="J26" s="6">
         <v>0.73611111111111205</v>
       </c>
@@ -1788,15 +1804,15 @@
       <c r="B27" s="30">
         <v>40831.791666666664</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
       <c r="J27" s="6">
         <v>0.77083333333333337</v>
       </c>
@@ -1811,15 +1827,15 @@
       <c r="B28" s="30">
         <v>40831.916666666664</v>
       </c>
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
       <c r="J28" s="6">
         <v>0.79166666666666663</v>
       </c>
@@ -1834,15 +1850,15 @@
       <c r="B29" s="30">
         <v>40831.9375</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
       <c r="J29" s="6">
         <v>0.91666666666666663</v>
       </c>
@@ -1857,15 +1873,15 @@
       <c r="B30" s="30">
         <v>40831.291666666664</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
       <c r="J30" s="6">
         <v>0.9375</v>
       </c>
@@ -1898,23 +1914,23 @@
       <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:11" s="4" customFormat="1" ht="15.75">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
     </row>
     <row r="34" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A34" s="33"/>
-      <c r="B34" s="33"/>
+      <c r="A34" s="38"/>
+      <c r="B34" s="38"/>
       <c r="C34" s="9" t="s">
         <v>9</v>
       </c>
@@ -1935,20 +1951,20 @@
       </c>
     </row>
     <row r="35" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A35" s="49">
+      <c r="A35" s="32">
         <v>40832.291666666664</v>
       </c>
-      <c r="B35" s="49">
+      <c r="B35" s="32">
         <v>40832.333333333336</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
       <c r="I35" s="8">
         <v>0.29166666666666669</v>
       </c>
@@ -1957,20 +1973,20 @@
       </c>
     </row>
     <row r="36" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A36" s="49">
+      <c r="A36" s="32">
         <v>40832.333333333336</v>
       </c>
-      <c r="B36" s="49">
+      <c r="B36" s="32">
         <v>40832.361111111109</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
       <c r="I36" s="8">
         <v>0.33333333333333331</v>
       </c>
@@ -1979,20 +1995,20 @@
       </c>
     </row>
     <row r="37" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A37" s="49">
+      <c r="A37" s="32">
         <v>40832.361111111109</v>
       </c>
-      <c r="B37" s="49">
+      <c r="B37" s="32">
         <v>40832.402777777781</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C37" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
       <c r="I37" s="8">
         <v>0.3611111111111111</v>
       </c>
@@ -2001,10 +2017,10 @@
       </c>
     </row>
     <row r="38" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A38" s="49">
+      <c r="A38" s="32">
         <v>40832.402777777781</v>
       </c>
-      <c r="B38" s="49">
+      <c r="B38" s="32">
         <v>40832.416666666664</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -2013,13 +2029,13 @@
       <c r="D38" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="33" t="s">
         <v>67</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="G38" s="31" t="s">
+      <c r="G38" s="33" t="s">
         <v>70</v>
       </c>
       <c r="H38" s="31" t="s">
@@ -2033,10 +2049,10 @@
       </c>
     </row>
     <row r="39" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A39" s="49">
+      <c r="A39" s="32">
         <v>40832.416666666664</v>
       </c>
-      <c r="B39" s="49">
+      <c r="B39" s="32">
         <v>40832.430555555555</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -2045,13 +2061,13 @@
       <c r="D39" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="31" t="s">
+      <c r="E39" s="33" t="s">
         <v>67</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="G39" s="31" t="s">
+      <c r="G39" s="33" t="s">
         <v>70</v>
       </c>
       <c r="H39" s="31" t="s">
@@ -2065,10 +2081,10 @@
       </c>
     </row>
     <row r="40" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A40" s="49">
+      <c r="A40" s="32">
         <v>40832.430555555555</v>
       </c>
-      <c r="B40" s="49">
+      <c r="B40" s="32">
         <v>40832.444444444445</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -2080,13 +2096,13 @@
       <c r="E40" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="31" t="s">
+      <c r="F40" s="33" t="s">
         <v>69</v>
       </c>
       <c r="G40" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="H40" s="31" t="s">
+      <c r="H40" s="33" t="s">
         <v>73</v>
       </c>
       <c r="I40" s="8">
@@ -2097,10 +2113,10 @@
       </c>
     </row>
     <row r="41" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A41" s="49">
+      <c r="A41" s="32">
         <v>40832.444444444445</v>
       </c>
-      <c r="B41" s="49">
+      <c r="B41" s="32">
         <v>40832.458333333336</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -2112,13 +2128,13 @@
       <c r="E41" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="F41" s="31" t="s">
+      <c r="F41" s="33" t="s">
         <v>69</v>
       </c>
       <c r="G41" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="H41" s="31" t="s">
+      <c r="H41" s="33" t="s">
         <v>73</v>
       </c>
       <c r="I41" s="8">
@@ -2129,10 +2145,10 @@
       </c>
     </row>
     <row r="42" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A42" s="49">
+      <c r="A42" s="32">
         <v>40832.458333333336</v>
       </c>
-      <c r="B42" s="49">
+      <c r="B42" s="32">
         <v>40832.472222222219</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -2141,13 +2157,13 @@
       <c r="D42" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="33" t="s">
         <v>69</v>
       </c>
       <c r="F42" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="G42" s="31" t="s">
+      <c r="G42" s="33" t="s">
         <v>72</v>
       </c>
       <c r="H42" s="31" t="s">
@@ -2161,10 +2177,10 @@
       </c>
     </row>
     <row r="43" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A43" s="49">
+      <c r="A43" s="32">
         <v>40832.472222222219</v>
       </c>
-      <c r="B43" s="49">
+      <c r="B43" s="32">
         <v>40832.486111111109</v>
       </c>
       <c r="C43" s="5" t="s">
@@ -2173,13 +2189,13 @@
       <c r="D43" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="31" t="s">
+      <c r="E43" s="33" t="s">
         <v>69</v>
       </c>
       <c r="F43" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="G43" s="31" t="s">
+      <c r="G43" s="33" t="s">
         <v>72</v>
       </c>
       <c r="H43" s="31" t="s">
@@ -2193,10 +2209,10 @@
       </c>
     </row>
     <row r="44" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A44" s="49">
+      <c r="A44" s="32">
         <v>40832.486111111109</v>
       </c>
-      <c r="B44" s="49">
+      <c r="B44" s="32">
         <v>40832.5</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -2208,13 +2224,13 @@
       <c r="E44" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="F44" s="31" t="s">
+      <c r="F44" s="33" t="s">
         <v>71</v>
       </c>
       <c r="G44" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="H44" s="31" t="s">
+      <c r="H44" s="33" t="s">
         <v>74</v>
       </c>
       <c r="I44" s="8">
@@ -2225,10 +2241,10 @@
       </c>
     </row>
     <row r="45" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A45" s="49">
+      <c r="A45" s="32">
         <v>40832.5</v>
       </c>
-      <c r="B45" s="49">
+      <c r="B45" s="32">
         <v>40832.513888888891</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -2240,13 +2256,13 @@
       <c r="E45" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="F45" s="31" t="s">
+      <c r="F45" s="33" t="s">
         <v>71</v>
       </c>
       <c r="G45" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="H45" s="31" t="s">
+      <c r="H45" s="33" t="s">
         <v>74</v>
       </c>
       <c r="I45" s="8">
@@ -2257,20 +2273,20 @@
       </c>
     </row>
     <row r="46" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A46" s="49">
+      <c r="A46" s="32">
         <v>40832.513888888891</v>
       </c>
-      <c r="B46" s="49">
+      <c r="B46" s="32">
         <v>40832.541666666664</v>
       </c>
-      <c r="C46" s="37" t="s">
+      <c r="C46" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="37"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
       <c r="I46" s="8">
         <v>0.51388888888888895</v>
       </c>
@@ -2279,10 +2295,10 @@
       </c>
     </row>
     <row r="47" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A47" s="49">
+      <c r="A47" s="32">
         <v>40832.541666666664</v>
       </c>
-      <c r="B47" s="49">
+      <c r="B47" s="32">
         <v>40832.555555555555</v>
       </c>
       <c r="C47" s="5" t="s">
@@ -2291,13 +2307,13 @@
       <c r="D47" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E47" s="31" t="s">
+      <c r="E47" s="33" t="s">
         <v>71</v>
       </c>
       <c r="F47" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="G47" s="31" t="s">
+      <c r="G47" s="33" t="s">
         <v>68</v>
       </c>
       <c r="H47" s="31" t="s">
@@ -2311,10 +2327,10 @@
       </c>
     </row>
     <row r="48" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A48" s="49">
+      <c r="A48" s="32">
         <v>40832.555555555555</v>
       </c>
-      <c r="B48" s="49">
+      <c r="B48" s="32">
         <v>40832.569444444445</v>
       </c>
       <c r="C48" s="5" t="s">
@@ -2323,13 +2339,13 @@
       <c r="D48" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E48" s="31" t="s">
+      <c r="E48" s="33" t="s">
         <v>71</v>
       </c>
       <c r="F48" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="G48" s="31" t="s">
+      <c r="G48" s="33" t="s">
         <v>68</v>
       </c>
       <c r="H48" s="31" t="s">
@@ -2343,10 +2359,10 @@
       </c>
     </row>
     <row r="49" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A49" s="49">
+      <c r="A49" s="32">
         <v>40832.569444444445</v>
       </c>
-      <c r="B49" s="49">
+      <c r="B49" s="32">
         <v>40832.583333333336</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -2358,13 +2374,13 @@
       <c r="E49" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="F49" s="31" t="s">
+      <c r="F49" s="33" t="s">
         <v>67</v>
       </c>
       <c r="G49" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="H49" s="31" t="s">
+      <c r="H49" s="33" t="s">
         <v>75</v>
       </c>
       <c r="I49" s="8">
@@ -2375,10 +2391,10 @@
       </c>
     </row>
     <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A50" s="49">
+      <c r="A50" s="32">
         <v>40832.583333333336</v>
       </c>
-      <c r="B50" s="49">
+      <c r="B50" s="32">
         <v>40832.597222222219</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -2390,13 +2406,13 @@
       <c r="E50" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="F50" s="31" t="s">
+      <c r="F50" s="33" t="s">
         <v>67</v>
       </c>
       <c r="G50" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="H50" s="31" t="s">
+      <c r="H50" s="33" t="s">
         <v>75</v>
       </c>
       <c r="I50" s="8">
@@ -2407,20 +2423,20 @@
       </c>
     </row>
     <row r="51" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A51" s="49">
+      <c r="A51" s="32">
         <v>40832.597222222219</v>
       </c>
-      <c r="B51" s="49">
+      <c r="B51" s="32">
         <v>40832.638888888891</v>
       </c>
-      <c r="C51" s="34" t="s">
+      <c r="C51" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="34"/>
-      <c r="H51" s="34"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
       <c r="I51" s="8">
         <v>0.59722222222222199</v>
       </c>
@@ -2429,20 +2445,20 @@
       </c>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A52" s="49">
+      <c r="A52" s="32">
         <v>40832.638888888891</v>
       </c>
-      <c r="B52" s="49">
+      <c r="B52" s="32">
         <v>40832.645833333336</v>
       </c>
-      <c r="C52" s="34" t="s">
+      <c r="C52" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
-      <c r="H52" s="34"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
       <c r="I52" s="8">
         <v>0.63888888888888895</v>
       </c>
@@ -2455,12 +2471,6 @@
     <row r="55" spans="1:10" s="4" customFormat="1" ht="12.75"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="C25:I25"/>
     <mergeCell ref="C26:I26"/>
     <mergeCell ref="C27:I27"/>
     <mergeCell ref="C51:H51"/>
@@ -2473,6 +2483,12 @@
     <mergeCell ref="C37:H37"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A33:K33"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="C25:I25"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2501,25 +2517,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="36"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
@@ -2546,14 +2562,14 @@
       <c r="B3" s="6">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
       <c r="I3" s="7">
         <v>0.39583333333333331</v>
       </c>
@@ -2568,14 +2584,14 @@
       <c r="B4" s="7">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
       <c r="I4" s="7">
         <v>0.41666666666666669</v>
       </c>
@@ -2590,14 +2606,14 @@
       <c r="B5" s="7">
         <v>0.5</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
       <c r="I5" s="7">
         <v>0.45833333333333331</v>
       </c>
@@ -2740,14 +2756,14 @@
       <c r="B10" s="7">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
       <c r="I10" s="7">
         <v>0.55555555555555558</v>
       </c>
@@ -3018,14 +3034,14 @@
       <c r="B19" s="7">
         <v>0.73611111111111116</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
       <c r="I19" s="7">
         <v>0.69444444444444497</v>
       </c>
@@ -3040,14 +3056,14 @@
       <c r="B20" s="7">
         <v>0.77083333333333337</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="40"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="43"/>
       <c r="I20" s="7">
         <v>0.73611111111111205</v>
       </c>
@@ -3062,14 +3078,14 @@
       <c r="B21" s="16">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
       <c r="I21" s="16">
         <v>0.77083333333333337</v>
       </c>
@@ -3492,14 +3508,14 @@
       <c r="B35" s="7">
         <v>0</v>
       </c>
-      <c r="C35" s="37" t="s">
+      <c r="C35" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="36"/>
       <c r="I35" s="7">
         <v>0.91666666666666663</v>
       </c>
@@ -3514,14 +3530,14 @@
       <c r="B36" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C36" s="37" t="s">
+      <c r="C36" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
       <c r="I36" s="7">
         <v>0</v>
       </c>
@@ -3562,19 +3578,19 @@
       <c r="H39" s="22"/>
     </row>
     <row r="40" spans="1:11" ht="15.75">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="37"/>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="3"/>
@@ -3590,10 +3606,10 @@
       <c r="K41" s="3"/>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="33" t="s">
+      <c r="A42" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="33"/>
+      <c r="B42" s="38"/>
       <c r="C42" s="9" t="s">
         <v>8</v>
       </c>
@@ -3623,15 +3639,15 @@
       <c r="B43" s="8">
         <v>0.3611111111111111</v>
       </c>
-      <c r="C43" s="41" t="s">
+      <c r="C43" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="43"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="46"/>
       <c r="J43" s="8">
         <v>0.33333333333333331</v>
       </c>
@@ -3646,15 +3662,15 @@
       <c r="B44" s="8">
         <v>0.3888888888888889</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="43"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="46"/>
       <c r="J44" s="8">
         <v>0.3611111111111111</v>
       </c>
@@ -3949,15 +3965,15 @@
       <c r="B53" s="8">
         <v>0.52777777777777779</v>
       </c>
-      <c r="C53" s="38" t="s">
+      <c r="C53" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="40"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="42"/>
+      <c r="H53" s="42"/>
+      <c r="I53" s="43"/>
       <c r="J53" s="8">
         <v>0.5</v>
       </c>
@@ -4252,15 +4268,15 @@
       <c r="B62" s="8">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C62" s="41" t="s">
+      <c r="C62" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="D62" s="42"/>
-      <c r="E62" s="42"/>
-      <c r="F62" s="42"/>
-      <c r="G62" s="42"/>
-      <c r="H62" s="42"/>
-      <c r="I62" s="43"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="45"/>
+      <c r="I62" s="46"/>
       <c r="J62" s="8">
         <v>0.63888888888888895</v>
       </c>
@@ -4311,22 +4327,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="2" t="s">
@@ -4512,18 +4528,18 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="47" t="s">
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="47"/>
+      <c r="K4" s="50"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -4536,13 +4552,13 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
-      <c r="X4" s="44" t="s">
+      <c r="X4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y4" s="45"/>
-      <c r="Z4" s="46"/>
-      <c r="AA4" s="44"/>
-      <c r="AB4" s="46"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="49"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="49"/>
       <c r="AC4" s="2"/>
     </row>
     <row r="5" spans="1:30">
@@ -4554,34 +4570,34 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="44" t="s">
+      <c r="G5" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="H5" s="45"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="47" t="s">
+      <c r="H5" s="48"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K5" s="47"/>
-      <c r="L5" s="44" t="s">
+      <c r="K5" s="50"/>
+      <c r="L5" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="46"/>
-      <c r="X5" s="44" t="s">
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="49"/>
+      <c r="X5" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y5" s="45"/>
-      <c r="Z5" s="46"/>
+      <c r="Y5" s="48"/>
+      <c r="Z5" s="49"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
@@ -4598,10 +4614,10 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="47" t="s">
+      <c r="J6" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="47"/>
+      <c r="K6" s="50"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -4614,11 +4630,11 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
-      <c r="X6" s="44" t="s">
+      <c r="X6" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y6" s="45"/>
-      <c r="Z6" s="46"/>
+      <c r="Y6" s="48"/>
+      <c r="Z6" s="49"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
@@ -4635,10 +4651,10 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="47" t="s">
+      <c r="J7" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="47"/>
+      <c r="K7" s="50"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -4651,11 +4667,11 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
-      <c r="X7" s="44" t="s">
+      <c r="X7" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y7" s="45"/>
-      <c r="Z7" s="46"/>
+      <c r="Y7" s="48"/>
+      <c r="Z7" s="49"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -4672,33 +4688,33 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="47"/>
-      <c r="L8" s="44" t="s">
+      <c r="K8" s="50"/>
+      <c r="L8" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="45"/>
-      <c r="W8" s="46"/>
-      <c r="X8" s="44" t="s">
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="49"/>
+      <c r="X8" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y8" s="45"/>
-      <c r="Z8" s="46"/>
-      <c r="AA8" s="44" t="s">
+      <c r="Y8" s="48"/>
+      <c r="Z8" s="49"/>
+      <c r="AA8" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="AB8" s="46"/>
+      <c r="AB8" s="49"/>
       <c r="AC8" s="2"/>
     </row>
     <row r="9" spans="1:30">
@@ -4710,15 +4726,15 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="44" t="s">
+      <c r="G9" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="H9" s="45"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="47" t="s">
+      <c r="H9" s="48"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K9" s="47"/>
+      <c r="K9" s="50"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -4731,15 +4747,15 @@
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
-      <c r="X9" s="44" t="s">
+      <c r="X9" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y9" s="45"/>
-      <c r="Z9" s="46"/>
-      <c r="AA9" s="44" t="s">
+      <c r="Y9" s="48"/>
+      <c r="Z9" s="49"/>
+      <c r="AA9" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="AB9" s="46"/>
+      <c r="AB9" s="49"/>
       <c r="AC9" s="2"/>
     </row>
     <row r="10" spans="1:30">
@@ -4754,10 +4770,10 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="47" t="s">
+      <c r="J10" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K10" s="47"/>
+      <c r="K10" s="50"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -4770,11 +4786,11 @@
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
-      <c r="X10" s="44" t="s">
+      <c r="X10" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y10" s="45"/>
-      <c r="Z10" s="46"/>
+      <c r="Y10" s="48"/>
+      <c r="Z10" s="49"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
@@ -4791,33 +4807,33 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="47" t="s">
+      <c r="J11" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47" t="s">
+      <c r="K11" s="50"/>
+      <c r="L11" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47" t="s">
+      <c r="M11" s="50"/>
+      <c r="N11" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="O11" s="47"/>
-      <c r="P11" s="47" t="s">
+      <c r="O11" s="50"/>
+      <c r="P11" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="Q11" s="47"/>
+      <c r="Q11" s="50"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
-      <c r="X11" s="44" t="s">
+      <c r="X11" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y11" s="45"/>
-      <c r="Z11" s="46"/>
+      <c r="Y11" s="48"/>
+      <c r="Z11" s="49"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
@@ -4834,31 +4850,31 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="47" t="s">
+      <c r="J12" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="47"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
-      <c r="X12" s="44" t="s">
+      <c r="X12" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y12" s="45"/>
-      <c r="Z12" s="46"/>
-      <c r="AA12" s="44" t="s">
+      <c r="Y12" s="48"/>
+      <c r="Z12" s="49"/>
+      <c r="AA12" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="AB12" s="46"/>
+      <c r="AB12" s="49"/>
       <c r="AC12" s="2"/>
     </row>
     <row r="13" spans="1:30">
@@ -4870,15 +4886,15 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="44" t="s">
+      <c r="G13" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="H13" s="45"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="47" t="s">
+      <c r="H13" s="48"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="47"/>
+      <c r="K13" s="50"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -4891,15 +4907,15 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-      <c r="X13" s="44" t="s">
+      <c r="X13" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y13" s="45"/>
-      <c r="Z13" s="46"/>
-      <c r="AA13" s="44" t="s">
+      <c r="Y13" s="48"/>
+      <c r="Z13" s="49"/>
+      <c r="AA13" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="AB13" s="46"/>
+      <c r="AB13" s="49"/>
       <c r="AC13" s="2"/>
     </row>
     <row r="14" spans="1:30">
@@ -4914,33 +4930,33 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47" t="s">
+      <c r="K14" s="50"/>
+      <c r="L14" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47" t="s">
+      <c r="M14" s="50"/>
+      <c r="N14" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47" t="s">
+      <c r="O14" s="50"/>
+      <c r="P14" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="Q14" s="47"/>
+      <c r="Q14" s="50"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
-      <c r="X14" s="44" t="s">
+      <c r="X14" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y14" s="45"/>
-      <c r="Z14" s="46"/>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="49"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
@@ -4951,18 +4967,18 @@
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="47" t="s">
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K15" s="47"/>
+      <c r="K15" s="50"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -4975,11 +4991,11 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
-      <c r="X15" s="44" t="s">
+      <c r="X15" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y15" s="45"/>
-      <c r="Z15" s="46"/>
+      <c r="Y15" s="48"/>
+      <c r="Z15" s="49"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
@@ -4996,10 +5012,10 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="47" t="s">
+      <c r="J16" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K16" s="47"/>
+      <c r="K16" s="50"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -5012,11 +5028,11 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
-      <c r="X16" s="44" t="s">
+      <c r="X16" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y16" s="45"/>
-      <c r="Z16" s="46"/>
+      <c r="Y16" s="48"/>
+      <c r="Z16" s="49"/>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
@@ -5033,10 +5049,10 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="47" t="s">
+      <c r="J17" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="47"/>
+      <c r="K17" s="50"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -5049,11 +5065,11 @@
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
-      <c r="X17" s="44" t="s">
+      <c r="X17" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y17" s="45"/>
-      <c r="Z17" s="46"/>
+      <c r="Y17" s="48"/>
+      <c r="Z17" s="49"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
@@ -5070,15 +5086,15 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="47" t="s">
+      <c r="J18" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K18" s="47"/>
-      <c r="L18" s="44" t="s">
+      <c r="K18" s="50"/>
+      <c r="L18" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="M18" s="45"/>
-      <c r="N18" s="46"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="49"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -5088,15 +5104,15 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
-      <c r="X18" s="44" t="s">
+      <c r="X18" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y18" s="45"/>
-      <c r="Z18" s="46"/>
-      <c r="AA18" s="44" t="s">
+      <c r="Y18" s="48"/>
+      <c r="Z18" s="49"/>
+      <c r="AA18" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="AB18" s="46"/>
+      <c r="AB18" s="49"/>
       <c r="AC18" s="2"/>
     </row>
     <row r="19" spans="1:29">
@@ -5111,10 +5127,10 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="47" t="s">
+      <c r="J19" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K19" s="47"/>
+      <c r="K19" s="50"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -5127,15 +5143,15 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
-      <c r="X19" s="44" t="s">
+      <c r="X19" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y19" s="45"/>
-      <c r="Z19" s="46"/>
-      <c r="AA19" s="44" t="s">
+      <c r="Y19" s="48"/>
+      <c r="Z19" s="49"/>
+      <c r="AA19" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="AB19" s="46"/>
+      <c r="AB19" s="49"/>
       <c r="AC19" s="2"/>
     </row>
     <row r="20" spans="1:29">
@@ -5150,10 +5166,10 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="47" t="s">
+      <c r="J20" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K20" s="47"/>
+      <c r="K20" s="50"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -5166,11 +5182,11 @@
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
-      <c r="X20" s="44" t="s">
+      <c r="X20" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y20" s="45"/>
-      <c r="Z20" s="46"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="49"/>
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
@@ -5187,10 +5203,10 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="47" t="s">
+      <c r="J21" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K21" s="47"/>
+      <c r="K21" s="50"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -5203,11 +5219,11 @@
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
-      <c r="X21" s="44" t="s">
+      <c r="X21" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y21" s="45"/>
-      <c r="Z21" s="46"/>
+      <c r="Y21" s="48"/>
+      <c r="Z21" s="49"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
@@ -5224,10 +5240,10 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="47" t="s">
+      <c r="J22" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K22" s="47"/>
+      <c r="K22" s="50"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -5240,11 +5256,11 @@
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
-      <c r="X22" s="44" t="s">
+      <c r="X22" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y22" s="45"/>
-      <c r="Z22" s="46"/>
+      <c r="Y22" s="48"/>
+      <c r="Z22" s="49"/>
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
@@ -5261,10 +5277,10 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="47" t="s">
+      <c r="J23" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K23" s="47"/>
+      <c r="K23" s="50"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -5277,11 +5293,11 @@
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
-      <c r="X23" s="44" t="s">
+      <c r="X23" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y23" s="45"/>
-      <c r="Z23" s="46"/>
+      <c r="Y23" s="48"/>
+      <c r="Z23" s="49"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
@@ -5298,10 +5314,10 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="47" t="s">
+      <c r="J24" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K24" s="47"/>
+      <c r="K24" s="50"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -5314,11 +5330,11 @@
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
-      <c r="X24" s="44" t="s">
+      <c r="X24" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y24" s="45"/>
-      <c r="Z24" s="46"/>
+      <c r="Y24" s="48"/>
+      <c r="Z24" s="49"/>
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
@@ -5335,10 +5351,10 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="47" t="s">
+      <c r="J25" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K25" s="47"/>
+      <c r="K25" s="50"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -5351,11 +5367,11 @@
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
-      <c r="X25" s="44" t="s">
+      <c r="X25" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y25" s="45"/>
-      <c r="Z25" s="46"/>
+      <c r="Y25" s="48"/>
+      <c r="Z25" s="49"/>
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
@@ -5372,10 +5388,10 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="47" t="s">
+      <c r="J26" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K26" s="47"/>
+      <c r="K26" s="50"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -5388,11 +5404,11 @@
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
-      <c r="X26" s="44" t="s">
+      <c r="X26" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y26" s="45"/>
-      <c r="Z26" s="46"/>
+      <c r="Y26" s="48"/>
+      <c r="Z26" s="49"/>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
@@ -5409,10 +5425,10 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="47" t="s">
+      <c r="J27" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K27" s="47"/>
+      <c r="K27" s="50"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -5425,11 +5441,11 @@
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
-      <c r="X27" s="44" t="s">
+      <c r="X27" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y27" s="45"/>
-      <c r="Z27" s="46"/>
+      <c r="Y27" s="48"/>
+      <c r="Z27" s="49"/>
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
@@ -5446,10 +5462,10 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="47" t="s">
+      <c r="J28" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K28" s="47"/>
+      <c r="K28" s="50"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -5462,11 +5478,11 @@
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
-      <c r="X28" s="44" t="s">
+      <c r="X28" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y28" s="45"/>
-      <c r="Z28" s="46"/>
+      <c r="Y28" s="48"/>
+      <c r="Z28" s="49"/>
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
@@ -5483,10 +5499,10 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="47" t="s">
+      <c r="J29" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K29" s="47"/>
+      <c r="K29" s="50"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -5499,11 +5515,11 @@
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
-      <c r="X29" s="44" t="s">
+      <c r="X29" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y29" s="45"/>
-      <c r="Z29" s="46"/>
+      <c r="Y29" s="48"/>
+      <c r="Z29" s="49"/>
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
@@ -5520,10 +5536,10 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="47" t="s">
+      <c r="J30" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K30" s="47"/>
+      <c r="K30" s="50"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -5536,11 +5552,11 @@
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
-      <c r="X30" s="44" t="s">
+      <c r="X30" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y30" s="45"/>
-      <c r="Z30" s="46"/>
+      <c r="Y30" s="48"/>
+      <c r="Z30" s="49"/>
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
@@ -5557,10 +5573,10 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="47" t="s">
+      <c r="J31" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K31" s="47"/>
+      <c r="K31" s="50"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -5573,11 +5589,11 @@
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
-      <c r="X31" s="44" t="s">
+      <c r="X31" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y31" s="45"/>
-      <c r="Z31" s="46"/>
+      <c r="Y31" s="48"/>
+      <c r="Z31" s="49"/>
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
@@ -5594,10 +5610,10 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="47" t="s">
+      <c r="J32" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K32" s="47"/>
+      <c r="K32" s="50"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5610,11 +5626,11 @@
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
-      <c r="X32" s="44" t="s">
+      <c r="X32" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y32" s="45"/>
-      <c r="Z32" s="46"/>
+      <c r="Y32" s="48"/>
+      <c r="Z32" s="49"/>
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
@@ -5631,10 +5647,10 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="47" t="s">
+      <c r="J33" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K33" s="47"/>
+      <c r="K33" s="50"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5647,11 +5663,11 @@
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
-      <c r="X33" s="44" t="s">
+      <c r="X33" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y33" s="45"/>
-      <c r="Z33" s="46"/>
+      <c r="Y33" s="48"/>
+      <c r="Z33" s="49"/>
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
@@ -5668,10 +5684,10 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="47" t="s">
+      <c r="J34" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K34" s="47"/>
+      <c r="K34" s="50"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5684,11 +5700,11 @@
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
-      <c r="X34" s="44" t="s">
+      <c r="X34" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y34" s="45"/>
-      <c r="Z34" s="46"/>
+      <c r="Y34" s="48"/>
+      <c r="Z34" s="49"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
@@ -5705,10 +5721,10 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="47" t="s">
+      <c r="J35" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K35" s="47"/>
+      <c r="K35" s="50"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5721,11 +5737,11 @@
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
-      <c r="X35" s="44" t="s">
+      <c r="X35" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y35" s="45"/>
-      <c r="Z35" s="46"/>
+      <c r="Y35" s="48"/>
+      <c r="Z35" s="49"/>
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
       <c r="AC35" s="2"/>
@@ -5742,10 +5758,10 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="47" t="s">
+      <c r="J36" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K36" s="47"/>
+      <c r="K36" s="50"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5758,11 +5774,11 @@
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
       <c r="W36" s="2"/>
-      <c r="X36" s="44" t="s">
+      <c r="X36" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y36" s="45"/>
-      <c r="Z36" s="46"/>
+      <c r="Y36" s="48"/>
+      <c r="Z36" s="49"/>
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
       <c r="AC36" s="2"/>
@@ -5779,10 +5795,10 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="47" t="s">
+      <c r="J37" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K37" s="47"/>
+      <c r="K37" s="50"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5795,11 +5811,11 @@
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
       <c r="W37" s="2"/>
-      <c r="X37" s="44" t="s">
+      <c r="X37" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="Y37" s="45"/>
-      <c r="Z37" s="46"/>
+      <c r="Y37" s="48"/>
+      <c r="Z37" s="49"/>
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
       <c r="AC37" s="2"/>

</xml_diff>

<commit_message>
Added column-activity dictionaries, to allow for a different one every day and for each type. This is HARDCODED!
</commit_message>
<xml_diff>
--- a/BarcodeScanner/planning kinderen en leiding.xlsx
+++ b/BarcodeScanner/planning kinderen en leiding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="9480" windowHeight="7920"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="9480" windowHeight="7920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kleine speltakken" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="117">
   <si>
     <t>Avondeten</t>
   </si>
@@ -361,6 +361,12 @@
   </si>
   <si>
     <t>19 + 20 + 21 + 22 + 23 + 24</t>
+  </si>
+  <si>
+    <t>zaterdag</t>
+  </si>
+  <si>
+    <t>zondag</t>
   </si>
 </sst>
 </file>
@@ -597,23 +603,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -655,6 +649,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -663,15 +674,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1007,9 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C5" sqref="C5:I5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1025,19 +1026,19 @@
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="12.75"/>
     <row r="2" spans="1:11" s="4" customFormat="1" ht="15.75">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
     </row>
     <row r="3" spans="1:11" s="4" customFormat="1" ht="12.75">
       <c r="A3" s="3"/>
@@ -1051,35 +1052,37 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="27" t="s">
+      <c r="A4" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="35"/>
+      <c r="C4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="29">
+      <c r="A5" s="25">
         <v>40831.395833333336</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="25">
         <v>40831.416666666664</v>
       </c>
       <c r="C5" s="41" t="s">
@@ -1099,31 +1102,31 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="29">
+      <c r="A6" s="25">
         <v>40831.416666666664</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="26">
         <v>40831.430555555555</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="27" t="s">
         <v>44</v>
       </c>
       <c r="J6" s="6">
@@ -1134,10 +1137,10 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A7" s="29">
+      <c r="A7" s="25">
         <v>40831.430555555555</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="26">
         <v>40831.444444444445</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -1149,16 +1152,16 @@
       <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="27" t="s">
         <v>44</v>
       </c>
       <c r="J7" s="6">
@@ -1169,10 +1172,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A8" s="29">
+      <c r="A8" s="25">
         <v>40831.444444444445</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="26">
         <v>40831.458333333336</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1184,16 +1187,16 @@
       <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="27" t="s">
         <v>44</v>
       </c>
       <c r="J8" s="6">
@@ -1204,10 +1207,10 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A9" s="29">
+      <c r="A9" s="25">
         <v>40831.458333333336</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="26">
         <v>40831.472222222219</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -1219,16 +1222,16 @@
       <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="I9" s="27" t="s">
         <v>44</v>
       </c>
       <c r="J9" s="6">
@@ -1239,10 +1242,10 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A10" s="29">
+      <c r="A10" s="25">
         <v>40831.472222222219</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="26">
         <v>40831.486111111109</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1254,16 +1257,16 @@
       <c r="E10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="31" t="s">
+      <c r="I10" s="27" t="s">
         <v>44</v>
       </c>
       <c r="J10" s="6">
@@ -1274,10 +1277,10 @@
       </c>
     </row>
     <row r="11" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A11" s="29">
+      <c r="A11" s="25">
         <v>40831.486111111109</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="26">
         <v>40831.5</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1289,16 +1292,16 @@
       <c r="E11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="27" t="s">
         <v>44</v>
       </c>
       <c r="J11" s="6">
@@ -1309,21 +1312,21 @@
       </c>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="29">
+      <c r="A12" s="25">
         <v>40831.5</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="26">
         <v>40831.527777777781</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="6">
         <v>0.5</v>
       </c>
@@ -1332,10 +1335,10 @@
       </c>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A13" s="29">
+      <c r="A13" s="25">
         <v>40831.527777777781</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="26">
         <v>40831.541666666664</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1347,16 +1350,16 @@
       <c r="E13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H13" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="31" t="s">
+      <c r="I13" s="27" t="s">
         <v>45</v>
       </c>
       <c r="J13" s="6">
@@ -1367,10 +1370,10 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A14" s="29">
+      <c r="A14" s="25">
         <v>40831.541666666664</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="26">
         <v>40831.555555555555</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -1382,16 +1385,16 @@
       <c r="E14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="31" t="s">
+      <c r="I14" s="27" t="s">
         <v>45</v>
       </c>
       <c r="J14" s="6">
@@ -1402,10 +1405,10 @@
       </c>
     </row>
     <row r="15" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A15" s="29">
+      <c r="A15" s="25">
         <v>40831.555555555555</v>
       </c>
-      <c r="B15" s="30">
+      <c r="B15" s="26">
         <v>40831.569444444445</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -1417,16 +1420,16 @@
       <c r="E15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H15" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="27" t="s">
         <v>45</v>
       </c>
       <c r="J15" s="6">
@@ -1437,10 +1440,10 @@
       </c>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A16" s="29">
+      <c r="A16" s="25">
         <v>40831.569444444445</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="26">
         <v>40831.583333333336</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -1452,16 +1455,16 @@
       <c r="E16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="31" t="s">
+      <c r="I16" s="27" t="s">
         <v>45</v>
       </c>
       <c r="J16" s="6">
@@ -1472,10 +1475,10 @@
       </c>
     </row>
     <row r="17" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A17" s="29">
+      <c r="A17" s="25">
         <v>40831.583333333336</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="26">
         <v>40831.597222222219</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1487,16 +1490,16 @@
       <c r="E17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="33" t="s">
+      <c r="G17" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="31" t="s">
+      <c r="H17" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="31" t="s">
+      <c r="I17" s="27" t="s">
         <v>45</v>
       </c>
       <c r="J17" s="6">
@@ -1507,10 +1510,10 @@
       </c>
     </row>
     <row r="18" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A18" s="29">
+      <c r="A18" s="25">
         <v>40831.597222222219</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="26">
         <v>40831.611111111109</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1522,16 +1525,16 @@
       <c r="E18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="G18" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="31" t="s">
+      <c r="H18" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="31" t="s">
+      <c r="I18" s="27" t="s">
         <v>45</v>
       </c>
       <c r="J18" s="6">
@@ -1542,10 +1545,10 @@
       </c>
     </row>
     <row r="19" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A19" s="29">
+      <c r="A19" s="25">
         <v>40831.611111111109</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="26">
         <v>40831.625</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -1557,16 +1560,16 @@
       <c r="E19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="I19" s="31" t="s">
+      <c r="I19" s="27" t="s">
         <v>46</v>
       </c>
       <c r="J19" s="6">
@@ -1577,10 +1580,10 @@
       </c>
     </row>
     <row r="20" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A20" s="29">
+      <c r="A20" s="25">
         <v>40831.625</v>
       </c>
-      <c r="B20" s="30">
+      <c r="B20" s="26">
         <v>40831.638888888891</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1592,16 +1595,16 @@
       <c r="E20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="I20" s="31" t="s">
+      <c r="I20" s="27" t="s">
         <v>46</v>
       </c>
       <c r="J20" s="6">
@@ -1612,10 +1615,10 @@
       </c>
     </row>
     <row r="21" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A21" s="29">
+      <c r="A21" s="25">
         <v>40831.638888888891</v>
       </c>
-      <c r="B21" s="30">
+      <c r="B21" s="26">
         <v>40831.652777777781</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -1627,16 +1630,16 @@
       <c r="E21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H21" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="27" t="s">
         <v>46</v>
       </c>
       <c r="J21" s="6">
@@ -1647,10 +1650,10 @@
       </c>
     </row>
     <row r="22" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A22" s="29">
+      <c r="A22" s="25">
         <v>40831.652777777781</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="26">
         <v>40831.666666666664</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -1662,16 +1665,16 @@
       <c r="E22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="34" t="s">
+      <c r="F22" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="33" t="s">
+      <c r="G22" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="H22" s="31" t="s">
+      <c r="H22" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="31" t="s">
+      <c r="I22" s="27" t="s">
         <v>46</v>
       </c>
       <c r="J22" s="6">
@@ -1682,10 +1685,10 @@
       </c>
     </row>
     <row r="23" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A23" s="29">
+      <c r="A23" s="25">
         <v>40831.666666666664</v>
       </c>
-      <c r="B23" s="30">
+      <c r="B23" s="26">
         <v>40831.680555555555</v>
       </c>
       <c r="C23" s="5" t="s">
@@ -1697,16 +1700,16 @@
       <c r="E23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="34" t="s">
+      <c r="F23" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="33" t="s">
+      <c r="G23" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="H23" s="31" t="s">
+      <c r="H23" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="31" t="s">
+      <c r="I23" s="27" t="s">
         <v>46</v>
       </c>
       <c r="J23" s="6">
@@ -1717,10 +1720,10 @@
       </c>
     </row>
     <row r="24" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A24" s="29">
+      <c r="A24" s="25">
         <v>40831.680555555555</v>
       </c>
-      <c r="B24" s="30">
+      <c r="B24" s="26">
         <v>40831.694444444445</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -1732,16 +1735,16 @@
       <c r="E24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="G24" s="33" t="s">
+      <c r="G24" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="H24" s="31" t="s">
+      <c r="H24" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="I24" s="31" t="s">
+      <c r="I24" s="27" t="s">
         <v>46</v>
       </c>
       <c r="J24" s="6">
@@ -1752,21 +1755,21 @@
       </c>
     </row>
     <row r="25" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A25" s="29">
+      <c r="A25" s="25">
         <v>40831.694444444445</v>
       </c>
-      <c r="B25" s="30">
+      <c r="B25" s="26">
         <v>40831.736111111109</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
       <c r="J25" s="6">
         <v>0.69444444444444497</v>
       </c>
@@ -1775,21 +1778,21 @@
       </c>
     </row>
     <row r="26" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A26" s="29">
+      <c r="A26" s="25">
         <v>40831.736111111109</v>
       </c>
-      <c r="B26" s="30">
+      <c r="B26" s="26">
         <v>40831.770833333336</v>
       </c>
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
       <c r="J26" s="6">
         <v>0.73611111111111205</v>
       </c>
@@ -1798,21 +1801,21 @@
       </c>
     </row>
     <row r="27" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A27" s="29">
+      <c r="A27" s="25">
         <v>40831.770833333336</v>
       </c>
-      <c r="B27" s="30">
+      <c r="B27" s="26">
         <v>40831.791666666664</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
       <c r="J27" s="6">
         <v>0.77083333333333337</v>
       </c>
@@ -1821,21 +1824,21 @@
       </c>
     </row>
     <row r="28" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A28" s="29">
+      <c r="A28" s="25">
         <v>40831.791666666664</v>
       </c>
-      <c r="B28" s="30">
+      <c r="B28" s="26">
         <v>40831.916666666664</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
       <c r="J28" s="6">
         <v>0.79166666666666663</v>
       </c>
@@ -1844,21 +1847,21 @@
       </c>
     </row>
     <row r="29" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A29" s="29">
+      <c r="A29" s="25">
         <v>40831.916666666664</v>
       </c>
-      <c r="B29" s="30">
+      <c r="B29" s="26">
         <v>40831.9375</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
       <c r="J29" s="6">
         <v>0.91666666666666663</v>
       </c>
@@ -1867,21 +1870,21 @@
       </c>
     </row>
     <row r="30" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A30" s="29">
+      <c r="A30" s="25">
         <v>40831.9375</v>
       </c>
-      <c r="B30" s="30">
+      <c r="B30" s="26">
         <v>40831.291666666664</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
       <c r="J30" s="6">
         <v>0.9375</v>
       </c>
@@ -1890,47 +1893,49 @@
       </c>
     </row>
     <row r="31" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
     </row>
     <row r="32" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A32" s="21"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
     </row>
     <row r="33" spans="1:11" s="4" customFormat="1" ht="15.75">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
     </row>
     <row r="34" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A34" s="38"/>
-      <c r="B34" s="38"/>
+      <c r="A34" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" s="37"/>
       <c r="C34" s="9" t="s">
         <v>9</v>
       </c>
@@ -1951,20 +1956,20 @@
       </c>
     </row>
     <row r="35" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A35" s="32">
+      <c r="A35" s="28">
         <v>40832.291666666664</v>
       </c>
-      <c r="B35" s="32">
+      <c r="B35" s="28">
         <v>40832.333333333336</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
       <c r="I35" s="8">
         <v>0.29166666666666669</v>
       </c>
@@ -1973,20 +1978,20 @@
       </c>
     </row>
     <row r="36" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A36" s="32">
+      <c r="A36" s="28">
         <v>40832.333333333336</v>
       </c>
-      <c r="B36" s="32">
+      <c r="B36" s="28">
         <v>40832.361111111109</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
       <c r="I36" s="8">
         <v>0.33333333333333331</v>
       </c>
@@ -1995,20 +2000,20 @@
       </c>
     </row>
     <row r="37" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A37" s="32">
+      <c r="A37" s="28">
         <v>40832.361111111109</v>
       </c>
-      <c r="B37" s="32">
+      <c r="B37" s="28">
         <v>40832.402777777781</v>
       </c>
-      <c r="C37" s="35" t="s">
+      <c r="C37" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="35"/>
-      <c r="H37" s="35"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
       <c r="I37" s="8">
         <v>0.3611111111111111</v>
       </c>
@@ -2017,10 +2022,10 @@
       </c>
     </row>
     <row r="38" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A38" s="32">
+      <c r="A38" s="28">
         <v>40832.402777777781</v>
       </c>
-      <c r="B38" s="32">
+      <c r="B38" s="28">
         <v>40832.416666666664</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -2029,16 +2034,16 @@
       <c r="D38" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="33" t="s">
+      <c r="E38" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="F38" s="31" t="s">
+      <c r="F38" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="G38" s="33" t="s">
+      <c r="G38" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="H38" s="31" t="s">
+      <c r="H38" s="27" t="s">
         <v>73</v>
       </c>
       <c r="I38" s="8">
@@ -2049,10 +2054,10 @@
       </c>
     </row>
     <row r="39" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A39" s="32">
+      <c r="A39" s="28">
         <v>40832.416666666664</v>
       </c>
-      <c r="B39" s="32">
+      <c r="B39" s="28">
         <v>40832.430555555555</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -2061,16 +2066,16 @@
       <c r="D39" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="33" t="s">
+      <c r="E39" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="31" t="s">
+      <c r="F39" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="G39" s="33" t="s">
+      <c r="G39" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="H39" s="31" t="s">
+      <c r="H39" s="27" t="s">
         <v>73</v>
       </c>
       <c r="I39" s="8">
@@ -2081,10 +2086,10 @@
       </c>
     </row>
     <row r="40" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A40" s="32">
+      <c r="A40" s="28">
         <v>40832.430555555555</v>
       </c>
-      <c r="B40" s="32">
+      <c r="B40" s="28">
         <v>40832.444444444445</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -2093,16 +2098,16 @@
       <c r="D40" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="33" t="s">
+      <c r="F40" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="G40" s="31" t="s">
+      <c r="G40" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="H40" s="33" t="s">
+      <c r="H40" s="29" t="s">
         <v>73</v>
       </c>
       <c r="I40" s="8">
@@ -2113,10 +2118,10 @@
       </c>
     </row>
     <row r="41" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A41" s="32">
+      <c r="A41" s="28">
         <v>40832.444444444445</v>
       </c>
-      <c r="B41" s="32">
+      <c r="B41" s="28">
         <v>40832.458333333336</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -2125,16 +2130,16 @@
       <c r="D41" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="31" t="s">
+      <c r="E41" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="F41" s="33" t="s">
+      <c r="F41" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="G41" s="31" t="s">
+      <c r="G41" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="H41" s="33" t="s">
+      <c r="H41" s="29" t="s">
         <v>73</v>
       </c>
       <c r="I41" s="8">
@@ -2145,10 +2150,10 @@
       </c>
     </row>
     <row r="42" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A42" s="32">
+      <c r="A42" s="28">
         <v>40832.458333333336</v>
       </c>
-      <c r="B42" s="32">
+      <c r="B42" s="28">
         <v>40832.472222222219</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -2157,16 +2162,16 @@
       <c r="D42" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="33" t="s">
+      <c r="E42" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F42" s="31" t="s">
+      <c r="F42" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="G42" s="33" t="s">
+      <c r="G42" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="H42" s="31" t="s">
+      <c r="H42" s="27" t="s">
         <v>74</v>
       </c>
       <c r="I42" s="8">
@@ -2177,10 +2182,10 @@
       </c>
     </row>
     <row r="43" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A43" s="32">
+      <c r="A43" s="28">
         <v>40832.472222222219</v>
       </c>
-      <c r="B43" s="32">
+      <c r="B43" s="28">
         <v>40832.486111111109</v>
       </c>
       <c r="C43" s="5" t="s">
@@ -2189,16 +2194,16 @@
       <c r="D43" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="33" t="s">
+      <c r="E43" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F43" s="31" t="s">
+      <c r="F43" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="G43" s="33" t="s">
+      <c r="G43" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="H43" s="31" t="s">
+      <c r="H43" s="27" t="s">
         <v>74</v>
       </c>
       <c r="I43" s="8">
@@ -2209,10 +2214,10 @@
       </c>
     </row>
     <row r="44" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A44" s="32">
+      <c r="A44" s="28">
         <v>40832.486111111109</v>
       </c>
-      <c r="B44" s="32">
+      <c r="B44" s="28">
         <v>40832.5</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -2221,16 +2226,16 @@
       <c r="D44" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="31" t="s">
+      <c r="E44" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="F44" s="33" t="s">
+      <c r="F44" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G44" s="31" t="s">
+      <c r="G44" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="H44" s="33" t="s">
+      <c r="H44" s="29" t="s">
         <v>74</v>
       </c>
       <c r="I44" s="8">
@@ -2241,10 +2246,10 @@
       </c>
     </row>
     <row r="45" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A45" s="32">
+      <c r="A45" s="28">
         <v>40832.5</v>
       </c>
-      <c r="B45" s="32">
+      <c r="B45" s="28">
         <v>40832.513888888891</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -2253,16 +2258,16 @@
       <c r="D45" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E45" s="31" t="s">
+      <c r="E45" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="F45" s="33" t="s">
+      <c r="F45" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G45" s="31" t="s">
+      <c r="G45" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="H45" s="33" t="s">
+      <c r="H45" s="29" t="s">
         <v>74</v>
       </c>
       <c r="I45" s="8">
@@ -2273,20 +2278,20 @@
       </c>
     </row>
     <row r="46" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A46" s="32">
+      <c r="A46" s="28">
         <v>40832.513888888891</v>
       </c>
-      <c r="B46" s="32">
+      <c r="B46" s="28">
         <v>40832.541666666664</v>
       </c>
-      <c r="C46" s="36" t="s">
+      <c r="C46" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="39"/>
       <c r="I46" s="8">
         <v>0.51388888888888895</v>
       </c>
@@ -2295,10 +2300,10 @@
       </c>
     </row>
     <row r="47" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A47" s="32">
+      <c r="A47" s="28">
         <v>40832.541666666664</v>
       </c>
-      <c r="B47" s="32">
+      <c r="B47" s="28">
         <v>40832.555555555555</v>
       </c>
       <c r="C47" s="5" t="s">
@@ -2307,16 +2312,16 @@
       <c r="D47" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E47" s="33" t="s">
+      <c r="E47" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F47" s="31" t="s">
+      <c r="F47" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="G47" s="33" t="s">
+      <c r="G47" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="H47" s="31" t="s">
+      <c r="H47" s="27" t="s">
         <v>75</v>
       </c>
       <c r="I47" s="8">
@@ -2327,10 +2332,10 @@
       </c>
     </row>
     <row r="48" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A48" s="32">
+      <c r="A48" s="28">
         <v>40832.555555555555</v>
       </c>
-      <c r="B48" s="32">
+      <c r="B48" s="28">
         <v>40832.569444444445</v>
       </c>
       <c r="C48" s="5" t="s">
@@ -2339,16 +2344,16 @@
       <c r="D48" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E48" s="33" t="s">
+      <c r="E48" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F48" s="31" t="s">
+      <c r="F48" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="G48" s="33" t="s">
+      <c r="G48" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="H48" s="31" t="s">
+      <c r="H48" s="27" t="s">
         <v>75</v>
       </c>
       <c r="I48" s="8">
@@ -2359,10 +2364,10 @@
       </c>
     </row>
     <row r="49" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A49" s="32">
+      <c r="A49" s="28">
         <v>40832.569444444445</v>
       </c>
-      <c r="B49" s="32">
+      <c r="B49" s="28">
         <v>40832.583333333336</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -2371,16 +2376,16 @@
       <c r="D49" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E49" s="31" t="s">
+      <c r="E49" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="F49" s="33" t="s">
+      <c r="F49" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="G49" s="31" t="s">
+      <c r="G49" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="H49" s="33" t="s">
+      <c r="H49" s="29" t="s">
         <v>75</v>
       </c>
       <c r="I49" s="8">
@@ -2391,10 +2396,10 @@
       </c>
     </row>
     <row r="50" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A50" s="32">
+      <c r="A50" s="28">
         <v>40832.583333333336</v>
       </c>
-      <c r="B50" s="32">
+      <c r="B50" s="28">
         <v>40832.597222222219</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -2403,16 +2408,16 @@
       <c r="D50" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E50" s="31" t="s">
+      <c r="E50" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="F50" s="33" t="s">
+      <c r="F50" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="G50" s="31" t="s">
+      <c r="G50" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="H50" s="33" t="s">
+      <c r="H50" s="29" t="s">
         <v>75</v>
       </c>
       <c r="I50" s="8">
@@ -2423,20 +2428,20 @@
       </c>
     </row>
     <row r="51" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A51" s="32">
+      <c r="A51" s="28">
         <v>40832.597222222219</v>
       </c>
-      <c r="B51" s="32">
+      <c r="B51" s="28">
         <v>40832.638888888891</v>
       </c>
-      <c r="C51" s="35" t="s">
+      <c r="C51" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="35"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="38"/>
       <c r="I51" s="8">
         <v>0.59722222222222199</v>
       </c>
@@ -2445,20 +2450,20 @@
       </c>
     </row>
     <row r="52" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A52" s="32">
+      <c r="A52" s="28">
         <v>40832.638888888891</v>
       </c>
-      <c r="B52" s="32">
+      <c r="B52" s="28">
         <v>40832.645833333336</v>
       </c>
-      <c r="C52" s="35" t="s">
+      <c r="C52" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="35"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
       <c r="I52" s="8">
         <v>0.63888888888888895</v>
       </c>
@@ -2470,18 +2475,14 @@
     <row r="54" spans="1:10" s="4" customFormat="1" ht="12.75"/>
     <row r="55" spans="1:10" s="4" customFormat="1" ht="12.75"/>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
+  <mergeCells count="16">
     <mergeCell ref="C51:H51"/>
     <mergeCell ref="C52:H52"/>
     <mergeCell ref="C46:H46"/>
     <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A34:B34"/>
     <mergeCell ref="C35:H35"/>
     <mergeCell ref="C36:H36"/>
     <mergeCell ref="C37:H37"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A33:K33"/>
     <mergeCell ref="C29:I29"/>
     <mergeCell ref="C30:I30"/>
@@ -2489,6 +2490,8 @@
     <mergeCell ref="C5:I5"/>
     <mergeCell ref="C12:I12"/>
     <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2497,15 +2500,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4"/>
+    <col min="1" max="2" width="13.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="4" customWidth="1"/>
     <col min="4" max="4" width="13.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="4" customWidth="1"/>
@@ -2517,25 +2520,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
@@ -2556,20 +2559,20 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="6">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C3" s="36" t="s">
+      <c r="A3" s="25">
+        <v>40831.395833333336</v>
+      </c>
+      <c r="B3" s="25">
+        <v>40831.416666666664</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
       <c r="I3" s="7">
         <v>0.39583333333333331</v>
       </c>
@@ -2578,20 +2581,20 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="6">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="B4" s="7">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="C4" s="36" t="s">
+      <c r="A4" s="25">
+        <v>40831.416666666664</v>
+      </c>
+      <c r="B4" s="26">
+        <v>40831.458333333336</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
       <c r="I4" s="7">
         <v>0.41666666666666669</v>
       </c>
@@ -2600,20 +2603,20 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
-      <c r="A5" s="6">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="B5" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="C5" s="36" t="s">
+      <c r="A5" s="25">
+        <v>40831.458333333336</v>
+      </c>
+      <c r="B5" s="26">
+        <v>40831.5</v>
+      </c>
+      <c r="C5" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
       <c r="I5" s="7">
         <v>0.45833333333333331</v>
       </c>
@@ -2622,11 +2625,11 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="B6" s="8">
-        <v>0.51388888888888895</v>
+      <c r="A6" s="28">
+        <v>40831.5</v>
+      </c>
+      <c r="B6" s="28">
+        <v>40831.513888888891</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>79</v>
@@ -2646,7 +2649,7 @@
       <c r="H6" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="21">
         <v>0.5</v>
       </c>
       <c r="J6" s="8">
@@ -2654,11 +2657,11 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="8">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="B7" s="8">
-        <v>0.52777777777777801</v>
+      <c r="A7" s="28">
+        <v>40831.513888888891</v>
+      </c>
+      <c r="B7" s="28">
+        <v>40831.527777777781</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>80</v>
@@ -2678,7 +2681,7 @@
       <c r="H7" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="21">
         <v>0.51388888888888895</v>
       </c>
       <c r="J7" s="8">
@@ -2686,11 +2689,11 @@
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="8">
-        <v>0.52777777777777801</v>
-      </c>
-      <c r="B8" s="8">
-        <v>0.54166666666666696</v>
+      <c r="A8" s="28">
+        <v>40831.527777777781</v>
+      </c>
+      <c r="B8" s="28">
+        <v>40831.541666666664</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>81</v>
@@ -2710,7 +2713,7 @@
       <c r="H8" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="21">
         <v>0.52777777777777801</v>
       </c>
       <c r="J8" s="8">
@@ -2718,11 +2721,11 @@
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="8">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="B9" s="8">
-        <v>0.55555555555555602</v>
+      <c r="A9" s="28">
+        <v>40831.541666666664</v>
+      </c>
+      <c r="B9" s="28">
+        <v>40831.555555555555</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>82</v>
@@ -2742,7 +2745,7 @@
       <c r="H9" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="21">
         <v>0.54166666666666696</v>
       </c>
       <c r="J9" s="8">
@@ -2750,20 +2753,20 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="6">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="B10" s="7">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="C10" s="36" t="s">
+      <c r="A10" s="25">
+        <v>40831.555555555555</v>
+      </c>
+      <c r="B10" s="26">
+        <v>40831.583333333336</v>
+      </c>
+      <c r="C10" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
       <c r="I10" s="7">
         <v>0.55555555555555558</v>
       </c>
@@ -2772,11 +2775,11 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="8">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="B11" s="8">
-        <v>0.59722222222222221</v>
+      <c r="A11" s="28">
+        <v>40831.583333333336</v>
+      </c>
+      <c r="B11" s="28">
+        <v>40831.597222222219</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>83</v>
@@ -2796,7 +2799,7 @@
       <c r="H11" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="21">
         <v>0.58333333333333337</v>
       </c>
       <c r="J11" s="8">
@@ -2804,11 +2807,11 @@
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="8">
-        <v>0.59722222222222299</v>
-      </c>
-      <c r="B12" s="8">
-        <v>0.61111111111111205</v>
+      <c r="A12" s="28">
+        <v>40831.597222222219</v>
+      </c>
+      <c r="B12" s="28">
+        <v>40831.611111111109</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>84</v>
@@ -2828,7 +2831,7 @@
       <c r="H12" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="21">
         <v>0.59722222222222299</v>
       </c>
       <c r="J12" s="8">
@@ -2836,11 +2839,11 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="8">
-        <v>0.61111111111111205</v>
-      </c>
-      <c r="B13" s="8">
-        <v>0.625</v>
+      <c r="A13" s="28">
+        <v>40831.611111111109</v>
+      </c>
+      <c r="B13" s="28">
+        <v>40831.625</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>85</v>
@@ -2860,7 +2863,7 @@
       <c r="H13" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="21">
         <v>0.61111111111111205</v>
       </c>
       <c r="J13" s="8">
@@ -2868,11 +2871,11 @@
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="8">
-        <v>0.625</v>
-      </c>
-      <c r="B14" s="8">
-        <v>0.63888888888888895</v>
+      <c r="A14" s="28">
+        <v>40831.625</v>
+      </c>
+      <c r="B14" s="28">
+        <v>40831.638888888891</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>86</v>
@@ -2892,7 +2895,7 @@
       <c r="H14" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="21">
         <v>0.625</v>
       </c>
       <c r="J14" s="8">
@@ -2900,11 +2903,11 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="8">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="B15" s="8">
-        <v>0.65277777777777801</v>
+      <c r="A15" s="28">
+        <v>40831.638888888891</v>
+      </c>
+      <c r="B15" s="28">
+        <v>40831.652777777781</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>87</v>
@@ -2924,7 +2927,7 @@
       <c r="H15" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="21">
         <v>0.63888888888888895</v>
       </c>
       <c r="J15" s="8">
@@ -2932,11 +2935,11 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="8">
-        <v>0.65277777777777801</v>
-      </c>
-      <c r="B16" s="8">
-        <v>0.66666666666666696</v>
+      <c r="A16" s="28">
+        <v>40831.652777777781</v>
+      </c>
+      <c r="B16" s="28">
+        <v>40831.666666666664</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>88</v>
@@ -2956,7 +2959,7 @@
       <c r="H16" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="21">
         <v>0.65277777777777801</v>
       </c>
       <c r="J16" s="8">
@@ -2964,11 +2967,11 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="8">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="B17" s="8">
-        <v>0.68055555555555602</v>
+      <c r="A17" s="28">
+        <v>40831.666666666664</v>
+      </c>
+      <c r="B17" s="28">
+        <v>40831.680555555555</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>89</v>
@@ -2988,7 +2991,7 @@
       <c r="H17" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="21">
         <v>0.66666666666666696</v>
       </c>
       <c r="J17" s="8">
@@ -2996,11 +2999,11 @@
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="8">
-        <v>0.68055555555555602</v>
-      </c>
-      <c r="B18" s="8">
-        <v>0.69444444444444453</v>
+      <c r="A18" s="28">
+        <v>40831.680555555555</v>
+      </c>
+      <c r="B18" s="28">
+        <v>40831.694444444445</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>90</v>
@@ -3020,7 +3023,7 @@
       <c r="H18" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="21">
         <v>0.68055555555555602</v>
       </c>
       <c r="J18" s="8">
@@ -3028,20 +3031,20 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1">
-      <c r="A19" s="6">
-        <v>0.69444444444444497</v>
-      </c>
-      <c r="B19" s="7">
-        <v>0.73611111111111116</v>
-      </c>
-      <c r="C19" s="36" t="s">
+      <c r="A19" s="25">
+        <v>40831.694444444445</v>
+      </c>
+      <c r="B19" s="26">
+        <v>40831.736111111109</v>
+      </c>
+      <c r="C19" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
       <c r="I19" s="7">
         <v>0.69444444444444497</v>
       </c>
@@ -3050,11 +3053,11 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1">
-      <c r="A20" s="6">
-        <v>0.73611111111111205</v>
-      </c>
-      <c r="B20" s="7">
-        <v>0.77083333333333337</v>
+      <c r="A20" s="25">
+        <v>40831.736111111109</v>
+      </c>
+      <c r="B20" s="26">
+        <v>40831.770833333336</v>
       </c>
       <c r="C20" s="41" t="s">
         <v>0</v>
@@ -3072,21 +3075,21 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1">
-      <c r="A21" s="15">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="B21" s="16">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="C21" s="36" t="s">
+      <c r="A21" s="31">
+        <v>40831.770833333336</v>
+      </c>
+      <c r="B21" s="32">
+        <v>40831.791666666664</v>
+      </c>
+      <c r="C21" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="16">
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="15">
         <v>0.77083333333333337</v>
       </c>
       <c r="J21" s="6">
@@ -3094,553 +3097,552 @@
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="7"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18" t="s">
+      <c r="A22" s="33">
+        <v>40831.791666666664</v>
+      </c>
+      <c r="B22" s="33">
+        <v>40831.802083333336</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I22" s="22">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="J22" s="8">
+        <v>0.80208333333333337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="28">
+        <v>40831.802083333336</v>
+      </c>
+      <c r="B23" s="28">
+        <v>40831.8125</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="I23" s="21">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="J23" s="8">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="28">
+        <v>40831.8125</v>
+      </c>
+      <c r="B24" s="28">
+        <v>40831.822916666664</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="I24" s="21">
+        <v>0.8125</v>
+      </c>
+      <c r="J24" s="8">
+        <v>0.82291666666666696</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="28">
+        <v>40831.822916666664</v>
+      </c>
+      <c r="B25" s="28">
+        <v>40831.833333333336</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I25" s="21">
+        <v>0.82291666666666696</v>
+      </c>
+      <c r="J25" s="8">
+        <v>0.83333333333333404</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="28">
+        <v>40831.833333333336</v>
+      </c>
+      <c r="B26" s="28">
+        <v>40831.84375</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="21">
+        <v>0.83333333333333404</v>
+      </c>
+      <c r="J26" s="8">
+        <v>0.84375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="28">
+        <v>40831.84375</v>
+      </c>
+      <c r="B27" s="28">
+        <v>40831.854166666664</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I27" s="21">
+        <v>0.84375</v>
+      </c>
+      <c r="J27" s="8">
+        <v>0.85416666666666696</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="28">
+        <v>40831.854166666664</v>
+      </c>
+      <c r="B28" s="28">
+        <v>40831.864583333336</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I28" s="21">
+        <v>0.85416666666666696</v>
+      </c>
+      <c r="J28" s="8">
+        <v>0.86458333333333404</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="28">
+        <v>40831.864583333336</v>
+      </c>
+      <c r="B29" s="28">
+        <v>40831.875</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I29" s="21">
+        <v>0.86458333333333404</v>
+      </c>
+      <c r="J29" s="8">
+        <v>0.875000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="28">
+        <v>40831.875</v>
+      </c>
+      <c r="B30" s="28">
+        <v>40831.885416666664</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" s="21">
+        <v>0.875000000000001</v>
+      </c>
+      <c r="J30" s="8">
+        <v>0.88541666666666696</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="28">
+        <v>40831.885416666664</v>
+      </c>
+      <c r="B31" s="28">
+        <v>40831.895833333336</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="I31" s="21">
+        <v>0.88541666666666696</v>
+      </c>
+      <c r="J31" s="8">
+        <v>0.89583333333333404</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="28">
+        <v>40831.895833333336</v>
+      </c>
+      <c r="B32" s="28">
+        <v>40831.90625</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I32" s="21">
+        <v>0.89583333333333404</v>
+      </c>
+      <c r="J32" s="8">
+        <v>0.906250000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="28">
+        <v>40831.90625</v>
+      </c>
+      <c r="B33" s="25">
+        <v>40831.916666666664</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I33" s="21">
+        <v>0.906250000000001</v>
+      </c>
+      <c r="J33" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="25">
+        <v>40831.916666666664</v>
+      </c>
+      <c r="B34" s="26">
+        <v>40831</v>
+      </c>
+      <c r="C34" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="7">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="J34" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="25">
+        <v>40831</v>
+      </c>
+      <c r="B35" s="26">
+        <v>40831.333333333336</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="7">
+        <v>0</v>
+      </c>
+      <c r="J35" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.75">
+      <c r="A39" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="40"/>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="37"/>
+      <c r="C41" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D41" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E41" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="F41" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="5" t="s">
+      <c r="I41" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="20">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="B23" s="20">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="I23" s="26">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="J23" s="8">
-        <v>0.80208333333333337</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="8">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="B24" s="8">
-        <v>0.8125</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I24" s="25">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="J24" s="8">
-        <v>0.8125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="8">
-        <v>0.8125</v>
-      </c>
-      <c r="B25" s="8">
-        <v>0.82291666666666696</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="I25" s="25">
-        <v>0.8125</v>
-      </c>
-      <c r="J25" s="8">
-        <v>0.82291666666666696</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="8">
-        <v>0.82291666666666696</v>
-      </c>
-      <c r="B26" s="8">
-        <v>0.83333333333333404</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="I26" s="25">
-        <v>0.82291666666666696</v>
-      </c>
-      <c r="J26" s="8">
-        <v>0.83333333333333404</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="8">
-        <v>0.83333333333333404</v>
-      </c>
-      <c r="B27" s="8">
-        <v>0.84375</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I27" s="25">
-        <v>0.83333333333333404</v>
-      </c>
-      <c r="J27" s="8">
-        <v>0.84375</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="8">
-        <v>0.84375</v>
-      </c>
-      <c r="B28" s="8">
-        <v>0.85416666666666696</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="I28" s="25">
-        <v>0.84375</v>
-      </c>
-      <c r="J28" s="8">
-        <v>0.85416666666666696</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="8">
-        <v>0.85416666666666696</v>
-      </c>
-      <c r="B29" s="8">
-        <v>0.86458333333333404</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H29" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="I29" s="25">
-        <v>0.85416666666666696</v>
-      </c>
-      <c r="J29" s="8">
-        <v>0.86458333333333404</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="8">
-        <v>0.86458333333333404</v>
-      </c>
-      <c r="B30" s="8">
-        <v>0.875000000000001</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="I30" s="25">
-        <v>0.86458333333333404</v>
-      </c>
-      <c r="J30" s="8">
-        <v>0.875000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="8">
-        <v>0.875000000000001</v>
-      </c>
-      <c r="B31" s="8">
-        <v>0.88541666666666696</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="I31" s="25">
-        <v>0.875000000000001</v>
-      </c>
-      <c r="J31" s="8">
-        <v>0.88541666666666696</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="8">
-        <v>0.88541666666666696</v>
-      </c>
-      <c r="B32" s="8">
-        <v>0.89583333333333404</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="I32" s="25">
-        <v>0.88541666666666696</v>
-      </c>
-      <c r="J32" s="8">
-        <v>0.89583333333333404</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" s="8">
-        <v>0.89583333333333404</v>
-      </c>
-      <c r="B33" s="8">
-        <v>0.906250000000001</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="H33" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="I33" s="25">
-        <v>0.89583333333333404</v>
-      </c>
-      <c r="J33" s="8">
-        <v>0.906250000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="8">
-        <v>0.906250000000001</v>
-      </c>
-      <c r="B34" s="6">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="I34" s="25">
-        <v>0.906250000000001</v>
-      </c>
-      <c r="J34" s="6">
-        <v>0.91666666666666663</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="6">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="B35" s="7">
-        <v>0</v>
-      </c>
-      <c r="C35" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="7">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="J35" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="6">
-        <v>0</v>
-      </c>
-      <c r="B36" s="7">
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="28">
+        <v>40832.333333333336</v>
+      </c>
+      <c r="B42" s="28">
+        <v>40832.361111111109</v>
+      </c>
+      <c r="C42" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C36" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="7">
-        <v>0</v>
-      </c>
-      <c r="J36" s="6">
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="21"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="21"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-    </row>
-    <row r="40" spans="1:11" ht="15.75">
-      <c r="A40" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="37"/>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="38"/>
-      <c r="C42" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I42" s="23" t="s">
-        <v>14</v>
+      <c r="K42" s="8">
+        <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="8">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="B43" s="8">
-        <v>0.3611111111111111</v>
+      <c r="A43" s="28">
+        <v>40832.361111111109</v>
+      </c>
+      <c r="B43" s="28">
+        <v>40832.388888888891</v>
       </c>
       <c r="C43" s="44" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="D43" s="45"/>
       <c r="E43" s="45"/>
@@ -3649,649 +3651,623 @@
       <c r="H43" s="45"/>
       <c r="I43" s="46"/>
       <c r="J43" s="8">
-        <v>0.33333333333333331</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="K43" s="8">
-        <v>0.3611111111111111</v>
+        <v>0.3888888888888889</v>
       </c>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="8">
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="B44" s="8">
+      <c r="A44" s="28">
+        <v>40832.388888888891</v>
+      </c>
+      <c r="B44" s="28">
+        <v>40832.402777777781</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J44" s="8">
         <v>0.3888888888888889</v>
       </c>
-      <c r="C44" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="8">
-        <v>0.3611111111111111</v>
-      </c>
       <c r="K44" s="8">
-        <v>0.3888888888888889</v>
+        <v>0.40277777777777773</v>
       </c>
     </row>
     <row r="45" spans="1:11">
-      <c r="A45" s="8">
-        <v>0.3888888888888889</v>
-      </c>
-      <c r="B45" s="8">
-        <v>0.40277777777777773</v>
-      </c>
-      <c r="C45" s="24" t="s">
+      <c r="A45" s="28">
+        <v>40832.402777777781</v>
+      </c>
+      <c r="B45" s="28">
+        <v>40832.416666666664</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="24" t="s">
+      <c r="E45" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="I45" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J45" s="8">
+        <v>0.40277777777777801</v>
+      </c>
+      <c r="K45" s="8">
+        <v>0.41666666666666702</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="28">
+        <v>40832.416666666664</v>
+      </c>
+      <c r="B46" s="28">
+        <v>40832.430555555555</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="I46" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="J46" s="8">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="K46" s="8">
+        <v>0.43055555555555602</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="28">
+        <v>40832.430555555555</v>
+      </c>
+      <c r="B47" s="28">
+        <v>40832.444444444445</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E47" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="F47" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" s="8">
+        <v>0.43055555555555602</v>
+      </c>
+      <c r="K47" s="8">
+        <v>0.44444444444444497</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="28">
+        <v>40832.444444444445</v>
+      </c>
+      <c r="B48" s="28">
+        <v>40832.458333333336</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="G48" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J48" s="8">
+        <v>0.44444444444444497</v>
+      </c>
+      <c r="K48" s="8">
+        <v>0.45833333333333298</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="28">
+        <v>40832.458333333336</v>
+      </c>
+      <c r="B49" s="28">
+        <v>40832.472222222219</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I49" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="J49" s="8">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="K49" s="8">
+        <v>0.47222222222222199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="28">
+        <v>40832.472222222219</v>
+      </c>
+      <c r="B50" s="28">
+        <v>40832.486111111109</v>
+      </c>
+      <c r="C50" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="D50" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E50" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H45" s="10" t="s">
+      <c r="F50" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="J50" s="8">
+        <v>0.47222222222222199</v>
+      </c>
+      <c r="K50" s="8">
+        <v>0.48611111111111099</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="28">
+        <v>40832.486111111109</v>
+      </c>
+      <c r="B51" s="28">
+        <v>40832.5</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I51" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J51" s="8">
+        <v>0.48611111111111099</v>
+      </c>
+      <c r="K51" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="28">
+        <v>40832.5</v>
+      </c>
+      <c r="B52" s="28">
+        <v>40832.527777777781</v>
+      </c>
+      <c r="C52" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="42"/>
+      <c r="G52" s="42"/>
+      <c r="H52" s="42"/>
+      <c r="I52" s="43"/>
+      <c r="J52" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="K52" s="8">
+        <v>0.52777777777777779</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="28">
+        <v>40832.527777777781</v>
+      </c>
+      <c r="B53" s="28">
+        <v>40832.541666666664</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G53" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="I45" s="10" t="s">
+      <c r="H53" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J53" s="8">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="K53" s="8">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="28">
+        <v>40832.541666666664</v>
+      </c>
+      <c r="B54" s="28">
+        <v>40832.555555555555</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="J45" s="8">
-        <v>0.3888888888888889</v>
-      </c>
-      <c r="K45" s="8">
-        <v>0.40277777777777773</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="8">
-        <v>0.40277777777777801</v>
-      </c>
-      <c r="B46" s="8">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="C46" s="24" t="s">
+      <c r="E54" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H54" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I54" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D46" s="24" t="s">
+      <c r="J54" s="8">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="K54" s="8">
+        <v>0.55555555555555602</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="28">
+        <v>40832.555555555555</v>
+      </c>
+      <c r="B55" s="28">
+        <v>40832.569444444445</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H55" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I55" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="J55" s="8">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="K55" s="8">
+        <v>0.56944444444444398</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="28">
+        <v>40832.569444444445</v>
+      </c>
+      <c r="B56" s="28">
+        <v>40832.583333333336</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J56" s="8">
+        <v>0.56944444444444398</v>
+      </c>
+      <c r="K56" s="8">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="28">
+        <v>40832.583333333336</v>
+      </c>
+      <c r="B57" s="28">
+        <v>40832.597222222219</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H57" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="I57" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="J57" s="8">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="K57" s="8">
+        <v>0.59722222222222199</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="28">
+        <v>40832.597222222219</v>
+      </c>
+      <c r="B58" s="28">
+        <v>40832.611111111109</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H58" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="J58" s="8">
+        <v>0.59722222222222199</v>
+      </c>
+      <c r="K58" s="8">
+        <v>0.61111111111111105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="28">
+        <v>40832.611111111109</v>
+      </c>
+      <c r="B59" s="28">
+        <v>40832.625</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="J59" s="8">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="K59" s="8">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="28">
+        <v>40832.625</v>
+      </c>
+      <c r="B60" s="28">
+        <v>40832.638888888891</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H60" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="I60" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G46" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="H46" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="I46" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="J46" s="8">
-        <v>0.40277777777777801</v>
-      </c>
-      <c r="K46" s="8">
-        <v>0.41666666666666702</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="8">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="B47" s="8">
-        <v>0.43055555555555602</v>
-      </c>
-      <c r="C47" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="D47" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="H47" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="I47" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="J47" s="8">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="K47" s="8">
-        <v>0.43055555555555602</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="8">
-        <v>0.43055555555555602</v>
-      </c>
-      <c r="B48" s="8">
-        <v>0.44444444444444497</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D48" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I48" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J48" s="8">
-        <v>0.43055555555555602</v>
-      </c>
-      <c r="K48" s="8">
-        <v>0.44444444444444497</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="8">
-        <v>0.44444444444444497</v>
-      </c>
-      <c r="B49" s="8">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="C49" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="D49" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="H49" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="I49" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="J49" s="8">
-        <v>0.44444444444444497</v>
-      </c>
-      <c r="K49" s="8">
-        <v>0.45833333333333298</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="8">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="B50" s="8">
-        <v>0.47222222222222199</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D50" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="H50" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="I50" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="J50" s="8">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="K50" s="8">
-        <v>0.47222222222222199</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="8">
-        <v>0.47222222222222199</v>
-      </c>
-      <c r="B51" s="8">
-        <v>0.48611111111111099</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="D51" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G51" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="H51" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="I51" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="J51" s="8">
-        <v>0.47222222222222199</v>
-      </c>
-      <c r="K51" s="8">
-        <v>0.48611111111111099</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="8">
-        <v>0.48611111111111099</v>
-      </c>
-      <c r="B52" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="D52" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I52" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="J52" s="8">
-        <v>0.48611111111111099</v>
-      </c>
-      <c r="K52" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="B53" s="8">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="C53" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="43"/>
-      <c r="J53" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="K53" s="8">
-        <v>0.52777777777777779</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="A54" s="8">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="B54" s="8">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D54" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="H54" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I54" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="J54" s="8">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="K54" s="8">
-        <v>0.54166666666666663</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="8">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="B55" s="8">
-        <v>0.55555555555555602</v>
-      </c>
-      <c r="C55" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="D55" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F55" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G55" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="H55" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="I55" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="J55" s="8">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="K55" s="8">
-        <v>0.55555555555555602</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="8">
-        <v>0.55555555555555602</v>
-      </c>
-      <c r="B56" s="8">
-        <v>0.56944444444444398</v>
-      </c>
-      <c r="C56" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="D56" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F56" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="G56" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="H56" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="I56" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="J56" s="8">
-        <v>0.55555555555555602</v>
-      </c>
-      <c r="K56" s="8">
-        <v>0.56944444444444398</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11">
-      <c r="A57" s="8">
-        <v>0.56944444444444398</v>
-      </c>
-      <c r="B57" s="8">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D57" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F57" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="G57" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H57" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="I57" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="J57" s="8">
-        <v>0.56944444444444398</v>
-      </c>
-      <c r="K57" s="8">
-        <v>0.58333333333333304</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11">
-      <c r="A58" s="8">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="B58" s="8">
-        <v>0.59722222222222199</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D58" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="I58" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="J58" s="8">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="K58" s="8">
-        <v>0.59722222222222199</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="A59" s="8">
-        <v>0.59722222222222199</v>
-      </c>
-      <c r="B59" s="8">
-        <v>0.61111111111111105</v>
-      </c>
-      <c r="C59" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D59" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F59" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="H59" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="I59" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="J59" s="8">
-        <v>0.59722222222222199</v>
-      </c>
-      <c r="K59" s="8">
-        <v>0.61111111111111105</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11">
-      <c r="A60" s="8">
-        <v>0.61111111111111105</v>
-      </c>
-      <c r="B60" s="8">
+      <c r="J60" s="8">
         <v>0.625</v>
       </c>
-      <c r="C60" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="D60" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="G60" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="H60" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="I60" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="J60" s="8">
-        <v>0.61111111111111105</v>
-      </c>
       <c r="K60" s="8">
-        <v>0.625</v>
+        <v>0.63888888888888895</v>
       </c>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="8">
-        <v>0.625</v>
-      </c>
-      <c r="B61" s="8">
+      <c r="A61" s="28">
+        <v>40832.638888888891</v>
+      </c>
+      <c r="B61" s="28">
+        <v>40832.645833333336</v>
+      </c>
+      <c r="C61" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D61" s="45"/>
+      <c r="E61" s="45"/>
+      <c r="F61" s="45"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="45"/>
+      <c r="I61" s="46"/>
+      <c r="J61" s="8">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C61" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D61" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F61" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="G61" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="I61" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="J61" s="8">
-        <v>0.625</v>
-      </c>
       <c r="K61" s="8">
-        <v>0.63888888888888895</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="8">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="B62" s="8">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C62" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="D62" s="45"/>
-      <c r="E62" s="45"/>
-      <c r="F62" s="45"/>
-      <c r="G62" s="45"/>
-      <c r="H62" s="45"/>
-      <c r="I62" s="46"/>
-      <c r="J62" s="8">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="K62" s="8">
-        <v>0.64583333333333337</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C43:I43"/>
-    <mergeCell ref="A2:B2"/>
+  <mergeCells count="15">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A40:K40"/>
-    <mergeCell ref="C62:I62"/>
+    <mergeCell ref="A39:K39"/>
+    <mergeCell ref="C61:I61"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C5:H5"/>
@@ -4299,10 +4275,11 @@
     <mergeCell ref="C21:H21"/>
     <mergeCell ref="C20:H20"/>
     <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C34:H34"/>
     <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C36:H36"/>
-    <mergeCell ref="C44:I44"/>
-    <mergeCell ref="C53:I53"/>
+    <mergeCell ref="C43:I43"/>
+    <mergeCell ref="C52:I52"/>
+    <mergeCell ref="C42:I42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4406,7 +4383,7 @@
       <c r="U2" s="1">
         <v>0.65277777777777779</v>
       </c>
-      <c r="V2" s="28">
+      <c r="V2" s="24">
         <v>0.66666666666666663</v>
       </c>
       <c r="W2" s="1">
@@ -4493,7 +4470,7 @@
       <c r="T3" s="1">
         <v>0.65277777777777779</v>
       </c>
-      <c r="U3" s="28">
+      <c r="U3" s="24">
         <v>0.66666666666666663</v>
       </c>
       <c r="V3" s="1">

</xml_diff>

<commit_message>
- Activities spanning multiple row now get merged into 1 big activity. - Added a border around the current activity
</commit_message>
<xml_diff>
--- a/BarcodeScanner/planning kinderen en leiding.xlsx
+++ b/BarcodeScanner/planning kinderen en leiding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="9480" windowHeight="7920" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="9480" windowHeight="7920"/>
   </bookViews>
   <sheets>
     <sheet name="Kleine speltakken" sheetId="1" r:id="rId1"/>
@@ -1009,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2502,8 +2502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Allerlaatste versie voor dit jaar. Dayselector ingesteld op Auto, dagindeling aangepast
</commit_message>
<xml_diff>
--- a/BarcodeScanner/planning kinderen en leiding.xlsx
+++ b/BarcodeScanner/planning kinderen en leiding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="9480" windowHeight="7920" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19245" windowHeight="4380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kleine speltakken" sheetId="1" r:id="rId1"/>
@@ -1583,7 +1583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2026,13 +2026,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2045,6 +2039,12 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2073,6 +2073,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3866,8 +3872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="B51" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3997,19 +4003,19 @@
       <c r="C6" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="204" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="94" t="s">
         <v>88</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="94" t="s">
         <v>86</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="94" t="s">
         <v>220</v>
       </c>
       <c r="I6" s="18">
@@ -4026,22 +4032,22 @@
       <c r="B7" s="89">
         <v>40831.527777777781</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="204" t="s">
         <v>83</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="94" t="s">
         <v>88</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="96" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="94" t="s">
         <v>220</v>
       </c>
       <c r="I7" s="18">
@@ -4061,19 +4067,19 @@
       <c r="C8" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="204" t="s">
         <v>85</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="94" t="s">
         <v>219</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="94" t="s">
         <v>220</v>
       </c>
       <c r="I8" s="18">
@@ -4090,7 +4096,7 @@
       <c r="B9" s="89">
         <v>40831.555555555555</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="204" t="s">
         <v>85</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -4099,13 +4105,13 @@
       <c r="E9" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="94" t="s">
         <v>219</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="94" t="s">
         <v>220</v>
       </c>
       <c r="I9" s="18">
@@ -4144,19 +4150,19 @@
       <c r="B11" s="89">
         <v>40831.597222222219</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="94" t="s">
         <v>231</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="205" t="s">
         <v>226</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="94" t="s">
         <v>75</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -4176,19 +4182,19 @@
       <c r="B12" s="89">
         <v>40831.611111111109</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="94" t="s">
         <v>231</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="205" t="s">
         <v>226</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="94" t="s">
         <v>75</v>
       </c>
       <c r="H12" s="9" t="s">
@@ -4208,19 +4214,19 @@
       <c r="B13" s="89">
         <v>40831.625</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="205" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="205" t="s">
         <v>231</v>
       </c>
       <c r="H13" s="9" t="s">
@@ -4240,19 +4246,19 @@
       <c r="B14" s="89">
         <v>40831.638888888891</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="205" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="205" t="s">
         <v>231</v>
       </c>
       <c r="H14" s="9" t="s">
@@ -4272,22 +4278,22 @@
       <c r="B15" s="89">
         <v>40831.652777777781</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="94" t="s">
         <v>230</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="205" t="s">
         <v>228</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="94" t="s">
         <v>229</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="94" t="s">
         <v>222</v>
       </c>
       <c r="I15" s="18">
@@ -4304,22 +4310,22 @@
       <c r="B16" s="89">
         <v>40831.666666666664</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="94" t="s">
         <v>230</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="205" t="s">
         <v>228</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="94" t="s">
         <v>229</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="95" t="s">
         <v>222</v>
       </c>
       <c r="I16" s="18">
@@ -4336,22 +4342,22 @@
       <c r="B17" s="89">
         <v>40831.680555555555</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="205" t="s">
         <v>229</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="94" t="s">
         <v>232</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="95" t="s">
         <v>222</v>
       </c>
       <c r="I17" s="18">
@@ -4368,22 +4374,22 @@
       <c r="B18" s="89">
         <v>40831.694444444445</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="205" t="s">
         <v>229</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="94" t="s">
         <v>232</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="96" t="s">
         <v>222</v>
       </c>
       <c r="I18" s="18">
@@ -4469,16 +4475,16 @@
       <c r="C22" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="204" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="94" t="s">
         <v>223</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="94" t="s">
         <v>225</v>
       </c>
       <c r="H22" s="94" t="s">
@@ -4498,19 +4504,19 @@
       <c r="B23" s="89">
         <v>40831.8125</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="204" t="s">
         <v>79</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="94" t="s">
         <v>223</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="94" t="s">
         <v>225</v>
       </c>
       <c r="H23" s="94" t="s">
@@ -4533,13 +4539,13 @@
       <c r="C24" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="204" t="s">
         <v>81</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="94" t="s">
         <v>223</v>
       </c>
       <c r="G24" s="9" t="s">
@@ -4562,7 +4568,7 @@
       <c r="B25" s="89">
         <v>40831.833333333336</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="204" t="s">
         <v>81</v>
       </c>
       <c r="D25" s="8" t="s">
@@ -4571,7 +4577,7 @@
       <c r="E25" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="94" t="s">
         <v>223</v>
       </c>
       <c r="G25" s="9" t="s">
@@ -4597,16 +4603,16 @@
       <c r="C26" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="204" t="s">
         <v>83</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="94" t="s">
         <v>75</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="94" t="s">
         <v>226</v>
       </c>
       <c r="H26" s="9" t="s">
@@ -4626,19 +4632,19 @@
       <c r="B27" s="89">
         <v>40831.854166666664</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="204" t="s">
         <v>83</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="94" t="s">
         <v>218</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="94" t="s">
         <v>226</v>
       </c>
       <c r="H27" s="11" t="s">
@@ -4661,13 +4667,13 @@
       <c r="C28" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="204" t="s">
         <v>85</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="94" t="s">
         <v>75</v>
       </c>
       <c r="G28" s="9" t="s">
@@ -4690,7 +4696,7 @@
       <c r="B29" s="89">
         <v>40831.875</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="204" t="s">
         <v>85</v>
       </c>
       <c r="D29" s="8" t="s">
@@ -4699,7 +4705,7 @@
       <c r="E29" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="94" t="s">
         <v>75</v>
       </c>
       <c r="G29" s="9" t="s">
@@ -4725,16 +4731,16 @@
       <c r="C30" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="204" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="94" t="s">
         <v>229</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G30" s="94" t="s">
         <v>228</v>
       </c>
       <c r="H30" s="94" t="s">
@@ -4754,19 +4760,19 @@
       <c r="B31" s="89">
         <v>40831.895833333336</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="204" t="s">
         <v>87</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="94" t="s">
         <v>229</v>
       </c>
       <c r="F31" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="94" t="s">
         <v>228</v>
       </c>
       <c r="H31" s="94" t="s">
@@ -4789,13 +4795,13 @@
       <c r="C32" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="204" t="s">
         <v>89</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F32" s="94" t="s">
         <v>229</v>
       </c>
       <c r="G32" s="9" t="s">
@@ -4818,7 +4824,7 @@
       <c r="B33" s="87">
         <v>40831.916666666664</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="204" t="s">
         <v>89</v>
       </c>
       <c r="D33" s="8" t="s">
@@ -4827,7 +4833,7 @@
       <c r="E33" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F33" s="94" t="s">
         <v>229</v>
       </c>
       <c r="G33" s="9" t="s">
@@ -5033,7 +5039,7 @@
       <c r="D44" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="94" t="s">
         <v>233</v>
       </c>
       <c r="F44" s="94" t="s">
@@ -5068,7 +5074,7 @@
       <c r="D45" s="97" t="s">
         <v>91</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="94" t="s">
         <v>233</v>
       </c>
       <c r="F45" s="94" t="s">
@@ -5106,10 +5112,10 @@
       <c r="E46" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="F46" s="94" t="s">
+      <c r="F46" s="205" t="s">
         <v>232</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="G46" s="94" t="s">
         <v>228</v>
       </c>
       <c r="H46" s="94" t="s">
@@ -5141,10 +5147,10 @@
       <c r="E47" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="F47" s="94" t="s">
+      <c r="F47" s="205" t="s">
         <v>232</v>
       </c>
-      <c r="G47" s="9" t="s">
+      <c r="G47" s="94" t="s">
         <v>228</v>
       </c>
       <c r="H47" s="94" t="s">
@@ -5176,10 +5182,10 @@
       <c r="E48" s="94" t="s">
         <v>228</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="F48" s="94" t="s">
         <v>233</v>
       </c>
-      <c r="G48" s="94" t="s">
+      <c r="G48" s="205" t="s">
         <v>234</v>
       </c>
       <c r="H48" s="9" t="s">
@@ -5211,10 +5217,10 @@
       <c r="E49" s="94" t="s">
         <v>228</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="94" t="s">
         <v>233</v>
       </c>
-      <c r="G49" s="94" t="s">
+      <c r="G49" s="205" t="s">
         <v>234</v>
       </c>
       <c r="H49" s="9" t="s">
@@ -5243,7 +5249,7 @@
       <c r="D50" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E50" s="94" t="s">
+      <c r="E50" s="205" t="s">
         <v>232</v>
       </c>
       <c r="F50" s="9" t="s">
@@ -5278,7 +5284,7 @@
       <c r="D51" s="97" t="s">
         <v>88</v>
       </c>
-      <c r="E51" s="94" t="s">
+      <c r="E51" s="205" t="s">
         <v>232</v>
       </c>
       <c r="F51" s="9" t="s">
@@ -9627,11 +9633,11 @@
       <c r="BB21" s="111"/>
       <c r="BC21" s="111"/>
       <c r="BD21" s="112"/>
-      <c r="BE21" s="191" t="s">
+      <c r="BE21" s="189" t="s">
         <v>165</v>
       </c>
-      <c r="BF21" s="192"/>
-      <c r="BG21" s="193"/>
+      <c r="BF21" s="190"/>
+      <c r="BG21" s="191"/>
       <c r="BH21" s="110" t="s">
         <v>168</v>
       </c>
@@ -9965,7 +9971,7 @@
       <c r="N23" s="157"/>
       <c r="O23" s="157"/>
       <c r="P23" s="157"/>
-      <c r="Q23" s="188"/>
+      <c r="Q23" s="193"/>
       <c r="R23" s="156" t="s">
         <v>7</v>
       </c>
@@ -10038,22 +10044,22 @@
       <c r="BW23" s="129"/>
       <c r="BX23" s="129"/>
       <c r="BY23" s="129"/>
-      <c r="BZ23" s="194" t="s">
+      <c r="BZ23" s="192" t="s">
         <v>175</v>
       </c>
-      <c r="CA23" s="194"/>
-      <c r="CB23" s="194"/>
-      <c r="CC23" s="194"/>
-      <c r="CD23" s="194"/>
-      <c r="CE23" s="194"/>
-      <c r="CF23" s="194" t="s">
+      <c r="CA23" s="192"/>
+      <c r="CB23" s="192"/>
+      <c r="CC23" s="192"/>
+      <c r="CD23" s="192"/>
+      <c r="CE23" s="192"/>
+      <c r="CF23" s="192" t="s">
         <v>77</v>
       </c>
-      <c r="CG23" s="194"/>
-      <c r="CH23" s="194"/>
-      <c r="CI23" s="194"/>
-      <c r="CJ23" s="194"/>
-      <c r="CK23" s="194"/>
+      <c r="CG23" s="192"/>
+      <c r="CH23" s="192"/>
+      <c r="CI23" s="192"/>
+      <c r="CJ23" s="192"/>
+      <c r="CK23" s="192"/>
       <c r="CL23" s="78"/>
       <c r="CM23" s="78"/>
       <c r="CN23" s="78"/>
@@ -10068,7 +10074,7 @@
       <c r="CS23" s="157"/>
       <c r="CT23" s="157"/>
       <c r="CU23" s="157"/>
-      <c r="CV23" s="188"/>
+      <c r="CV23" s="193"/>
       <c r="CW23" s="156" t="s">
         <v>51</v>
       </c>
@@ -10092,7 +10098,7 @@
       <c r="DK23" s="157"/>
       <c r="DL23" s="157"/>
       <c r="DM23" s="157"/>
-      <c r="DN23" s="188"/>
+      <c r="DN23" s="193"/>
       <c r="DO23" s="156" t="s">
         <v>195</v>
       </c>
@@ -10108,7 +10114,7 @@
       </c>
       <c r="DX23" s="157"/>
       <c r="DY23" s="157"/>
-      <c r="DZ23" s="188"/>
+      <c r="DZ23" s="193"/>
       <c r="EA23" s="156" t="s">
         <v>9</v>
       </c>
@@ -10168,7 +10174,7 @@
       <c r="AA24" s="66"/>
       <c r="AB24" s="66"/>
       <c r="AC24" s="67"/>
-      <c r="AD24" s="189" t="s">
+      <c r="AD24" s="188" t="s">
         <v>192</v>
       </c>
       <c r="AE24" s="184"/>
@@ -10226,20 +10232,20 @@
       <c r="BW24" s="114"/>
       <c r="BX24" s="114"/>
       <c r="BY24" s="114"/>
-      <c r="BZ24" s="194" t="s">
+      <c r="BZ24" s="192" t="s">
         <v>174</v>
       </c>
-      <c r="CA24" s="194"/>
-      <c r="CB24" s="194"/>
-      <c r="CC24" s="194"/>
-      <c r="CD24" s="194"/>
-      <c r="CE24" s="194"/>
-      <c r="CF24" s="194"/>
-      <c r="CG24" s="194"/>
-      <c r="CH24" s="194"/>
-      <c r="CI24" s="194"/>
-      <c r="CJ24" s="194"/>
-      <c r="CK24" s="194"/>
+      <c r="CA24" s="192"/>
+      <c r="CB24" s="192"/>
+      <c r="CC24" s="192"/>
+      <c r="CD24" s="192"/>
+      <c r="CE24" s="192"/>
+      <c r="CF24" s="192"/>
+      <c r="CG24" s="192"/>
+      <c r="CH24" s="192"/>
+      <c r="CI24" s="192"/>
+      <c r="CJ24" s="192"/>
+      <c r="CK24" s="192"/>
       <c r="CL24" s="78"/>
       <c r="CM24" s="78"/>
       <c r="CN24" s="78"/>
@@ -10247,15 +10253,15 @@
       <c r="CP24" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="CQ24" s="189" t="s">
+      <c r="CQ24" s="188" t="s">
         <v>176</v>
       </c>
       <c r="CR24" s="184"/>
       <c r="CS24" s="184"/>
       <c r="CT24" s="184"/>
       <c r="CU24" s="184"/>
-      <c r="CV24" s="190"/>
-      <c r="CW24" s="189" t="s">
+      <c r="CV24" s="194"/>
+      <c r="CW24" s="188" t="s">
         <v>51</v>
       </c>
       <c r="CX24" s="184"/>
@@ -10278,8 +10284,8 @@
       <c r="DK24" s="184"/>
       <c r="DL24" s="184"/>
       <c r="DM24" s="184"/>
-      <c r="DN24" s="190"/>
-      <c r="DO24" s="189" t="s">
+      <c r="DN24" s="194"/>
+      <c r="DO24" s="188" t="s">
         <v>8</v>
       </c>
       <c r="DP24" s="184"/>
@@ -10294,8 +10300,8 @@
       </c>
       <c r="DX24" s="184"/>
       <c r="DY24" s="184"/>
-      <c r="DZ24" s="190"/>
-      <c r="EA24" s="189" t="s">
+      <c r="DZ24" s="194"/>
+      <c r="EA24" s="188" t="s">
         <v>195</v>
       </c>
       <c r="EB24" s="184"/>
@@ -12133,11 +12139,11 @@
       <c r="BB34" s="25"/>
       <c r="BC34" s="1"/>
       <c r="BD34" s="1"/>
-      <c r="BE34" s="191" t="s">
+      <c r="BE34" s="189" t="s">
         <v>164</v>
       </c>
-      <c r="BF34" s="192"/>
-      <c r="BG34" s="193"/>
+      <c r="BF34" s="190"/>
+      <c r="BG34" s="191"/>
       <c r="BH34" s="110" t="s">
         <v>10</v>
       </c>
@@ -15447,6 +15453,7 @@
     <mergeCell ref="AZ38:BD38"/>
     <mergeCell ref="AZ39:BD39"/>
     <mergeCell ref="AZ40:BD40"/>
+    <mergeCell ref="AT34:AY34"/>
     <mergeCell ref="AD46:AK46"/>
     <mergeCell ref="AP46:AS46"/>
     <mergeCell ref="AD42:AK42"/>
@@ -15493,7 +15500,6 @@
     <mergeCell ref="R33:U33"/>
     <mergeCell ref="V33:Y33"/>
     <mergeCell ref="L46:Q46"/>
-    <mergeCell ref="DG27:DN27"/>
     <mergeCell ref="DG29:DN29"/>
     <mergeCell ref="DO26:DV26"/>
     <mergeCell ref="DO27:DV27"/>
@@ -15507,6 +15513,15 @@
     <mergeCell ref="EA23:EH23"/>
     <mergeCell ref="EA24:EH24"/>
     <mergeCell ref="EA25:EH25"/>
+    <mergeCell ref="DW24:DZ24"/>
+    <mergeCell ref="DW25:DZ25"/>
+    <mergeCell ref="DW26:DZ26"/>
+    <mergeCell ref="DW27:DZ27"/>
+    <mergeCell ref="DW28:DZ28"/>
+    <mergeCell ref="DW20:DZ20"/>
+    <mergeCell ref="DW21:DZ21"/>
+    <mergeCell ref="DW22:DZ22"/>
+    <mergeCell ref="DW23:DZ23"/>
     <mergeCell ref="EA14:EH14"/>
     <mergeCell ref="EA17:EH17"/>
     <mergeCell ref="EA18:EH18"/>
@@ -15705,21 +15720,6 @@
     <mergeCell ref="CW31:CZ31"/>
     <mergeCell ref="CQ25:CV25"/>
     <mergeCell ref="CQ26:CV26"/>
-    <mergeCell ref="CW45:CZ45"/>
-    <mergeCell ref="CW44:CZ44"/>
-    <mergeCell ref="CW42:CZ42"/>
-    <mergeCell ref="CW41:CZ41"/>
-    <mergeCell ref="CW38:CZ38"/>
-    <mergeCell ref="CW40:CZ40"/>
-    <mergeCell ref="CW39:CZ39"/>
-    <mergeCell ref="DA46:DD46"/>
-    <mergeCell ref="DA45:DD45"/>
-    <mergeCell ref="DA44:DD44"/>
-    <mergeCell ref="DA38:DD38"/>
-    <mergeCell ref="DA39:DD39"/>
-    <mergeCell ref="DA40:DD40"/>
-    <mergeCell ref="DA41:DD41"/>
-    <mergeCell ref="DA42:DD42"/>
     <mergeCell ref="CQ10:CV10"/>
     <mergeCell ref="CQ12:CV12"/>
     <mergeCell ref="CQ15:CV15"/>
@@ -15747,6 +15747,8 @@
     <mergeCell ref="AD32:AK32"/>
     <mergeCell ref="AD33:AK33"/>
     <mergeCell ref="R35:U35"/>
+    <mergeCell ref="Z41:AC41"/>
+    <mergeCell ref="Z42:AC42"/>
     <mergeCell ref="CF10:CK10"/>
     <mergeCell ref="BZ12:CK12"/>
     <mergeCell ref="BZ13:CK13"/>
@@ -15777,8 +15779,6 @@
     <mergeCell ref="L42:Q42"/>
     <mergeCell ref="L41:Q41"/>
     <mergeCell ref="L40:Q40"/>
-    <mergeCell ref="Z41:AC41"/>
-    <mergeCell ref="Z42:AC42"/>
     <mergeCell ref="Z46:AC46"/>
     <mergeCell ref="Z31:AC31"/>
     <mergeCell ref="Z32:AC32"/>
@@ -15788,12 +15788,6 @@
     <mergeCell ref="Z36:AC36"/>
     <mergeCell ref="Z44:AC44"/>
     <mergeCell ref="Z45:AC45"/>
-    <mergeCell ref="AT34:AY34"/>
-    <mergeCell ref="DW24:DZ24"/>
-    <mergeCell ref="DW25:DZ25"/>
-    <mergeCell ref="DW26:DZ26"/>
-    <mergeCell ref="DW27:DZ27"/>
-    <mergeCell ref="DW28:DZ28"/>
     <mergeCell ref="AZ24:BD24"/>
     <mergeCell ref="BE34:BG46"/>
     <mergeCell ref="BE21:BG32"/>
@@ -15803,19 +15797,6 @@
     <mergeCell ref="DA33:DD33"/>
     <mergeCell ref="DA34:DD34"/>
     <mergeCell ref="DA35:DD35"/>
-    <mergeCell ref="DU46:DX46"/>
-    <mergeCell ref="DU45:DX45"/>
-    <mergeCell ref="DU44:DX44"/>
-    <mergeCell ref="DU41:DX41"/>
-    <mergeCell ref="DU40:DX40"/>
-    <mergeCell ref="DU39:DX39"/>
-    <mergeCell ref="DU38:DX38"/>
-    <mergeCell ref="CW43:CZ43"/>
-    <mergeCell ref="CW46:CZ46"/>
-    <mergeCell ref="DW20:DZ20"/>
-    <mergeCell ref="DW21:DZ21"/>
-    <mergeCell ref="DW22:DZ22"/>
-    <mergeCell ref="DW23:DZ23"/>
     <mergeCell ref="DA28:DF28"/>
     <mergeCell ref="DA29:DF29"/>
     <mergeCell ref="CW22:CZ22"/>
@@ -15826,6 +15807,30 @@
     <mergeCell ref="CW28:CZ28"/>
     <mergeCell ref="CW27:CZ27"/>
     <mergeCell ref="CW26:CZ26"/>
+    <mergeCell ref="CW45:CZ45"/>
+    <mergeCell ref="CW44:CZ44"/>
+    <mergeCell ref="CW42:CZ42"/>
+    <mergeCell ref="CW41:CZ41"/>
+    <mergeCell ref="CW38:CZ38"/>
+    <mergeCell ref="DU46:DX46"/>
+    <mergeCell ref="DU45:DX45"/>
+    <mergeCell ref="DU44:DX44"/>
+    <mergeCell ref="DU41:DX41"/>
+    <mergeCell ref="DU40:DX40"/>
+    <mergeCell ref="DU39:DX39"/>
+    <mergeCell ref="DU38:DX38"/>
+    <mergeCell ref="CW43:CZ43"/>
+    <mergeCell ref="CW46:CZ46"/>
+    <mergeCell ref="CW40:CZ40"/>
+    <mergeCell ref="CW39:CZ39"/>
+    <mergeCell ref="DA46:DD46"/>
+    <mergeCell ref="DA45:DD45"/>
+    <mergeCell ref="DA44:DD44"/>
+    <mergeCell ref="DA38:DD38"/>
+    <mergeCell ref="DA39:DD39"/>
+    <mergeCell ref="DA40:DD40"/>
+    <mergeCell ref="DA41:DD41"/>
+    <mergeCell ref="DA42:DD42"/>
     <mergeCell ref="DA20:DF20"/>
     <mergeCell ref="DA21:DF21"/>
     <mergeCell ref="DA22:DF22"/>
@@ -15836,6 +15841,7 @@
     <mergeCell ref="DO25:DV25"/>
     <mergeCell ref="DO20:DV20"/>
     <mergeCell ref="DG26:DN26"/>
+    <mergeCell ref="DG27:DN27"/>
     <mergeCell ref="EI29:EN29"/>
     <mergeCell ref="DW10:DZ10"/>
     <mergeCell ref="DW11:DZ11"/>

</xml_diff>